<commit_message>
updated code for example datasets
</commit_message>
<xml_diff>
--- a/datasets/lab_detail.xlsx
+++ b/datasets/lab_detail.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="269">
   <si>
     <t>sampleid</t>
   </si>
@@ -81,342 +81,345 @@
     <t>substance</t>
   </si>
   <si>
+    <t>p-fluorofentanyl</t>
+  </si>
+  <si>
+    <t>xylazine</t>
+  </si>
+  <si>
+    <t>fentanyl</t>
+  </si>
+  <si>
+    <t>phenethyl 4-ANPP</t>
+  </si>
+  <si>
+    <t>4-ANPP</t>
+  </si>
+  <si>
+    <t>despropionyl p-fluorofentanyl</t>
+  </si>
+  <si>
     <t>dimethyl sulfone (methylsulfonylmethane MSM)</t>
   </si>
   <si>
+    <t>3,4-MDMA</t>
+  </si>
+  <si>
+    <t>3,4-methylenedioxy-N-benzylcathinone (BMDP)</t>
+  </si>
+  <si>
+    <t>3,4-MDMA</t>
+  </si>
+  <si>
+    <t>tropacocaine</t>
+  </si>
+  <si>
+    <t>levamisole</t>
+  </si>
+  <si>
+    <t>cocaine</t>
+  </si>
+  <si>
+    <t>methyl ecgonidine (MED)</t>
+  </si>
+  <si>
+    <t>norcocaine</t>
+  </si>
+  <si>
+    <t>benzoylecgonine (BZ)</t>
+  </si>
+  <si>
+    <t>phenacetin</t>
+  </si>
+  <si>
+    <t>non-specific sugars</t>
+  </si>
+  <si>
+    <t>methamphetamine</t>
+  </si>
+  <si>
     <t>4-ANPP</t>
   </si>
   <si>
+    <t>tramadol</t>
+  </si>
+  <si>
+    <t>despropionyl p-fluorofentanyl</t>
+  </si>
+  <si>
+    <t>p-fluoro phenethyl 4-ANPP</t>
+  </si>
+  <si>
+    <t>fentanyl</t>
+  </si>
+  <si>
+    <t>methamphetamine</t>
+  </si>
+  <si>
+    <t>caffeine</t>
+  </si>
+  <si>
+    <t>eutylone</t>
+  </si>
+  <si>
+    <t>xylazine</t>
+  </si>
+  <si>
+    <t>urea</t>
+  </si>
+  <si>
+    <t>4-ANPP</t>
+  </si>
+  <si>
+    <t>heroin</t>
+  </si>
+  <si>
+    <t>fentanyl</t>
+  </si>
+  <si>
+    <t>6-monoacetylmorphine (6-MAM)</t>
+  </si>
+  <si>
+    <t>non-specific sugars</t>
+  </si>
+  <si>
+    <t>acetylcodeine</t>
+  </si>
+  <si>
     <t>phenethyl 4-ANPP</t>
   </si>
   <si>
+    <t>caffeine</t>
+  </si>
+  <si>
+    <t>cocaine</t>
+  </si>
+  <si>
     <t>fentanyl</t>
   </si>
   <si>
+    <t>4-ANPP</t>
+  </si>
+  <si>
+    <t>fentanyl</t>
+  </si>
+  <si>
+    <t>N-phenylpropanamide</t>
+  </si>
+  <si>
+    <t>N-ethyl-4-ANPP</t>
+  </si>
+  <si>
+    <t>acetaminophen</t>
+  </si>
+  <si>
+    <t>phenethyl 4-ANPP</t>
+  </si>
+  <si>
+    <t>4-ANPP</t>
+  </si>
+  <si>
+    <t>xylazine</t>
+  </si>
+  <si>
+    <t>1,3-Diacetin</t>
+  </si>
+  <si>
+    <t>lidocaine</t>
+  </si>
+  <si>
     <t>p-fluorofentanyl</t>
   </si>
   <si>
+    <t>heroin</t>
+  </si>
+  <si>
+    <t>acetylcodeine</t>
+  </si>
+  <si>
+    <t>dimethyl sulfone (methylsulfonylmethane MSM)</t>
+  </si>
+  <si>
+    <t>tramadol</t>
+  </si>
+  <si>
+    <t>6-monoacetylmorphine (6-MAM)</t>
+  </si>
+  <si>
+    <t>acetylcodeine</t>
+  </si>
+  <si>
+    <t>1,3-Diacetin</t>
+  </si>
+  <si>
+    <t>fentanyl</t>
+  </si>
+  <si>
+    <t>non-specific sugars</t>
+  </si>
+  <si>
+    <t>diphenhydramine</t>
+  </si>
+  <si>
+    <t>phenethyl 4-ANPP</t>
+  </si>
+  <si>
+    <t>heroin</t>
+  </si>
+  <si>
+    <t>methamphetamine</t>
+  </si>
+  <si>
+    <t>inositol</t>
+  </si>
+  <si>
+    <t>methadone</t>
+  </si>
+  <si>
+    <t>N-piperidinyl etonitazene</t>
+  </si>
+  <si>
+    <t>quinine</t>
+  </si>
+  <si>
+    <t>4-ANPP</t>
+  </si>
+  <si>
+    <t>metonitazene</t>
+  </si>
+  <si>
+    <t>gabapentin</t>
+  </si>
+  <si>
+    <t>dimethyl sulfone (methylsulfonylmethane MSM)</t>
+  </si>
+  <si>
+    <t>non-specific organic acids</t>
+  </si>
+  <si>
+    <t>fentanyl</t>
+  </si>
+  <si>
+    <t>methamphetamine</t>
+  </si>
+  <si>
+    <t>cocaine</t>
+  </si>
+  <si>
+    <t>xylazine</t>
+  </si>
+  <si>
+    <t>heroin</t>
+  </si>
+  <si>
+    <t>procaine</t>
+  </si>
+  <si>
+    <t>fentanyl</t>
+  </si>
+  <si>
+    <t>4-ANPP</t>
+  </si>
+  <si>
+    <t>xylazine</t>
+  </si>
+  <si>
     <t>despropionyl p-fluorofentanyl</t>
   </si>
   <si>
-    <t>xylazine</t>
-  </si>
-  <si>
-    <t>3,4-methylenedioxy-N-benzylcathinone (BMDP)</t>
-  </si>
-  <si>
-    <t>3,4-MDMA</t>
-  </si>
-  <si>
-    <t>benzoylecgonine (BZ)</t>
-  </si>
-  <si>
-    <t>phenacetin</t>
+    <t>phenethylbromide</t>
+  </si>
+  <si>
+    <t>p-fluorofentanyl</t>
+  </si>
+  <si>
+    <t>menthol</t>
+  </si>
+  <si>
+    <t>phenethyl chloride</t>
+  </si>
+  <si>
+    <t>nicotine</t>
+  </si>
+  <si>
+    <t>p-fluoro phenethyl 4-ANPP</t>
+  </si>
+  <si>
+    <t>1,3-Diacetin</t>
+  </si>
+  <si>
+    <t>diphenhydramine</t>
+  </si>
+  <si>
+    <t>N-ethyl-4-ANPP</t>
+  </si>
+  <si>
+    <t>1,3-Diacetin</t>
+  </si>
+  <si>
+    <t>fentanyl</t>
+  </si>
+  <si>
+    <t>p-fluorofentanyl</t>
+  </si>
+  <si>
+    <t>quinine</t>
+  </si>
+  <si>
+    <t>4-ANPP</t>
+  </si>
+  <si>
+    <t>1-phenethyl-4-propionyloxypiperidine</t>
+  </si>
+  <si>
+    <t>caffeine</t>
+  </si>
+  <si>
+    <t>N-phenylpropanamide</t>
+  </si>
+  <si>
+    <t>N-ethyl-4-ANPP</t>
+  </si>
+  <si>
+    <t>acetaminophen</t>
+  </si>
+  <si>
+    <t>tramadol</t>
+  </si>
+  <si>
+    <t>4-ANPP</t>
+  </si>
+  <si>
+    <t>methamphetamine</t>
+  </si>
+  <si>
+    <t>fentanyl</t>
+  </si>
+  <si>
+    <t>methamphetamine</t>
+  </si>
+  <si>
+    <t>fentanyl</t>
+  </si>
+  <si>
+    <t>tropacocaine</t>
+  </si>
+  <si>
+    <t>levamisole</t>
+  </si>
+  <si>
+    <t>cocaine</t>
+  </si>
+  <si>
+    <t>ecgonine methylester (EME)</t>
   </si>
   <si>
     <t>methyl ecgonidine (MED)</t>
   </si>
   <si>
-    <t>norcocaine</t>
-  </si>
-  <si>
-    <t>cocaine</t>
-  </si>
-  <si>
-    <t>levamisole</t>
-  </si>
-  <si>
-    <t>tropacocaine</t>
-  </si>
-  <si>
-    <t>fentanyl</t>
-  </si>
-  <si>
-    <t>tramadol</t>
-  </si>
-  <si>
     <t>methamphetamine</t>
   </si>
   <si>
-    <t>despropionyl p-fluorofentanyl</t>
-  </si>
-  <si>
-    <t>4-ANPP</t>
-  </si>
-  <si>
-    <t>p-fluoro phenethyl 4-ANPP</t>
-  </si>
-  <si>
-    <t>non-specific sugars</t>
-  </si>
-  <si>
-    <t>caffeine</t>
-  </si>
-  <si>
-    <t>methamphetamine</t>
-  </si>
-  <si>
-    <t>eutylone</t>
-  </si>
-  <si>
-    <t>xylazine</t>
-  </si>
-  <si>
-    <t>urea</t>
-  </si>
-  <si>
-    <t>acetylcodeine</t>
-  </si>
-  <si>
-    <t>6-monoacetylmorphine (6-MAM)</t>
-  </si>
-  <si>
-    <t>phenethyl 4-ANPP</t>
-  </si>
-  <si>
-    <t>4-ANPP</t>
-  </si>
-  <si>
-    <t>non-specific sugars</t>
-  </si>
-  <si>
-    <t>fentanyl</t>
-  </si>
-  <si>
-    <t>heroin</t>
-  </si>
-  <si>
-    <t>cocaine</t>
-  </si>
-  <si>
-    <t>caffeine</t>
-  </si>
-  <si>
-    <t>4-ANPP</t>
-  </si>
-  <si>
-    <t>fentanyl</t>
-  </si>
-  <si>
-    <t>N-phenylpropanamide</t>
-  </si>
-  <si>
-    <t>tramadol</t>
-  </si>
-  <si>
-    <t>N-ethyl-4-ANPP</t>
-  </si>
-  <si>
-    <t>6-monoacetylmorphine (6-MAM)</t>
-  </si>
-  <si>
-    <t>p-fluorofentanyl</t>
-  </si>
-  <si>
-    <t>acetylcodeine</t>
-  </si>
-  <si>
-    <t>4-ANPP</t>
-  </si>
-  <si>
-    <t>acetaminophen</t>
-  </si>
-  <si>
-    <t>heroin</t>
-  </si>
-  <si>
-    <t>xylazine</t>
-  </si>
-  <si>
-    <t>lidocaine</t>
-  </si>
-  <si>
-    <t>phenethyl 4-ANPP</t>
-  </si>
-  <si>
-    <t>dimethyl sulfone (methylsulfonylmethane MSM)</t>
-  </si>
-  <si>
-    <t>fentanyl</t>
-  </si>
-  <si>
-    <t>1,3-Diacetin</t>
-  </si>
-  <si>
-    <t>N-piperidinyl etonitazene</t>
-  </si>
-  <si>
-    <t>4-ANPP</t>
-  </si>
-  <si>
-    <t>inositol</t>
-  </si>
-  <si>
-    <t>methamphetamine</t>
-  </si>
-  <si>
-    <t>non-specific sugars</t>
-  </si>
-  <si>
-    <t>methadone</t>
-  </si>
-  <si>
-    <t>heroin</t>
-  </si>
-  <si>
-    <t>diphenhydramine</t>
-  </si>
-  <si>
-    <t>quinine</t>
-  </si>
-  <si>
-    <t>fentanyl</t>
-  </si>
-  <si>
-    <t>phenethyl 4-ANPP</t>
-  </si>
-  <si>
-    <t>acetylcodeine</t>
-  </si>
-  <si>
-    <t>1,3-Diacetin</t>
-  </si>
-  <si>
-    <t>metonitazene</t>
-  </si>
-  <si>
-    <t>gabapentin</t>
-  </si>
-  <si>
-    <t>dimethyl sulfone (methylsulfonylmethane MSM)</t>
-  </si>
-  <si>
-    <t>non-specific organic acids</t>
-  </si>
-  <si>
-    <t>fentanyl</t>
-  </si>
-  <si>
-    <t>methamphetamine</t>
-  </si>
-  <si>
-    <t>xylazine</t>
-  </si>
-  <si>
-    <t>fentanyl</t>
-  </si>
-  <si>
-    <t>4-ANPP</t>
-  </si>
-  <si>
-    <t>procaine</t>
-  </si>
-  <si>
-    <t>cocaine</t>
-  </si>
-  <si>
-    <t>heroin</t>
-  </si>
-  <si>
-    <t>menthol</t>
-  </si>
-  <si>
-    <t>phenethylbromide</t>
-  </si>
-  <si>
-    <t>p-fluoro phenethyl 4-ANPP</t>
-  </si>
-  <si>
-    <t>xylazine</t>
-  </si>
-  <si>
-    <t>1,3-Diacetin</t>
-  </si>
-  <si>
-    <t>phenethyl chloride</t>
-  </si>
-  <si>
-    <t>p-fluorofentanyl</t>
-  </si>
-  <si>
-    <t>nicotine</t>
-  </si>
-  <si>
-    <t>despropionyl p-fluorofentanyl</t>
-  </si>
-  <si>
-    <t>1-phenethyl-4-propionyloxypiperidine</t>
-  </si>
-  <si>
-    <t>fentanyl</t>
-  </si>
-  <si>
-    <t>diphenhydramine</t>
-  </si>
-  <si>
-    <t>N-ethyl-4-ANPP</t>
-  </si>
-  <si>
-    <t>1,3-Diacetin</t>
-  </si>
-  <si>
-    <t>p-fluorofentanyl</t>
-  </si>
-  <si>
-    <t>quinine</t>
-  </si>
-  <si>
-    <t>4-ANPP</t>
-  </si>
-  <si>
-    <t>caffeine</t>
-  </si>
-  <si>
-    <t>fentanyl</t>
-  </si>
-  <si>
-    <t>N-phenylpropanamide</t>
-  </si>
-  <si>
-    <t>N-ethyl-4-ANPP</t>
-  </si>
-  <si>
-    <t>methamphetamine</t>
-  </si>
-  <si>
-    <t>4-ANPP</t>
-  </si>
-  <si>
-    <t>acetaminophen</t>
-  </si>
-  <si>
-    <t>tramadol</t>
-  </si>
-  <si>
-    <t>methamphetamine</t>
-  </si>
-  <si>
-    <t>fentanyl</t>
-  </si>
-  <si>
-    <t>cocaine</t>
-  </si>
-  <si>
-    <t>ecgonine methylester (EME)</t>
-  </si>
-  <si>
-    <t>levamisole</t>
-  </si>
-  <si>
-    <t>tropacocaine</t>
-  </si>
-  <si>
-    <t>methyl ecgonidine (MED)</t>
-  </si>
-  <si>
-    <t>methamphetamine</t>
-  </si>
-  <si>
     <t>no compounds of interest detected</t>
   </si>
   <si>
@@ -444,9 +447,15 @@
     <t/>
   </si>
   <si>
+    <t>trace</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>trace</t>
   </si>
   <si>
@@ -471,6 +480,9 @@
     <t/>
   </si>
   <si>
+    <t>trace</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
@@ -480,6 +492,9 @@
     <t/>
   </si>
   <si>
+    <t>trace</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
@@ -489,21 +504,33 @@
     <t/>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>trace</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>trace</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
+    <t>trace</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
+    <t>trace</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
@@ -513,12 +540,21 @@
     <t/>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>trace</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t>trace</t>
   </si>
   <si>
@@ -531,30 +567,81 @@
     <t/>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t>trace</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t>trace</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
+    <t>trace</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
     <t/>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>trace</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
+    <t>trace</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
@@ -567,6 +654,9 @@
     <t/>
   </si>
   <si>
+    <t>trace</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
@@ -576,12 +666,21 @@
     <t/>
   </si>
   <si>
+    <t>trace</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
+    <t>trace</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>trace</t>
   </si>
   <si>
@@ -591,6 +690,9 @@
     <t/>
   </si>
   <si>
+    <t>trace</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
@@ -603,102 +705,6 @@
     <t/>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>trace</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>trace</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>trace</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>trace</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>trace</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>trace</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>trace</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>trace</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>trace</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>trace</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
     <t>method</t>
   </si>
   <si>
@@ -751,15 +757,6 @@
   </si>
   <si>
     <t>GCMS</t>
-  </si>
-  <si>
-    <t>Derivatized GCMS</t>
-  </si>
-  <si>
-    <t>GCMS</t>
-  </si>
-  <si>
-    <t>Derivatized GCMS</t>
   </si>
   <si>
     <t>date_complete</t>
@@ -881,73 +878,73 @@
         <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D1" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="E1" t="s">
+        <v>248</v>
+      </c>
+      <c r="F1" t="s">
         <v>249</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>250</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>251</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>252</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>253</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>254</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>255</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>256</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>257</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>258</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>259</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>260</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>261</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>262</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>263</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>264</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>265</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>266</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>267</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>268</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="2">
@@ -958,10 +955,10 @@
         <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D2" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="E2" s="1">
         <v>44603</v>
@@ -1033,10 +1030,10 @@
         <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D3" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="E3" s="1">
         <v>44603</v>
@@ -1061,10 +1058,10 @@
         <v>0</v>
       </c>
       <c r="M3" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N3" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O3" s="2">
         <v>0</v>
@@ -1108,10 +1105,10 @@
         <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D4" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="E4" s="1">
         <v>44603</v>
@@ -1130,10 +1127,10 @@
         <v>7</v>
       </c>
       <c r="K4" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M4" s="2">
         <v>0</v>
@@ -1183,10 +1180,10 @@
         <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D5" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="E5" s="1">
         <v>44603</v>
@@ -1205,10 +1202,10 @@
         <v>7</v>
       </c>
       <c r="K5" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L5" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M5" s="2">
         <v>0</v>
@@ -1258,10 +1255,10 @@
         <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D6" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="E6" s="1">
         <v>44603</v>
@@ -1333,10 +1330,10 @@
         <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D7" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="E7" s="1">
         <v>44603</v>
@@ -1408,10 +1405,10 @@
         <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D8" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="E8" s="1">
         <v>44603</v>
@@ -1436,10 +1433,10 @@
         <v>0</v>
       </c>
       <c r="M8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O8" s="2">
         <v>0</v>
@@ -1483,19 +1480,19 @@
         <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D9" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="E9" s="1">
         <v>44777</v>
       </c>
       <c r="F9" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2">
@@ -1532,7 +1529,7 @@
         <v>0</v>
       </c>
       <c r="T9" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U9" s="2">
         <v>0</v>
@@ -1558,19 +1555,19 @@
         <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D10" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="E10" s="1">
         <v>44777</v>
       </c>
       <c r="F10" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2">
@@ -1607,7 +1604,7 @@
         <v>0</v>
       </c>
       <c r="T10" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U10" s="2">
         <v>0</v>
@@ -1630,13 +1627,13 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D11" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="E11" s="1">
         <v>44758</v>
@@ -1705,13 +1702,13 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D12" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E12" s="1">
         <v>44714</v>
@@ -1780,13 +1777,13 @@
         <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D13" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E13" s="1">
         <v>44714</v>
@@ -1829,7 +1826,7 @@
         <v>0</v>
       </c>
       <c r="S13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T13" s="2">
         <v>0</v>
@@ -1855,10 +1852,10 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D14" t="s">
         <v>231</v>
@@ -1867,10 +1864,10 @@
         <v>44714</v>
       </c>
       <c r="F14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2">
@@ -1919,7 +1916,7 @@
         <v>0</v>
       </c>
       <c r="X14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y14" s="2">
         <v>0</v>
@@ -1930,10 +1927,10 @@
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D15" t="s">
         <v>231</v>
@@ -2005,10 +2002,10 @@
         <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D16" t="s">
         <v>231</v>
@@ -2017,10 +2014,10 @@
         <v>44714</v>
       </c>
       <c r="F16" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2">
@@ -2069,7 +2066,7 @@
         <v>0</v>
       </c>
       <c r="X16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y16" s="2">
         <v>0</v>
@@ -2080,13 +2077,13 @@
         <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C17" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D17" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E17" s="1">
         <v>44714</v>
@@ -2129,7 +2126,7 @@
         <v>0</v>
       </c>
       <c r="S17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T17" s="2">
         <v>0</v>
@@ -2144,7 +2141,7 @@
         <v>0</v>
       </c>
       <c r="X17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y17" s="2">
         <v>0</v>
@@ -2155,13 +2152,13 @@
         <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C18" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D18" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E18" s="1">
         <v>44714</v>
@@ -2219,7 +2216,7 @@
         <v>0</v>
       </c>
       <c r="X18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y18" s="2">
         <v>0</v>
@@ -2230,13 +2227,13 @@
         <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C19" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D19" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E19" s="1">
         <v>44759</v>
@@ -2255,10 +2252,10 @@
         <v>4</v>
       </c>
       <c r="K19" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L19" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M19" s="2">
         <v>0</v>
@@ -2305,13 +2302,13 @@
         <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C20" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D20" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E20" s="1">
         <v>44759</v>
@@ -2345,7 +2342,7 @@
         <v>0</v>
       </c>
       <c r="P20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q20" s="2">
         <v>0</v>
@@ -2360,7 +2357,7 @@
         <v>0</v>
       </c>
       <c r="U20" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V20" s="2">
         <v>0</v>
@@ -2380,22 +2377,22 @@
         <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D21" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E21" s="1">
         <v>44759</v>
       </c>
       <c r="F21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2">
@@ -2420,7 +2417,7 @@
         <v>0</v>
       </c>
       <c r="P21" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q21" s="2">
         <v>0</v>
@@ -2455,10 +2452,10 @@
         <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C22" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D22" t="s">
         <v>233</v>
@@ -2467,10 +2464,10 @@
         <v>44759</v>
       </c>
       <c r="F22" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="2">
@@ -2510,7 +2507,7 @@
         <v>0</v>
       </c>
       <c r="U22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V22" s="2">
         <v>0</v>
@@ -2530,10 +2527,10 @@
         <v>5</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C23" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D23" t="s">
         <v>233</v>
@@ -2605,10 +2602,10 @@
         <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C24" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D24" t="s">
         <v>233</v>
@@ -2680,13 +2677,13 @@
         <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C25" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D25" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E25" s="1">
         <v>44759</v>
@@ -2705,10 +2702,10 @@
         <v>4</v>
       </c>
       <c r="K25" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L25" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M25" s="2">
         <v>0</v>
@@ -2755,22 +2752,22 @@
         <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C26" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D26" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E26" s="1">
         <v>44721</v>
       </c>
       <c r="F26" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G26" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26" s="2"/>
       <c r="I26" s="2">
@@ -2795,10 +2792,10 @@
         <v>0</v>
       </c>
       <c r="P26" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q26" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R26" s="2">
         <v>0</v>
@@ -2830,22 +2827,22 @@
         <v>6</v>
       </c>
       <c r="B27" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C27" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D27" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E27" s="1">
         <v>44721</v>
       </c>
       <c r="F27" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G27" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H27" s="2"/>
       <c r="I27" s="2">
@@ -2870,10 +2867,10 @@
         <v>0</v>
       </c>
       <c r="P27" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q27" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R27" s="2">
         <v>0</v>
@@ -2905,13 +2902,13 @@
         <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C28" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="D28" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E28" s="1">
         <v>44721</v>
@@ -2980,13 +2977,13 @@
         <v>7</v>
       </c>
       <c r="B29" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C29" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="D29" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E29" s="1">
         <v>44707</v>
@@ -3055,13 +3052,13 @@
         <v>7</v>
       </c>
       <c r="B30" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C30" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="D30" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E30" s="1">
         <v>44707</v>
@@ -3130,22 +3127,22 @@
         <v>7</v>
       </c>
       <c r="B31" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C31" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E31" s="1">
         <v>44707</v>
       </c>
       <c r="F31" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H31" s="2"/>
       <c r="I31" s="2">
@@ -3205,22 +3202,22 @@
         <v>7</v>
       </c>
       <c r="B32" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C32" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D32" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E32" s="1">
         <v>44707</v>
       </c>
       <c r="F32" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G32" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H32" s="2"/>
       <c r="I32" s="2">
@@ -3280,22 +3277,22 @@
         <v>7</v>
       </c>
       <c r="B33" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C33" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="D33" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="E33" s="1">
         <v>44707</v>
       </c>
       <c r="F33" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G33" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H33" s="2"/>
       <c r="I33" s="2">
@@ -3305,10 +3302,10 @@
         <v>5</v>
       </c>
       <c r="K33" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L33" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M33" s="2">
         <v>0</v>
@@ -3355,13 +3352,13 @@
         <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C34" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="D34" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="E34" s="1">
         <v>44707</v>
@@ -3430,13 +3427,13 @@
         <v>7</v>
       </c>
       <c r="B35" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C35" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="D35" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="E35" s="1">
         <v>44707</v>
@@ -3505,13 +3502,13 @@
         <v>7</v>
       </c>
       <c r="B36" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C36" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="D36" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E36" s="1">
         <v>44707</v>
@@ -3530,10 +3527,10 @@
         <v>5</v>
       </c>
       <c r="K36" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L36" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M36" s="2">
         <v>0</v>
@@ -3580,22 +3577,22 @@
         <v>7</v>
       </c>
       <c r="B37" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C37" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="D37" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E37" s="1">
         <v>44707</v>
       </c>
       <c r="F37" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G37" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H37" s="2"/>
       <c r="I37" s="2">
@@ -3655,22 +3652,22 @@
         <v>8</v>
       </c>
       <c r="B38" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C38" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="D38" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E38" s="1">
         <v>44789</v>
       </c>
       <c r="F38" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G38" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H38" s="2"/>
       <c r="I38" s="2">
@@ -3698,7 +3695,7 @@
         <v>0</v>
       </c>
       <c r="Q38" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R38" s="2">
         <v>0</v>
@@ -3730,22 +3727,22 @@
         <v>8</v>
       </c>
       <c r="B39" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C39" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="D39" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E39" s="1">
         <v>44789</v>
       </c>
       <c r="F39" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G39" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H39" s="2"/>
       <c r="I39" s="2">
@@ -3773,7 +3770,7 @@
         <v>0</v>
       </c>
       <c r="Q39" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R39" s="2">
         <v>0</v>
@@ -3805,22 +3802,22 @@
         <v>8</v>
       </c>
       <c r="B40" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C40" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="D40" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E40" s="1">
         <v>44789</v>
       </c>
       <c r="F40" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G40" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H40" s="2"/>
       <c r="I40" s="2">
@@ -3830,10 +3827,10 @@
         <v>2</v>
       </c>
       <c r="K40" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L40" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M40" s="2">
         <v>0</v>
@@ -3880,22 +3877,22 @@
         <v>8</v>
       </c>
       <c r="B41" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C41" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="D41" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E41" s="1">
         <v>44789</v>
       </c>
       <c r="F41" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G41" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H41" s="2"/>
       <c r="I41" s="2">
@@ -3905,10 +3902,10 @@
         <v>2</v>
       </c>
       <c r="K41" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L41" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M41" s="2">
         <v>0</v>
@@ -3955,22 +3952,22 @@
         <v>9</v>
       </c>
       <c r="B42" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C42" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="D42" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E42" s="1">
         <v>44818</v>
       </c>
       <c r="F42" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G42" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H42" s="2"/>
       <c r="I42" s="2">
@@ -3980,10 +3977,10 @@
         <v>3</v>
       </c>
       <c r="K42" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L42" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M42" s="2">
         <v>0</v>
@@ -4030,13 +4027,13 @@
         <v>9</v>
       </c>
       <c r="B43" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C43" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="D43" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E43" s="1">
         <v>44818</v>
@@ -4085,7 +4082,7 @@
         <v>0</v>
       </c>
       <c r="U43" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V43" s="2">
         <v>0</v>
@@ -4105,13 +4102,13 @@
         <v>9</v>
       </c>
       <c r="B44" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C44" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="D44" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E44" s="1">
         <v>44818</v>
@@ -4180,13 +4177,13 @@
         <v>9</v>
       </c>
       <c r="B45" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C45" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="D45" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E45" s="1">
         <v>44818</v>
@@ -4255,13 +4252,13 @@
         <v>9</v>
       </c>
       <c r="B46" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C46" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="D46" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E46" s="1">
         <v>44818</v>
@@ -4330,22 +4327,22 @@
         <v>9</v>
       </c>
       <c r="B47" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C47" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="D47" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E47" s="1">
         <v>44818</v>
       </c>
       <c r="F47" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G47" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H47" s="2"/>
       <c r="I47" s="2">
@@ -4405,13 +4402,13 @@
         <v>9</v>
       </c>
       <c r="B48" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C48" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="D48" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E48" s="1">
         <v>44818</v>
@@ -4436,10 +4433,10 @@
         <v>0</v>
       </c>
       <c r="M48" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N48" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O48" s="2">
         <v>0</v>
@@ -4480,13 +4477,13 @@
         <v>9</v>
       </c>
       <c r="B49" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C49" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="D49" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E49" s="1">
         <v>44818</v>
@@ -4555,13 +4552,13 @@
         <v>9</v>
       </c>
       <c r="B50" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C50" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="D50" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E50" s="1">
         <v>44818</v>
@@ -4630,22 +4627,22 @@
         <v>9</v>
       </c>
       <c r="B51" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C51" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="D51" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E51" s="1">
         <v>44818</v>
       </c>
       <c r="F51" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G51" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H51" s="2"/>
       <c r="I51" s="2">
@@ -4661,10 +4658,10 @@
         <v>0</v>
       </c>
       <c r="M51" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N51" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O51" s="2">
         <v>0</v>
@@ -4705,13 +4702,13 @@
         <v>9</v>
       </c>
       <c r="B52" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C52" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D52" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E52" s="1">
         <v>44818</v>
@@ -4780,13 +4777,13 @@
         <v>9</v>
       </c>
       <c r="B53" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C53" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D53" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E53" s="1">
         <v>44818</v>
@@ -4855,13 +4852,13 @@
         <v>9</v>
       </c>
       <c r="B54" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C54" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D54" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E54" s="1">
         <v>44818</v>
@@ -4930,22 +4927,22 @@
         <v>9</v>
       </c>
       <c r="B55" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C55" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="D55" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E55" s="1">
         <v>44818</v>
       </c>
       <c r="F55" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G55" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H55" s="2"/>
       <c r="I55" s="2">
@@ -4955,10 +4952,10 @@
         <v>3</v>
       </c>
       <c r="K55" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L55" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M55" s="2">
         <v>0</v>
@@ -4985,7 +4982,7 @@
         <v>0</v>
       </c>
       <c r="U55" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V55" s="2">
         <v>0</v>
@@ -5005,13 +5002,13 @@
         <v>9</v>
       </c>
       <c r="B56" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C56" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D56" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E56" s="1">
         <v>44818</v>
@@ -5080,22 +5077,22 @@
         <v>10</v>
       </c>
       <c r="B57" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C57" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D57" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E57" s="1">
         <v>44771</v>
       </c>
       <c r="F57" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G57" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H57" s="2"/>
       <c r="I57" s="2">
@@ -5155,13 +5152,13 @@
         <v>10</v>
       </c>
       <c r="B58" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C58" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D58" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E58" s="1">
         <v>44771</v>
@@ -5230,13 +5227,13 @@
         <v>10</v>
       </c>
       <c r="B59" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C59" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D59" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="E59" s="1">
         <v>44771</v>
@@ -5255,10 +5252,10 @@
         <v>11</v>
       </c>
       <c r="K59" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L59" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M59" s="2">
         <v>0</v>
@@ -5305,22 +5302,22 @@
         <v>10</v>
       </c>
       <c r="B60" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C60" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D60" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="E60" s="1">
         <v>44771</v>
       </c>
       <c r="F60" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G60" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H60" s="2"/>
       <c r="I60" s="2">
@@ -5345,7 +5342,7 @@
         <v>0</v>
       </c>
       <c r="P60" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q60" s="2">
         <v>0</v>
@@ -5380,22 +5377,22 @@
         <v>10</v>
       </c>
       <c r="B61" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C61" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D61" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="E61" s="1">
         <v>44771</v>
       </c>
       <c r="F61" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G61" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H61" s="2"/>
       <c r="I61" s="2">
@@ -5455,22 +5452,22 @@
         <v>10</v>
       </c>
       <c r="B62" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C62" t="s">
         <v>180</v>
       </c>
       <c r="D62" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="E62" s="1">
         <v>44771</v>
       </c>
       <c r="F62" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G62" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H62" s="2"/>
       <c r="I62" s="2">
@@ -5530,13 +5527,13 @@
         <v>10</v>
       </c>
       <c r="B63" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C63" t="s">
         <v>181</v>
       </c>
       <c r="D63" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="E63" s="1">
         <v>44771</v>
@@ -5605,13 +5602,13 @@
         <v>10</v>
       </c>
       <c r="B64" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C64" t="s">
         <v>182</v>
       </c>
       <c r="D64" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="E64" s="1">
         <v>44771</v>
@@ -5645,7 +5642,7 @@
         <v>0</v>
       </c>
       <c r="P64" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q64" s="2">
         <v>0</v>
@@ -5680,13 +5677,13 @@
         <v>10</v>
       </c>
       <c r="B65" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C65" t="s">
         <v>183</v>
       </c>
       <c r="D65" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="E65" s="1">
         <v>44771</v>
@@ -5755,13 +5752,13 @@
         <v>10</v>
       </c>
       <c r="B66" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C66" t="s">
         <v>184</v>
       </c>
       <c r="D66" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="E66" s="1">
         <v>44771</v>
@@ -5780,10 +5777,10 @@
         <v>11</v>
       </c>
       <c r="K66" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L66" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M66" s="2">
         <v>0</v>
@@ -5830,22 +5827,22 @@
         <v>10</v>
       </c>
       <c r="B67" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C67" t="s">
         <v>185</v>
       </c>
       <c r="D67" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="E67" s="1">
         <v>44771</v>
       </c>
       <c r="F67" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G67" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H67" s="2"/>
       <c r="I67" s="2">
@@ -5905,22 +5902,22 @@
         <v>10</v>
       </c>
       <c r="B68" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C68" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D68" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E68" s="1">
         <v>44771</v>
       </c>
       <c r="F68" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G68" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H68" s="2"/>
       <c r="I68" s="2">
@@ -5980,13 +5977,13 @@
         <v>10</v>
       </c>
       <c r="B69" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C69" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D69" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E69" s="1">
         <v>44771</v>
@@ -6055,13 +6052,13 @@
         <v>10</v>
       </c>
       <c r="B70" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C70" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D70" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E70" s="1">
         <v>44771</v>
@@ -6130,13 +6127,13 @@
         <v>10</v>
       </c>
       <c r="B71" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C71" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D71" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E71" s="1">
         <v>44771</v>
@@ -6205,13 +6202,13 @@
         <v>11</v>
       </c>
       <c r="B72" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C72" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D72" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E72" s="1">
         <v>44845</v>
@@ -6280,13 +6277,13 @@
         <v>11</v>
       </c>
       <c r="B73" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C73" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D73" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E73" s="1">
         <v>44845</v>
@@ -6355,13 +6352,13 @@
         <v>11</v>
       </c>
       <c r="B74" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C74" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D74" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E74" s="1">
         <v>44845</v>
@@ -6430,13 +6427,13 @@
         <v>12</v>
       </c>
       <c r="B75" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C75" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D75" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E75" s="1">
         <v>44803</v>
@@ -6505,13 +6502,13 @@
         <v>13</v>
       </c>
       <c r="B76" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C76" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D76" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E76" s="1">
         <v>44840</v>
@@ -6536,10 +6533,10 @@
         <v>0</v>
       </c>
       <c r="M76" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N76" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O76" s="2">
         <v>0</v>
@@ -6580,13 +6577,13 @@
         <v>13</v>
       </c>
       <c r="B77" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C77" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D77" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E77" s="1">
         <v>44840</v>
@@ -6605,16 +6602,16 @@
         <v>6</v>
       </c>
       <c r="K77" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L77" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M77" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N77" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O77" s="2">
         <v>0</v>
@@ -6655,13 +6652,13 @@
         <v>13</v>
       </c>
       <c r="B78" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C78" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D78" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E78" s="1">
         <v>44840</v>
@@ -6730,13 +6727,13 @@
         <v>13</v>
       </c>
       <c r="B79" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C79" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D79" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E79" s="1">
         <v>44840</v>
@@ -6805,13 +6802,13 @@
         <v>13</v>
       </c>
       <c r="B80" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C80" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D80" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E80" s="1">
         <v>44840</v>
@@ -6830,10 +6827,10 @@
         <v>6</v>
       </c>
       <c r="K80" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L80" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M80" s="2">
         <v>0</v>
@@ -6880,13 +6877,13 @@
         <v>13</v>
       </c>
       <c r="B81" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C81" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D81" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E81" s="1">
         <v>44840</v>
@@ -6955,22 +6952,22 @@
         <v>14</v>
       </c>
       <c r="B82" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C82" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D82" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E82" s="1">
         <v>44894</v>
       </c>
       <c r="F82" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G82" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H82" s="2"/>
       <c r="I82" s="2">
@@ -6989,7 +6986,7 @@
         <v>0</v>
       </c>
       <c r="N82" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O82" s="2">
         <v>0</v>
@@ -7030,22 +7027,22 @@
         <v>14</v>
       </c>
       <c r="B83" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C83" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D83" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E83" s="1">
         <v>44894</v>
       </c>
       <c r="F83" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G83" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H83" s="2"/>
       <c r="I83" s="2">
@@ -7105,13 +7102,13 @@
         <v>14</v>
       </c>
       <c r="B84" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C84" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="D84" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E84" s="1">
         <v>44894</v>
@@ -7180,22 +7177,22 @@
         <v>14</v>
       </c>
       <c r="B85" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C85" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="D85" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E85" s="1">
         <v>44894</v>
       </c>
       <c r="F85" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G85" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H85" s="2"/>
       <c r="I85" s="2">
@@ -7214,7 +7211,7 @@
         <v>0</v>
       </c>
       <c r="N85" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O85" s="2">
         <v>0</v>
@@ -7255,22 +7252,22 @@
         <v>14</v>
       </c>
       <c r="B86" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C86" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="D86" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E86" s="1">
         <v>44894</v>
       </c>
       <c r="F86" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G86" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H86" s="2"/>
       <c r="I86" s="2">
@@ -7330,13 +7327,13 @@
         <v>14</v>
       </c>
       <c r="B87" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C87" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="D87" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E87" s="1">
         <v>44894</v>
@@ -7405,22 +7402,22 @@
         <v>14</v>
       </c>
       <c r="B88" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C88" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="D88" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E88" s="1">
         <v>44894</v>
       </c>
       <c r="F88" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G88" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H88" s="2"/>
       <c r="I88" s="2">
@@ -7480,13 +7477,13 @@
         <v>14</v>
       </c>
       <c r="B89" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C89" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="D89" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E89" s="1">
         <v>44894</v>
@@ -7555,22 +7552,22 @@
         <v>14</v>
       </c>
       <c r="B90" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C90" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="D90" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E90" s="1">
         <v>44894</v>
       </c>
       <c r="F90" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G90" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H90" s="2"/>
       <c r="I90" s="2">
@@ -7630,22 +7627,22 @@
         <v>15</v>
       </c>
       <c r="B91" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C91" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D91" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E91" s="1">
         <v>44865</v>
       </c>
       <c r="F91" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G91" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H91" s="2"/>
       <c r="I91" s="2">
@@ -7705,22 +7702,22 @@
         <v>15</v>
       </c>
       <c r="B92" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C92" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D92" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E92" s="1">
         <v>44865</v>
       </c>
       <c r="F92" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G92" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H92" s="2"/>
       <c r="I92" s="2">
@@ -7730,10 +7727,10 @@
         <v>5</v>
       </c>
       <c r="K92" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L92" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M92" s="2">
         <v>0</v>
@@ -7780,13 +7777,13 @@
         <v>15</v>
       </c>
       <c r="B93" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C93" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="D93" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E93" s="1">
         <v>44865</v>
@@ -7855,22 +7852,22 @@
         <v>15</v>
       </c>
       <c r="B94" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C94" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="D94" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E94" s="1">
         <v>44865</v>
       </c>
       <c r="F94" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G94" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H94" s="2"/>
       <c r="I94" s="2">
@@ -7880,10 +7877,10 @@
         <v>5</v>
       </c>
       <c r="K94" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L94" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M94" s="2">
         <v>0</v>
@@ -7930,22 +7927,22 @@
         <v>15</v>
       </c>
       <c r="B95" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C95" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="D95" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E95" s="1">
         <v>44865</v>
       </c>
       <c r="F95" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G95" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H95" s="2"/>
       <c r="I95" s="2">
@@ -8005,13 +8002,13 @@
         <v>15</v>
       </c>
       <c r="B96" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C96" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D96" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E96" s="1">
         <v>44865</v>
@@ -8080,22 +8077,22 @@
         <v>15</v>
       </c>
       <c r="B97" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C97" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="D97" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E97" s="1">
         <v>44865</v>
       </c>
       <c r="F97" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G97" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H97" s="2"/>
       <c r="I97" s="2">
@@ -8155,22 +8152,22 @@
         <v>15</v>
       </c>
       <c r="B98" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C98" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D98" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E98" s="1">
         <v>44865</v>
       </c>
       <c r="F98" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G98" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H98" s="2"/>
       <c r="I98" s="2">
@@ -8230,13 +8227,13 @@
         <v>15</v>
       </c>
       <c r="B99" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C99" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="D99" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E99" s="1">
         <v>44865</v>
@@ -8305,22 +8302,22 @@
         <v>16</v>
       </c>
       <c r="B100" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C100" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="D100" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E100" s="1">
         <v>44879</v>
       </c>
       <c r="F100" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G100" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H100" s="2"/>
       <c r="I100" s="2">
@@ -8330,10 +8327,10 @@
         <v>3</v>
       </c>
       <c r="K100" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L100" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M100" s="2">
         <v>0</v>
@@ -8380,13 +8377,13 @@
         <v>16</v>
       </c>
       <c r="B101" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C101" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D101" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E101" s="1">
         <v>44879</v>
@@ -8455,22 +8452,22 @@
         <v>16</v>
       </c>
       <c r="B102" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C102" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="D102" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E102" s="1">
         <v>44879</v>
       </c>
       <c r="F102" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G102" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H102" s="2"/>
       <c r="I102" s="2">
@@ -8530,13 +8527,13 @@
         <v>16</v>
       </c>
       <c r="B103" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C103" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="D103" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E103" s="1">
         <v>44879</v>
@@ -8570,7 +8567,7 @@
         <v>0</v>
       </c>
       <c r="P103" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q103" s="2">
         <v>0</v>
@@ -8585,7 +8582,7 @@
         <v>0</v>
       </c>
       <c r="U103" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V103" s="2">
         <v>0</v>
@@ -8605,13 +8602,13 @@
         <v>16</v>
       </c>
       <c r="B104" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C104" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="D104" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E104" s="1">
         <v>44879</v>
@@ -8680,22 +8677,22 @@
         <v>16</v>
       </c>
       <c r="B105" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C105" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="D105" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E105" s="1">
         <v>44879</v>
       </c>
       <c r="F105" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G105" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H105" s="2"/>
       <c r="I105" s="2">
@@ -8720,7 +8717,7 @@
         <v>0</v>
       </c>
       <c r="P105" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q105" s="2">
         <v>0</v>
@@ -8755,22 +8752,22 @@
         <v>16</v>
       </c>
       <c r="B106" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C106" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="D106" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E106" s="1">
         <v>44879</v>
       </c>
       <c r="F106" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G106" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H106" s="2"/>
       <c r="I106" s="2">
@@ -8780,10 +8777,10 @@
         <v>3</v>
       </c>
       <c r="K106" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L106" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M106" s="2">
         <v>0</v>
@@ -8810,7 +8807,7 @@
         <v>0</v>
       </c>
       <c r="U106" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V106" s="2">
         <v>0</v>
@@ -8830,13 +8827,13 @@
         <v>17</v>
       </c>
       <c r="B107" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C107" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="D107" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E107" s="1">
         <v>44893</v>
@@ -8905,13 +8902,13 @@
         <v>17</v>
       </c>
       <c r="B108" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C108" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="D108" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E108" s="1">
         <v>44893</v>
@@ -8980,22 +8977,22 @@
         <v>18</v>
       </c>
       <c r="B109" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C109" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D109" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E109" s="1">
         <v>44887</v>
       </c>
       <c r="F109" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G109" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H109" s="2"/>
       <c r="I109" s="2">
@@ -9044,7 +9041,7 @@
         <v>0</v>
       </c>
       <c r="X109" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y109" s="2">
         <v>0</v>
@@ -9055,22 +9052,22 @@
         <v>18</v>
       </c>
       <c r="B110" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C110" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="D110" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E110" s="1">
         <v>44887</v>
       </c>
       <c r="F110" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G110" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H110" s="2"/>
       <c r="I110" s="2">
@@ -9104,7 +9101,7 @@
         <v>0</v>
       </c>
       <c r="S110" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T110" s="2">
         <v>0</v>
@@ -9119,7 +9116,7 @@
         <v>0</v>
       </c>
       <c r="X110" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y110" s="2">
         <v>0</v>
@@ -9130,13 +9127,13 @@
         <v>18</v>
       </c>
       <c r="B111" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C111" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="D111" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E111" s="1">
         <v>44887</v>
@@ -9179,7 +9176,7 @@
         <v>0</v>
       </c>
       <c r="S111" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T111" s="2">
         <v>0</v>
@@ -9205,13 +9202,13 @@
         <v>18</v>
       </c>
       <c r="B112" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C112" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="D112" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E112" s="1">
         <v>44887</v>
@@ -9280,13 +9277,13 @@
         <v>18</v>
       </c>
       <c r="B113" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C113" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="D113" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E113" s="1">
         <v>44887</v>
@@ -9355,13 +9352,13 @@
         <v>19</v>
       </c>
       <c r="B114" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C114" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D114" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E114" s="1">
         <v>44896</v>
@@ -9430,13 +9427,13 @@
         <v>20</v>
       </c>
       <c r="B115" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C115" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="D115" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E115" s="1">
         <v>44714</v>
@@ -9507,13 +9504,13 @@
         <v>20</v>
       </c>
       <c r="B116" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C116" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="D116" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E116" s="1">
         <v>44714</v>

</xml_diff>

<commit_message>
updated everything to final
</commit_message>
<xml_diff>
--- a/datasets/lab_detail.xlsx
+++ b/datasets/lab_detail.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="267">
   <si>
     <t>sampleid</t>
   </si>
@@ -84,342 +84,342 @@
     <t>p-fluorofentanyl</t>
   </si>
   <si>
+    <t>dimethyl sulfone (methylsulfonylmethane MSM)</t>
+  </si>
+  <si>
+    <t>phenethyl 4-ANPP</t>
+  </si>
+  <si>
+    <t>fentanyl</t>
+  </si>
+  <si>
+    <t>4-ANPP</t>
+  </si>
+  <si>
     <t>xylazine</t>
   </si>
   <si>
+    <t>despropionyl p-fluorofentanyl</t>
+  </si>
+  <si>
+    <t>3,4-MDMA</t>
+  </si>
+  <si>
+    <t>3,4-methylenedioxy-N-benzylcathinone (BMDP)</t>
+  </si>
+  <si>
+    <t>3,4-MDMA</t>
+  </si>
+  <si>
+    <t>benzoylecgonine (BZ)</t>
+  </si>
+  <si>
+    <t>tropacocaine</t>
+  </si>
+  <si>
+    <t>norcocaine</t>
+  </si>
+  <si>
+    <t>phenacetin</t>
+  </si>
+  <si>
+    <t>cocaine</t>
+  </si>
+  <si>
+    <t>levamisole</t>
+  </si>
+  <si>
+    <t>methyl ecgonidine (MED)</t>
+  </si>
+  <si>
+    <t>p-fluoro phenethyl 4-ANPP</t>
+  </si>
+  <si>
+    <t>despropionyl p-fluorofentanyl</t>
+  </si>
+  <si>
+    <t>tramadol</t>
+  </si>
+  <si>
+    <t>methamphetamine</t>
+  </si>
+  <si>
     <t>fentanyl</t>
   </si>
   <si>
+    <t>4-ANPP</t>
+  </si>
+  <si>
+    <t>non-specific sugars</t>
+  </si>
+  <si>
+    <t>caffeine</t>
+  </si>
+  <si>
+    <t>methamphetamine</t>
+  </si>
+  <si>
+    <t>eutylone</t>
+  </si>
+  <si>
+    <t>non-specific sugars</t>
+  </si>
+  <si>
+    <t>6-monoacetylmorphine (6-MAM)</t>
+  </si>
+  <si>
+    <t>acetylcodeine</t>
+  </si>
+  <si>
+    <t>urea</t>
+  </si>
+  <si>
     <t>phenethyl 4-ANPP</t>
   </si>
   <si>
+    <t>xylazine</t>
+  </si>
+  <si>
     <t>4-ANPP</t>
   </si>
   <si>
+    <t>heroin</t>
+  </si>
+  <si>
+    <t>fentanyl</t>
+  </si>
+  <si>
+    <t>cocaine</t>
+  </si>
+  <si>
+    <t>4-ANPP</t>
+  </si>
+  <si>
+    <t>caffeine</t>
+  </si>
+  <si>
+    <t>fentanyl</t>
+  </si>
+  <si>
+    <t>N-phenylpropanamide</t>
+  </si>
+  <si>
+    <t>4-ANPP</t>
+  </si>
+  <si>
+    <t>xylazine</t>
+  </si>
+  <si>
+    <t>6-monoacetylmorphine (6-MAM)</t>
+  </si>
+  <si>
+    <t>acetaminophen</t>
+  </si>
+  <si>
+    <t>p-fluorofentanyl</t>
+  </si>
+  <si>
+    <t>tramadol</t>
+  </si>
+  <si>
+    <t>dimethyl sulfone (methylsulfonylmethane MSM)</t>
+  </si>
+  <si>
+    <t>1,3-Diacetin</t>
+  </si>
+  <si>
+    <t>acetylcodeine</t>
+  </si>
+  <si>
+    <t>heroin</t>
+  </si>
+  <si>
+    <t>N-ethyl-4-ANPP</t>
+  </si>
+  <si>
+    <t>fentanyl</t>
+  </si>
+  <si>
+    <t>phenethyl 4-ANPP</t>
+  </si>
+  <si>
+    <t>lidocaine</t>
+  </si>
+  <si>
+    <t>4-ANPP</t>
+  </si>
+  <si>
+    <t>methamphetamine</t>
+  </si>
+  <si>
+    <t>gabapentin</t>
+  </si>
+  <si>
+    <t>quinine</t>
+  </si>
+  <si>
+    <t>N-piperidinyl etonitazene</t>
+  </si>
+  <si>
+    <t>phenethyl 4-ANPP</t>
+  </si>
+  <si>
+    <t>1,3-Diacetin</t>
+  </si>
+  <si>
+    <t>metonitazene</t>
+  </si>
+  <si>
+    <t>inositol</t>
+  </si>
+  <si>
+    <t>methadone</t>
+  </si>
+  <si>
+    <t>non-specific sugars</t>
+  </si>
+  <si>
+    <t>heroin</t>
+  </si>
+  <si>
+    <t>acetylcodeine</t>
+  </si>
+  <si>
+    <t>diphenhydramine</t>
+  </si>
+  <si>
+    <t>fentanyl</t>
+  </si>
+  <si>
+    <t>dimethyl sulfone (methylsulfonylmethane MSM)</t>
+  </si>
+  <si>
+    <t>fentanyl</t>
+  </si>
+  <si>
+    <t>non-specific organic acids</t>
+  </si>
+  <si>
+    <t>methamphetamine</t>
+  </si>
+  <si>
+    <t>4-ANPP</t>
+  </si>
+  <si>
+    <t>heroin</t>
+  </si>
+  <si>
+    <t>xylazine</t>
+  </si>
+  <si>
+    <t>procaine</t>
+  </si>
+  <si>
+    <t>cocaine</t>
+  </si>
+  <si>
+    <t>fentanyl</t>
+  </si>
+  <si>
     <t>despropionyl p-fluorofentanyl</t>
   </si>
   <si>
-    <t>dimethyl sulfone (methylsulfonylmethane MSM)</t>
-  </si>
-  <si>
-    <t>3,4-MDMA</t>
-  </si>
-  <si>
-    <t>3,4-methylenedioxy-N-benzylcathinone (BMDP)</t>
-  </si>
-  <si>
-    <t>3,4-MDMA</t>
+    <t>phenethylbromide</t>
+  </si>
+  <si>
+    <t>p-fluorofentanyl</t>
+  </si>
+  <si>
+    <t>xylazine</t>
+  </si>
+  <si>
+    <t>p-fluoro phenethyl 4-ANPP</t>
+  </si>
+  <si>
+    <t>phenethyl chloride</t>
+  </si>
+  <si>
+    <t>nicotine</t>
+  </si>
+  <si>
+    <t>1,3-Diacetin</t>
+  </si>
+  <si>
+    <t>menthol</t>
+  </si>
+  <si>
+    <t>1,3-Diacetin</t>
+  </si>
+  <si>
+    <t>caffeine</t>
+  </si>
+  <si>
+    <t>fentanyl</t>
+  </si>
+  <si>
+    <t>diphenhydramine</t>
+  </si>
+  <si>
+    <t>p-fluorofentanyl</t>
+  </si>
+  <si>
+    <t>N-ethyl-4-ANPP</t>
+  </si>
+  <si>
+    <t>4-ANPP</t>
+  </si>
+  <si>
+    <t>1-phenethyl-4-propionyloxypiperidine</t>
+  </si>
+  <si>
+    <t>quinine</t>
+  </si>
+  <si>
+    <t>acetaminophen</t>
+  </si>
+  <si>
+    <t>fentanyl</t>
+  </si>
+  <si>
+    <t>N-phenylpropanamide</t>
+  </si>
+  <si>
+    <t>tramadol</t>
+  </si>
+  <si>
+    <t>N-ethyl-4-ANPP</t>
+  </si>
+  <si>
+    <t>methamphetamine</t>
+  </si>
+  <si>
+    <t>4-ANPP</t>
+  </si>
+  <si>
+    <t>methamphetamine</t>
+  </si>
+  <si>
+    <t>fentanyl</t>
   </si>
   <si>
     <t>tropacocaine</t>
   </si>
   <si>
+    <t>cocaine</t>
+  </si>
+  <si>
     <t>levamisole</t>
   </si>
   <si>
-    <t>cocaine</t>
-  </si>
-  <si>
     <t>methyl ecgonidine (MED)</t>
   </si>
   <si>
-    <t>norcocaine</t>
-  </si>
-  <si>
-    <t>benzoylecgonine (BZ)</t>
-  </si>
-  <si>
-    <t>phenacetin</t>
-  </si>
-  <si>
-    <t>non-specific sugars</t>
+    <t>ecgonine methylester (EME)</t>
   </si>
   <si>
     <t>methamphetamine</t>
   </si>
   <si>
-    <t>4-ANPP</t>
-  </si>
-  <si>
-    <t>tramadol</t>
-  </si>
-  <si>
-    <t>despropionyl p-fluorofentanyl</t>
-  </si>
-  <si>
-    <t>p-fluoro phenethyl 4-ANPP</t>
-  </si>
-  <si>
-    <t>fentanyl</t>
-  </si>
-  <si>
-    <t>methamphetamine</t>
-  </si>
-  <si>
-    <t>caffeine</t>
-  </si>
-  <si>
-    <t>eutylone</t>
-  </si>
-  <si>
-    <t>xylazine</t>
-  </si>
-  <si>
-    <t>urea</t>
-  </si>
-  <si>
-    <t>4-ANPP</t>
-  </si>
-  <si>
-    <t>heroin</t>
-  </si>
-  <si>
-    <t>fentanyl</t>
-  </si>
-  <si>
-    <t>6-monoacetylmorphine (6-MAM)</t>
-  </si>
-  <si>
-    <t>non-specific sugars</t>
-  </si>
-  <si>
-    <t>acetylcodeine</t>
-  </si>
-  <si>
-    <t>phenethyl 4-ANPP</t>
-  </si>
-  <si>
-    <t>caffeine</t>
-  </si>
-  <si>
-    <t>cocaine</t>
-  </si>
-  <si>
-    <t>fentanyl</t>
-  </si>
-  <si>
-    <t>4-ANPP</t>
-  </si>
-  <si>
-    <t>fentanyl</t>
-  </si>
-  <si>
-    <t>N-phenylpropanamide</t>
-  </si>
-  <si>
-    <t>N-ethyl-4-ANPP</t>
-  </si>
-  <si>
-    <t>acetaminophen</t>
-  </si>
-  <si>
-    <t>phenethyl 4-ANPP</t>
-  </si>
-  <si>
-    <t>4-ANPP</t>
-  </si>
-  <si>
-    <t>xylazine</t>
-  </si>
-  <si>
-    <t>1,3-Diacetin</t>
-  </si>
-  <si>
-    <t>lidocaine</t>
-  </si>
-  <si>
-    <t>p-fluorofentanyl</t>
-  </si>
-  <si>
-    <t>heroin</t>
-  </si>
-  <si>
-    <t>acetylcodeine</t>
-  </si>
-  <si>
-    <t>dimethyl sulfone (methylsulfonylmethane MSM)</t>
-  </si>
-  <si>
-    <t>tramadol</t>
-  </si>
-  <si>
-    <t>6-monoacetylmorphine (6-MAM)</t>
-  </si>
-  <si>
-    <t>acetylcodeine</t>
-  </si>
-  <si>
-    <t>1,3-Diacetin</t>
-  </si>
-  <si>
-    <t>fentanyl</t>
-  </si>
-  <si>
-    <t>non-specific sugars</t>
-  </si>
-  <si>
-    <t>diphenhydramine</t>
-  </si>
-  <si>
-    <t>phenethyl 4-ANPP</t>
-  </si>
-  <si>
-    <t>heroin</t>
-  </si>
-  <si>
-    <t>methamphetamine</t>
-  </si>
-  <si>
-    <t>inositol</t>
-  </si>
-  <si>
-    <t>methadone</t>
-  </si>
-  <si>
-    <t>N-piperidinyl etonitazene</t>
-  </si>
-  <si>
-    <t>quinine</t>
-  </si>
-  <si>
-    <t>4-ANPP</t>
-  </si>
-  <si>
-    <t>metonitazene</t>
-  </si>
-  <si>
-    <t>gabapentin</t>
-  </si>
-  <si>
-    <t>dimethyl sulfone (methylsulfonylmethane MSM)</t>
-  </si>
-  <si>
-    <t>non-specific organic acids</t>
-  </si>
-  <si>
-    <t>fentanyl</t>
-  </si>
-  <si>
-    <t>methamphetamine</t>
-  </si>
-  <si>
-    <t>cocaine</t>
-  </si>
-  <si>
-    <t>xylazine</t>
-  </si>
-  <si>
-    <t>heroin</t>
-  </si>
-  <si>
-    <t>procaine</t>
-  </si>
-  <si>
-    <t>fentanyl</t>
-  </si>
-  <si>
-    <t>4-ANPP</t>
-  </si>
-  <si>
-    <t>xylazine</t>
-  </si>
-  <si>
-    <t>despropionyl p-fluorofentanyl</t>
-  </si>
-  <si>
-    <t>phenethylbromide</t>
-  </si>
-  <si>
-    <t>p-fluorofentanyl</t>
-  </si>
-  <si>
-    <t>menthol</t>
-  </si>
-  <si>
-    <t>phenethyl chloride</t>
-  </si>
-  <si>
-    <t>nicotine</t>
-  </si>
-  <si>
-    <t>p-fluoro phenethyl 4-ANPP</t>
-  </si>
-  <si>
-    <t>1,3-Diacetin</t>
-  </si>
-  <si>
-    <t>diphenhydramine</t>
-  </si>
-  <si>
-    <t>N-ethyl-4-ANPP</t>
-  </si>
-  <si>
-    <t>1,3-Diacetin</t>
-  </si>
-  <si>
-    <t>fentanyl</t>
-  </si>
-  <si>
-    <t>p-fluorofentanyl</t>
-  </si>
-  <si>
-    <t>quinine</t>
-  </si>
-  <si>
-    <t>4-ANPP</t>
-  </si>
-  <si>
-    <t>1-phenethyl-4-propionyloxypiperidine</t>
-  </si>
-  <si>
-    <t>caffeine</t>
-  </si>
-  <si>
-    <t>N-phenylpropanamide</t>
-  </si>
-  <si>
-    <t>N-ethyl-4-ANPP</t>
-  </si>
-  <si>
-    <t>acetaminophen</t>
-  </si>
-  <si>
-    <t>tramadol</t>
-  </si>
-  <si>
-    <t>4-ANPP</t>
-  </si>
-  <si>
-    <t>methamphetamine</t>
-  </si>
-  <si>
-    <t>fentanyl</t>
-  </si>
-  <si>
-    <t>methamphetamine</t>
-  </si>
-  <si>
-    <t>fentanyl</t>
-  </si>
-  <si>
-    <t>tropacocaine</t>
-  </si>
-  <si>
-    <t>levamisole</t>
-  </si>
-  <si>
-    <t>cocaine</t>
-  </si>
-  <si>
-    <t>ecgonine methylester (EME)</t>
-  </si>
-  <si>
-    <t>methyl ecgonidine (MED)</t>
-  </si>
-  <si>
-    <t>methamphetamine</t>
-  </si>
-  <si>
     <t>no compounds of interest detected</t>
   </si>
   <si>
@@ -474,6 +474,15 @@
     <t/>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t>trace</t>
   </si>
   <si>
@@ -498,6 +507,9 @@
     <t/>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>trace</t>
   </si>
   <si>
@@ -534,6 +546,12 @@
     <t/>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t>trace</t>
   </si>
   <si>
@@ -543,18 +561,57 @@
     <t/>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t>trace</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
+    <t>trace</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
     <t/>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t>trace</t>
   </si>
   <si>
@@ -567,6 +624,9 @@
     <t/>
   </si>
   <si>
+    <t>trace</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
@@ -582,6 +642,9 @@
     <t/>
   </si>
   <si>
+    <t>trace</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
@@ -594,12 +657,18 @@
     <t/>
   </si>
   <si>
+    <t>trace</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
     <t/>
   </si>
   <si>
+    <t>trace</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
@@ -609,102 +678,18 @@
     <t/>
   </si>
   <si>
+    <t>trace</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>trace</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
-    <t>trace</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>trace</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>trace</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>trace</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>trace</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>trace</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>trace</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>trace</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>trace</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>trace</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
     <t>method</t>
   </si>
   <si>
@@ -757,6 +742,15 @@
   </si>
   <si>
     <t>GCMS</t>
+  </si>
+  <si>
+    <t>Derivatized GCMS</t>
+  </si>
+  <si>
+    <t>GCMS</t>
+  </si>
+  <si>
+    <t>Derivatized GCMS</t>
   </si>
   <si>
     <t>date_complete</t>
@@ -881,70 +875,70 @@
         <v>136</v>
       </c>
       <c r="D1" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="E1" t="s">
+        <v>246</v>
+      </c>
+      <c r="F1" t="s">
+        <v>247</v>
+      </c>
+      <c r="G1" t="s">
         <v>248</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>249</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>250</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>251</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>252</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>253</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>254</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>255</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>256</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>257</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>258</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>259</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>260</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>261</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>262</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>263</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>264</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>265</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>266</v>
-      </c>
-      <c r="X1" t="s">
-        <v>267</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="2">
@@ -958,7 +952,7 @@
         <v>137</v>
       </c>
       <c r="D2" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="E2" s="1">
         <v>44603</v>
@@ -1033,7 +1027,7 @@
         <v>138</v>
       </c>
       <c r="D3" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="E3" s="1">
         <v>44603</v>
@@ -1058,10 +1052,10 @@
         <v>0</v>
       </c>
       <c r="M3" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N3" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O3" s="2">
         <v>0</v>
@@ -1108,7 +1102,7 @@
         <v>139</v>
       </c>
       <c r="D4" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="E4" s="1">
         <v>44603</v>
@@ -1127,10 +1121,10 @@
         <v>7</v>
       </c>
       <c r="K4" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L4" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M4" s="2">
         <v>0</v>
@@ -1183,7 +1177,7 @@
         <v>140</v>
       </c>
       <c r="D5" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="E5" s="1">
         <v>44603</v>
@@ -1202,10 +1196,10 @@
         <v>7</v>
       </c>
       <c r="K5" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L5" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M5" s="2">
         <v>0</v>
@@ -1258,7 +1252,7 @@
         <v>141</v>
       </c>
       <c r="D6" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="E6" s="1">
         <v>44603</v>
@@ -1333,7 +1327,7 @@
         <v>142</v>
       </c>
       <c r="D7" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="E7" s="1">
         <v>44603</v>
@@ -1358,10 +1352,10 @@
         <v>0</v>
       </c>
       <c r="M7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O7" s="2">
         <v>0</v>
@@ -1408,7 +1402,7 @@
         <v>143</v>
       </c>
       <c r="D8" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="E8" s="1">
         <v>44603</v>
@@ -1483,7 +1477,7 @@
         <v>144</v>
       </c>
       <c r="D9" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="E9" s="1">
         <v>44777</v>
@@ -1558,7 +1552,7 @@
         <v>145</v>
       </c>
       <c r="D10" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="E10" s="1">
         <v>44777</v>
@@ -1633,7 +1627,7 @@
         <v>146</v>
       </c>
       <c r="D11" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="E11" s="1">
         <v>44758</v>
@@ -1708,7 +1702,7 @@
         <v>147</v>
       </c>
       <c r="D12" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E12" s="1">
         <v>44714</v>
@@ -1783,7 +1777,7 @@
         <v>147</v>
       </c>
       <c r="D13" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="E13" s="1">
         <v>44714</v>
@@ -1826,7 +1820,7 @@
         <v>0</v>
       </c>
       <c r="S13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T13" s="2">
         <v>0</v>
@@ -1841,7 +1835,7 @@
         <v>0</v>
       </c>
       <c r="X13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y13" s="2">
         <v>0</v>
@@ -1855,19 +1849,19 @@
         <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D14" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="E14" s="1">
         <v>44714</v>
       </c>
       <c r="F14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2">
@@ -1916,7 +1910,7 @@
         <v>0</v>
       </c>
       <c r="X14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y14" s="2">
         <v>0</v>
@@ -1930,10 +1924,10 @@
         <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D15" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E15" s="1">
         <v>44714</v>
@@ -1991,7 +1985,7 @@
         <v>0</v>
       </c>
       <c r="X15" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y15" s="2">
         <v>0</v>
@@ -2005,19 +1999,19 @@
         <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D16" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E16" s="1">
         <v>44714</v>
       </c>
       <c r="F16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2">
@@ -2066,7 +2060,7 @@
         <v>0</v>
       </c>
       <c r="X16" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y16" s="2">
         <v>0</v>
@@ -2083,7 +2077,7 @@
         <v>149</v>
       </c>
       <c r="D17" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E17" s="1">
         <v>44714</v>
@@ -2126,7 +2120,7 @@
         <v>0</v>
       </c>
       <c r="S17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T17" s="2">
         <v>0</v>
@@ -2141,7 +2135,7 @@
         <v>0</v>
       </c>
       <c r="X17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y17" s="2">
         <v>0</v>
@@ -2158,7 +2152,7 @@
         <v>149</v>
       </c>
       <c r="D18" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E18" s="1">
         <v>44714</v>
@@ -2216,7 +2210,7 @@
         <v>0</v>
       </c>
       <c r="X18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y18" s="2">
         <v>0</v>
@@ -2230,19 +2224,19 @@
         <v>39</v>
       </c>
       <c r="C19" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D19" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E19" s="1">
         <v>44759</v>
       </c>
       <c r="F19" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2">
@@ -2305,19 +2299,19 @@
         <v>40</v>
       </c>
       <c r="C20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D20" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E20" s="1">
         <v>44759</v>
       </c>
       <c r="F20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2">
@@ -2342,7 +2336,7 @@
         <v>0</v>
       </c>
       <c r="P20" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q20" s="2">
         <v>0</v>
@@ -2380,19 +2374,19 @@
         <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D21" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E21" s="1">
         <v>44759</v>
       </c>
       <c r="F21" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2">
@@ -2432,7 +2426,7 @@
         <v>0</v>
       </c>
       <c r="U21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V21" s="2">
         <v>0</v>
@@ -2455,10 +2449,10 @@
         <v>42</v>
       </c>
       <c r="C22" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D22" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E22" s="1">
         <v>44759</v>
@@ -2492,7 +2486,7 @@
         <v>0</v>
       </c>
       <c r="P22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q22" s="2">
         <v>0</v>
@@ -2507,7 +2501,7 @@
         <v>0</v>
       </c>
       <c r="U22" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V22" s="2">
         <v>0</v>
@@ -2530,10 +2524,10 @@
         <v>43</v>
       </c>
       <c r="C23" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D23" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E23" s="1">
         <v>44759</v>
@@ -2552,10 +2546,10 @@
         <v>4</v>
       </c>
       <c r="K23" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L23" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M23" s="2">
         <v>0</v>
@@ -2605,19 +2599,19 @@
         <v>44</v>
       </c>
       <c r="C24" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D24" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E24" s="1">
         <v>44759</v>
       </c>
       <c r="F24" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2">
@@ -2680,7 +2674,7 @@
         <v>45</v>
       </c>
       <c r="C25" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D25" t="s">
         <v>233</v>
@@ -2702,10 +2696,10 @@
         <v>4</v>
       </c>
       <c r="K25" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L25" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M25" s="2">
         <v>0</v>
@@ -2755,19 +2749,19 @@
         <v>46</v>
       </c>
       <c r="C26" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D26" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E26" s="1">
         <v>44721</v>
       </c>
       <c r="F26" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G26" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H26" s="2"/>
       <c r="I26" s="2">
@@ -2792,10 +2786,10 @@
         <v>0</v>
       </c>
       <c r="P26" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q26" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R26" s="2">
         <v>0</v>
@@ -2830,19 +2824,19 @@
         <v>47</v>
       </c>
       <c r="C27" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D27" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E27" s="1">
         <v>44721</v>
       </c>
       <c r="F27" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G27" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H27" s="2"/>
       <c r="I27" s="2">
@@ -2867,10 +2861,10 @@
         <v>0</v>
       </c>
       <c r="P27" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q27" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R27" s="2">
         <v>0</v>
@@ -2905,10 +2899,10 @@
         <v>48</v>
       </c>
       <c r="C28" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D28" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E28" s="1">
         <v>44721</v>
@@ -2980,10 +2974,10 @@
         <v>49</v>
       </c>
       <c r="C29" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D29" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="E29" s="1">
         <v>44707</v>
@@ -3008,10 +3002,10 @@
         <v>0</v>
       </c>
       <c r="M29" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N29" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O29" s="2">
         <v>0</v>
@@ -3055,10 +3049,10 @@
         <v>50</v>
       </c>
       <c r="C30" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D30" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="E30" s="1">
         <v>44707</v>
@@ -3130,19 +3124,19 @@
         <v>51</v>
       </c>
       <c r="C31" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D31" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E31" s="1">
         <v>44707</v>
       </c>
       <c r="F31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G31" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H31" s="2"/>
       <c r="I31" s="2">
@@ -3205,19 +3199,19 @@
         <v>52</v>
       </c>
       <c r="C32" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D32" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="E32" s="1">
         <v>44707</v>
       </c>
       <c r="F32" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G32" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H32" s="2"/>
       <c r="I32" s="2">
@@ -3280,19 +3274,19 @@
         <v>53</v>
       </c>
       <c r="C33" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D33" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="E33" s="1">
         <v>44707</v>
       </c>
       <c r="F33" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G33" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H33" s="2"/>
       <c r="I33" s="2">
@@ -3302,10 +3296,10 @@
         <v>5</v>
       </c>
       <c r="K33" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L33" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M33" s="2">
         <v>0</v>
@@ -3355,19 +3349,19 @@
         <v>54</v>
       </c>
       <c r="C34" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D34" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="E34" s="1">
         <v>44707</v>
       </c>
       <c r="F34" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G34" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H34" s="2"/>
       <c r="I34" s="2">
@@ -3383,10 +3377,10 @@
         <v>0</v>
       </c>
       <c r="M34" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N34" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O34" s="2">
         <v>0</v>
@@ -3430,19 +3424,19 @@
         <v>55</v>
       </c>
       <c r="C35" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D35" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="E35" s="1">
         <v>44707</v>
       </c>
       <c r="F35" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G35" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H35" s="2"/>
       <c r="I35" s="2">
@@ -3505,10 +3499,10 @@
         <v>56</v>
       </c>
       <c r="C36" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D36" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E36" s="1">
         <v>44707</v>
@@ -3580,7 +3574,7 @@
         <v>57</v>
       </c>
       <c r="C37" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D37" t="s">
         <v>238</v>
@@ -3589,10 +3583,10 @@
         <v>44707</v>
       </c>
       <c r="F37" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G37" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H37" s="2"/>
       <c r="I37" s="2">
@@ -3602,10 +3596,10 @@
         <v>5</v>
       </c>
       <c r="K37" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L37" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M37" s="2">
         <v>0</v>
@@ -3655,19 +3649,19 @@
         <v>58</v>
       </c>
       <c r="C38" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E38" s="1">
         <v>44789</v>
       </c>
       <c r="F38" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G38" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H38" s="2"/>
       <c r="I38" s="2">
@@ -3695,7 +3689,7 @@
         <v>0</v>
       </c>
       <c r="Q38" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R38" s="2">
         <v>0</v>
@@ -3730,10 +3724,10 @@
         <v>59</v>
       </c>
       <c r="C39" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D39" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E39" s="1">
         <v>44789</v>
@@ -3805,10 +3799,10 @@
         <v>60</v>
       </c>
       <c r="C40" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D40" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E40" s="1">
         <v>44789</v>
@@ -3827,10 +3821,10 @@
         <v>2</v>
       </c>
       <c r="K40" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L40" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M40" s="2">
         <v>0</v>
@@ -3845,7 +3839,7 @@
         <v>0</v>
       </c>
       <c r="Q40" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R40" s="2">
         <v>0</v>
@@ -3880,19 +3874,19 @@
         <v>61</v>
       </c>
       <c r="C41" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D41" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E41" s="1">
         <v>44789</v>
       </c>
       <c r="F41" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G41" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H41" s="2"/>
       <c r="I41" s="2">
@@ -3902,10 +3896,10 @@
         <v>2</v>
       </c>
       <c r="K41" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L41" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M41" s="2">
         <v>0</v>
@@ -3955,19 +3949,19 @@
         <v>62</v>
       </c>
       <c r="C42" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D42" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E42" s="1">
         <v>44818</v>
       </c>
       <c r="F42" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G42" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H42" s="2"/>
       <c r="I42" s="2">
@@ -3977,10 +3971,10 @@
         <v>3</v>
       </c>
       <c r="K42" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L42" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M42" s="2">
         <v>0</v>
@@ -4030,19 +4024,19 @@
         <v>63</v>
       </c>
       <c r="C43" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D43" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E43" s="1">
         <v>44818</v>
       </c>
       <c r="F43" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G43" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H43" s="2"/>
       <c r="I43" s="2">
@@ -4105,19 +4099,19 @@
         <v>64</v>
       </c>
       <c r="C44" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D44" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E44" s="1">
         <v>44818</v>
       </c>
       <c r="F44" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G44" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H44" s="2"/>
       <c r="I44" s="2">
@@ -4133,10 +4127,10 @@
         <v>0</v>
       </c>
       <c r="M44" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N44" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O44" s="2">
         <v>0</v>
@@ -4180,10 +4174,10 @@
         <v>65</v>
       </c>
       <c r="C45" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D45" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E45" s="1">
         <v>44818</v>
@@ -4255,10 +4249,10 @@
         <v>66</v>
       </c>
       <c r="C46" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D46" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E46" s="1">
         <v>44818</v>
@@ -4330,19 +4324,19 @@
         <v>67</v>
       </c>
       <c r="C47" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D47" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E47" s="1">
         <v>44818</v>
       </c>
       <c r="F47" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G47" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H47" s="2"/>
       <c r="I47" s="2">
@@ -4405,19 +4399,19 @@
         <v>68</v>
       </c>
       <c r="C48" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D48" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E48" s="1">
         <v>44818</v>
       </c>
       <c r="F48" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G48" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H48" s="2"/>
       <c r="I48" s="2">
@@ -4433,10 +4427,10 @@
         <v>0</v>
       </c>
       <c r="M48" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N48" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O48" s="2">
         <v>0</v>
@@ -4457,7 +4451,7 @@
         <v>0</v>
       </c>
       <c r="U48" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V48" s="2">
         <v>0</v>
@@ -4480,10 +4474,10 @@
         <v>69</v>
       </c>
       <c r="C49" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D49" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E49" s="1">
         <v>44818</v>
@@ -4555,10 +4549,10 @@
         <v>70</v>
       </c>
       <c r="C50" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D50" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E50" s="1">
         <v>44818</v>
@@ -4630,10 +4624,10 @@
         <v>71</v>
       </c>
       <c r="C51" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D51" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E51" s="1">
         <v>44818</v>
@@ -4705,10 +4699,10 @@
         <v>72</v>
       </c>
       <c r="C52" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D52" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E52" s="1">
         <v>44818</v>
@@ -4780,10 +4774,10 @@
         <v>73</v>
       </c>
       <c r="C53" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D53" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E53" s="1">
         <v>44818</v>
@@ -4855,19 +4849,19 @@
         <v>74</v>
       </c>
       <c r="C54" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D54" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E54" s="1">
         <v>44818</v>
       </c>
       <c r="F54" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G54" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H54" s="2"/>
       <c r="I54" s="2">
@@ -4877,10 +4871,10 @@
         <v>3</v>
       </c>
       <c r="K54" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L54" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M54" s="2">
         <v>0</v>
@@ -4930,10 +4924,10 @@
         <v>75</v>
       </c>
       <c r="C55" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D55" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E55" s="1">
         <v>44818</v>
@@ -4982,7 +4976,7 @@
         <v>0</v>
       </c>
       <c r="U55" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V55" s="2">
         <v>0</v>
@@ -5005,10 +4999,10 @@
         <v>76</v>
       </c>
       <c r="C56" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D56" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E56" s="1">
         <v>44818</v>
@@ -5080,19 +5074,19 @@
         <v>77</v>
       </c>
       <c r="C57" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D57" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E57" s="1">
         <v>44771</v>
       </c>
       <c r="F57" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G57" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H57" s="2"/>
       <c r="I57" s="2">
@@ -5155,19 +5149,19 @@
         <v>78</v>
       </c>
       <c r="C58" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D58" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E58" s="1">
         <v>44771</v>
       </c>
       <c r="F58" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G58" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H58" s="2"/>
       <c r="I58" s="2">
@@ -5192,7 +5186,7 @@
         <v>0</v>
       </c>
       <c r="P58" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q58" s="2">
         <v>0</v>
@@ -5230,10 +5224,10 @@
         <v>79</v>
       </c>
       <c r="C59" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D59" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E59" s="1">
         <v>44771</v>
@@ -5252,10 +5246,10 @@
         <v>11</v>
       </c>
       <c r="K59" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L59" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M59" s="2">
         <v>0</v>
@@ -5273,7 +5267,7 @@
         <v>0</v>
       </c>
       <c r="R59" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S59" s="2">
         <v>0</v>
@@ -5305,10 +5299,10 @@
         <v>80</v>
       </c>
       <c r="C60" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D60" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E60" s="1">
         <v>44771</v>
@@ -5380,19 +5374,19 @@
         <v>81</v>
       </c>
       <c r="C61" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D61" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E61" s="1">
         <v>44771</v>
       </c>
       <c r="F61" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G61" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H61" s="2"/>
       <c r="I61" s="2">
@@ -5455,10 +5449,10 @@
         <v>82</v>
       </c>
       <c r="C62" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D62" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E62" s="1">
         <v>44771</v>
@@ -5530,10 +5524,10 @@
         <v>83</v>
       </c>
       <c r="C63" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D63" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E63" s="1">
         <v>44771</v>
@@ -5605,19 +5599,19 @@
         <v>84</v>
       </c>
       <c r="C64" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D64" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E64" s="1">
         <v>44771</v>
       </c>
       <c r="F64" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G64" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H64" s="2"/>
       <c r="I64" s="2">
@@ -5642,7 +5636,7 @@
         <v>0</v>
       </c>
       <c r="P64" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q64" s="2">
         <v>0</v>
@@ -5680,10 +5674,10 @@
         <v>85</v>
       </c>
       <c r="C65" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D65" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E65" s="1">
         <v>44771</v>
@@ -5755,10 +5749,10 @@
         <v>86</v>
       </c>
       <c r="C66" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D66" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E66" s="1">
         <v>44771</v>
@@ -5830,7 +5824,7 @@
         <v>87</v>
       </c>
       <c r="C67" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D67" t="s">
         <v>243</v>
@@ -5905,7 +5899,7 @@
         <v>88</v>
       </c>
       <c r="C68" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D68" t="s">
         <v>244</v>
@@ -5980,19 +5974,19 @@
         <v>89</v>
       </c>
       <c r="C69" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D69" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E69" s="1">
         <v>44771</v>
       </c>
       <c r="F69" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G69" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H69" s="2"/>
       <c r="I69" s="2">
@@ -6055,19 +6049,19 @@
         <v>90</v>
       </c>
       <c r="C70" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D70" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E70" s="1">
         <v>44771</v>
       </c>
       <c r="F70" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G70" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H70" s="2"/>
       <c r="I70" s="2">
@@ -6130,10 +6124,10 @@
         <v>91</v>
       </c>
       <c r="C71" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D71" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E71" s="1">
         <v>44771</v>
@@ -6152,10 +6146,10 @@
         <v>11</v>
       </c>
       <c r="K71" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L71" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M71" s="2">
         <v>0</v>
@@ -6173,7 +6167,7 @@
         <v>0</v>
       </c>
       <c r="R71" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S71" s="2">
         <v>0</v>
@@ -6205,10 +6199,10 @@
         <v>92</v>
       </c>
       <c r="C72" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D72" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E72" s="1">
         <v>44845</v>
@@ -6280,10 +6274,10 @@
         <v>93</v>
       </c>
       <c r="C73" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D73" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E73" s="1">
         <v>44845</v>
@@ -6302,10 +6296,10 @@
         <v>2</v>
       </c>
       <c r="K73" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L73" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M73" s="2">
         <v>0</v>
@@ -6355,10 +6349,10 @@
         <v>94</v>
       </c>
       <c r="C74" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D74" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E74" s="1">
         <v>44845</v>
@@ -6377,10 +6371,10 @@
         <v>2</v>
       </c>
       <c r="K74" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L74" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M74" s="2">
         <v>0</v>
@@ -6430,10 +6424,10 @@
         <v>95</v>
       </c>
       <c r="C75" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D75" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E75" s="1">
         <v>44803</v>
@@ -6505,10 +6499,10 @@
         <v>96</v>
       </c>
       <c r="C76" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D76" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E76" s="1">
         <v>44840</v>
@@ -6580,10 +6574,10 @@
         <v>97</v>
       </c>
       <c r="C77" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D77" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E77" s="1">
         <v>44840</v>
@@ -6608,10 +6602,10 @@
         <v>0</v>
       </c>
       <c r="M77" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N77" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O77" s="2">
         <v>0</v>
@@ -6655,10 +6649,10 @@
         <v>98</v>
       </c>
       <c r="C78" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D78" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E78" s="1">
         <v>44840</v>
@@ -6683,10 +6677,10 @@
         <v>0</v>
       </c>
       <c r="M78" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N78" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O78" s="2">
         <v>0</v>
@@ -6730,10 +6724,10 @@
         <v>99</v>
       </c>
       <c r="C79" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D79" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E79" s="1">
         <v>44840</v>
@@ -6805,10 +6799,10 @@
         <v>100</v>
       </c>
       <c r="C80" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D80" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E80" s="1">
         <v>44840</v>
@@ -6827,10 +6821,10 @@
         <v>6</v>
       </c>
       <c r="K80" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L80" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M80" s="2">
         <v>0</v>
@@ -6880,10 +6874,10 @@
         <v>101</v>
       </c>
       <c r="C81" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D81" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E81" s="1">
         <v>44840</v>
@@ -6902,10 +6896,10 @@
         <v>6</v>
       </c>
       <c r="K81" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L81" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M81" s="2">
         <v>0</v>
@@ -6955,19 +6949,19 @@
         <v>102</v>
       </c>
       <c r="C82" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D82" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E82" s="1">
         <v>44894</v>
       </c>
       <c r="F82" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G82" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H82" s="2"/>
       <c r="I82" s="2">
@@ -6986,7 +6980,7 @@
         <v>0</v>
       </c>
       <c r="N82" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O82" s="2">
         <v>0</v>
@@ -7030,19 +7024,19 @@
         <v>103</v>
       </c>
       <c r="C83" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D83" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E83" s="1">
         <v>44894</v>
       </c>
       <c r="F83" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G83" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H83" s="2"/>
       <c r="I83" s="2">
@@ -7105,19 +7099,19 @@
         <v>104</v>
       </c>
       <c r="C84" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D84" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E84" s="1">
         <v>44894</v>
       </c>
       <c r="F84" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G84" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H84" s="2"/>
       <c r="I84" s="2">
@@ -7180,19 +7174,19 @@
         <v>105</v>
       </c>
       <c r="C85" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D85" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E85" s="1">
         <v>44894</v>
       </c>
       <c r="F85" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G85" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H85" s="2"/>
       <c r="I85" s="2">
@@ -7211,7 +7205,7 @@
         <v>0</v>
       </c>
       <c r="N85" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O85" s="2">
         <v>0</v>
@@ -7255,19 +7249,19 @@
         <v>106</v>
       </c>
       <c r="C86" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D86" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E86" s="1">
         <v>44894</v>
       </c>
       <c r="F86" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G86" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H86" s="2"/>
       <c r="I86" s="2">
@@ -7330,10 +7324,10 @@
         <v>107</v>
       </c>
       <c r="C87" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D87" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E87" s="1">
         <v>44894</v>
@@ -7405,10 +7399,10 @@
         <v>108</v>
       </c>
       <c r="C88" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D88" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E88" s="1">
         <v>44894</v>
@@ -7480,10 +7474,10 @@
         <v>109</v>
       </c>
       <c r="C89" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D89" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E89" s="1">
         <v>44894</v>
@@ -7555,19 +7549,19 @@
         <v>110</v>
       </c>
       <c r="C90" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D90" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E90" s="1">
         <v>44894</v>
       </c>
       <c r="F90" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G90" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H90" s="2"/>
       <c r="I90" s="2">
@@ -7630,10 +7624,10 @@
         <v>111</v>
       </c>
       <c r="C91" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D91" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E91" s="1">
         <v>44865</v>
@@ -7705,19 +7699,19 @@
         <v>112</v>
       </c>
       <c r="C92" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D92" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E92" s="1">
         <v>44865</v>
       </c>
       <c r="F92" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G92" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H92" s="2"/>
       <c r="I92" s="2">
@@ -7745,7 +7739,7 @@
         <v>0</v>
       </c>
       <c r="Q92" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R92" s="2">
         <v>0</v>
@@ -7780,10 +7774,10 @@
         <v>113</v>
       </c>
       <c r="C93" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D93" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E93" s="1">
         <v>44865</v>
@@ -7802,10 +7796,10 @@
         <v>5</v>
       </c>
       <c r="K93" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L93" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M93" s="2">
         <v>0</v>
@@ -7855,10 +7849,10 @@
         <v>114</v>
       </c>
       <c r="C94" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D94" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E94" s="1">
         <v>44865</v>
@@ -7877,10 +7871,10 @@
         <v>5</v>
       </c>
       <c r="K94" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L94" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M94" s="2">
         <v>0</v>
@@ -7930,10 +7924,10 @@
         <v>115</v>
       </c>
       <c r="C95" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D95" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E95" s="1">
         <v>44865</v>
@@ -8005,10 +7999,10 @@
         <v>116</v>
       </c>
       <c r="C96" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D96" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E96" s="1">
         <v>44865</v>
@@ -8080,10 +8074,10 @@
         <v>117</v>
       </c>
       <c r="C97" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D97" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E97" s="1">
         <v>44865</v>
@@ -8155,10 +8149,10 @@
         <v>118</v>
       </c>
       <c r="C98" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D98" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E98" s="1">
         <v>44865</v>
@@ -8230,19 +8224,19 @@
         <v>119</v>
       </c>
       <c r="C99" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D99" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E99" s="1">
         <v>44865</v>
       </c>
       <c r="F99" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G99" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H99" s="2"/>
       <c r="I99" s="2">
@@ -8270,7 +8264,7 @@
         <v>0</v>
       </c>
       <c r="Q99" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R99" s="2">
         <v>0</v>
@@ -8305,19 +8299,19 @@
         <v>120</v>
       </c>
       <c r="C100" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D100" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E100" s="1">
         <v>44879</v>
       </c>
       <c r="F100" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G100" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H100" s="2"/>
       <c r="I100" s="2">
@@ -8380,19 +8374,19 @@
         <v>121</v>
       </c>
       <c r="C101" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D101" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E101" s="1">
         <v>44879</v>
       </c>
       <c r="F101" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G101" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H101" s="2"/>
       <c r="I101" s="2">
@@ -8402,10 +8396,10 @@
         <v>3</v>
       </c>
       <c r="K101" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L101" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M101" s="2">
         <v>0</v>
@@ -8455,19 +8449,19 @@
         <v>122</v>
       </c>
       <c r="C102" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D102" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E102" s="1">
         <v>44879</v>
       </c>
       <c r="F102" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G102" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H102" s="2"/>
       <c r="I102" s="2">
@@ -8530,10 +8524,10 @@
         <v>123</v>
       </c>
       <c r="C103" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D103" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E103" s="1">
         <v>44879</v>
@@ -8605,19 +8599,19 @@
         <v>124</v>
       </c>
       <c r="C104" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="D104" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E104" s="1">
         <v>44879</v>
       </c>
       <c r="F104" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G104" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H104" s="2"/>
       <c r="I104" s="2">
@@ -8680,10 +8674,10 @@
         <v>125</v>
       </c>
       <c r="C105" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D105" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E105" s="1">
         <v>44879</v>
@@ -8755,10 +8749,10 @@
         <v>126</v>
       </c>
       <c r="C106" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="D106" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E106" s="1">
         <v>44879</v>
@@ -8777,10 +8771,10 @@
         <v>3</v>
       </c>
       <c r="K106" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L106" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M106" s="2">
         <v>0</v>
@@ -8830,10 +8824,10 @@
         <v>127</v>
       </c>
       <c r="C107" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D107" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E107" s="1">
         <v>44893</v>
@@ -8905,10 +8899,10 @@
         <v>128</v>
       </c>
       <c r="C108" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D108" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E108" s="1">
         <v>44893</v>
@@ -8980,10 +8974,10 @@
         <v>129</v>
       </c>
       <c r="C109" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D109" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E109" s="1">
         <v>44887</v>
@@ -9055,10 +9049,10 @@
         <v>130</v>
       </c>
       <c r="C110" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="D110" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E110" s="1">
         <v>44887</v>
@@ -9101,7 +9095,7 @@
         <v>0</v>
       </c>
       <c r="S110" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T110" s="2">
         <v>0</v>
@@ -9130,10 +9124,10 @@
         <v>131</v>
       </c>
       <c r="C111" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="D111" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E111" s="1">
         <v>44887</v>
@@ -9176,7 +9170,7 @@
         <v>0</v>
       </c>
       <c r="S111" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T111" s="2">
         <v>0</v>
@@ -9205,19 +9199,19 @@
         <v>132</v>
       </c>
       <c r="C112" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="D112" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E112" s="1">
         <v>44887</v>
       </c>
       <c r="F112" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G112" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H112" s="2"/>
       <c r="I112" s="2">
@@ -9280,19 +9274,19 @@
         <v>133</v>
       </c>
       <c r="C113" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="D113" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E113" s="1">
         <v>44887</v>
       </c>
       <c r="F113" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G113" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H113" s="2"/>
       <c r="I113" s="2">
@@ -9355,10 +9349,10 @@
         <v>134</v>
       </c>
       <c r="C114" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="D114" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E114" s="1">
         <v>44896</v>
@@ -9430,10 +9424,10 @@
         <v>135</v>
       </c>
       <c r="C115" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="D115" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E115" s="1">
         <v>44714</v>
@@ -9507,10 +9501,10 @@
         <v>135</v>
       </c>
       <c r="C116" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="D116" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E116" s="1">
         <v>44714</v>

</xml_diff>

<commit_message>
update pending and code
</commit_message>
<xml_diff>
--- a/datasets/lab_detail.xlsx
+++ b/datasets/lab_detail.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="274">
   <si>
     <t>sampleid</t>
   </si>
@@ -81,6 +81,15 @@
     <t>substance</t>
   </si>
   <si>
+    <t>dimethyl sulfone (methylsulfonylmethane MSM)</t>
+  </si>
+  <si>
+    <t>phenethyl 4-ANPP</t>
+  </si>
+  <si>
+    <t>p-fluorofentanyl</t>
+  </si>
+  <si>
     <t>despropionyl p-fluorofentanyl</t>
   </si>
   <si>
@@ -90,330 +99,321 @@
     <t>fentanyl</t>
   </si>
   <si>
+    <t>4-ANPP</t>
+  </si>
+  <si>
+    <t>3,4-methylenedioxy-N-benzylcathinone (BMDP)</t>
+  </si>
+  <si>
+    <t>3,4-MDMA</t>
+  </si>
+  <si>
+    <t>benzoylecgonine (BZ)</t>
+  </si>
+  <si>
+    <t>cocaine</t>
+  </si>
+  <si>
+    <t>levamisole</t>
+  </si>
+  <si>
+    <t>phenacetin</t>
+  </si>
+  <si>
+    <t>methyl ecgonidine (MED)</t>
+  </si>
+  <si>
+    <t>norcocaine</t>
+  </si>
+  <si>
+    <t>tropacocaine</t>
+  </si>
+  <si>
+    <t>fentanyl</t>
+  </si>
+  <si>
+    <t>4-ANPP</t>
+  </si>
+  <si>
+    <t>tramadol</t>
+  </si>
+  <si>
+    <t>p-fluoro phenethyl 4-ANPP</t>
+  </si>
+  <si>
+    <t>non-specific sugars</t>
+  </si>
+  <si>
+    <t>methamphetamine</t>
+  </si>
+  <si>
+    <t>despropionyl p-fluorofentanyl</t>
+  </si>
+  <si>
+    <t>eutylone</t>
+  </si>
+  <si>
+    <t>caffeine</t>
+  </si>
+  <si>
+    <t>methamphetamine</t>
+  </si>
+  <si>
+    <t>heroin</t>
+  </si>
+  <si>
+    <t>fentanyl</t>
+  </si>
+  <si>
+    <t>xylazine</t>
+  </si>
+  <si>
+    <t>acetylcodeine</t>
+  </si>
+  <si>
+    <t>6-monoacetylmorphine (6-MAM)</t>
+  </si>
+  <si>
+    <t>4-ANPP</t>
+  </si>
+  <si>
+    <t>urea</t>
+  </si>
+  <si>
+    <t>non-specific sugars</t>
+  </si>
+  <si>
+    <t>phenethyl 4-ANPP</t>
+  </si>
+  <si>
+    <t>caffeine</t>
+  </si>
+  <si>
+    <t>fentanyl</t>
+  </si>
+  <si>
+    <t>4-ANPP</t>
+  </si>
+  <si>
+    <t>cocaine</t>
+  </si>
+  <si>
+    <t>fentanyl</t>
+  </si>
+  <si>
+    <t>xylazine</t>
+  </si>
+  <si>
+    <t>4-ANPP</t>
+  </si>
+  <si>
+    <t>tramadol</t>
+  </si>
+  <si>
+    <t>heroin</t>
+  </si>
+  <si>
+    <t>N-ethyl-4-ANPP</t>
+  </si>
+  <si>
+    <t>acetylcodeine</t>
+  </si>
+  <si>
+    <t>1,3-Diacetin</t>
+  </si>
+  <si>
+    <t>phenethyl 4-ANPP</t>
+  </si>
+  <si>
+    <t>p-fluorofentanyl</t>
+  </si>
+  <si>
+    <t>N-phenylpropanamide</t>
+  </si>
+  <si>
+    <t>lidocaine</t>
+  </si>
+  <si>
     <t>dimethyl sulfone (methylsulfonylmethane MSM)</t>
   </si>
   <si>
+    <t>acetaminophen</t>
+  </si>
+  <si>
+    <t>6-monoacetylmorphine (6-MAM)</t>
+  </si>
+  <si>
+    <t>quinine</t>
+  </si>
+  <si>
+    <t>metonitazene</t>
+  </si>
+  <si>
     <t>phenethyl 4-ANPP</t>
   </si>
   <si>
+    <t>fentanyl</t>
+  </si>
+  <si>
     <t>4-ANPP</t>
   </si>
   <si>
+    <t>heroin</t>
+  </si>
+  <si>
+    <t>inositol</t>
+  </si>
+  <si>
+    <t>methadone</t>
+  </si>
+  <si>
+    <t>acetylcodeine</t>
+  </si>
+  <si>
+    <t>1,3-Diacetin</t>
+  </si>
+  <si>
+    <t>non-specific sugars</t>
+  </si>
+  <si>
+    <t>gabapentin</t>
+  </si>
+  <si>
+    <t>diphenhydramine</t>
+  </si>
+  <si>
+    <t>methamphetamine</t>
+  </si>
+  <si>
+    <t>N-piperidinyl etonitazene</t>
+  </si>
+  <si>
+    <t>fentanyl</t>
+  </si>
+  <si>
+    <t>dimethyl sulfone (methylsulfonylmethane MSM)</t>
+  </si>
+  <si>
+    <t>non-specific organic acids</t>
+  </si>
+  <si>
+    <t>methamphetamine</t>
+  </si>
+  <si>
+    <t>procaine</t>
+  </si>
+  <si>
+    <t>heroin</t>
+  </si>
+  <si>
+    <t>fentanyl</t>
+  </si>
+  <si>
+    <t>cocaine</t>
+  </si>
+  <si>
+    <t>xylazine</t>
+  </si>
+  <si>
+    <t>4-ANPP</t>
+  </si>
+  <si>
+    <t>phenethylbromide</t>
+  </si>
+  <si>
+    <t>1,3-Diacetin</t>
+  </si>
+  <si>
     <t>p-fluorofentanyl</t>
   </si>
   <si>
-    <t>3,4-methylenedioxy-N-benzylcathinone (BMDP)</t>
-  </si>
-  <si>
-    <t>3,4-MDMA</t>
+    <t>p-fluoro phenethyl 4-ANPP</t>
+  </si>
+  <si>
+    <t>despropionyl p-fluorofentanyl</t>
+  </si>
+  <si>
+    <t>nicotine</t>
+  </si>
+  <si>
+    <t>xylazine</t>
+  </si>
+  <si>
+    <t>phenethyl chloride</t>
+  </si>
+  <si>
+    <t>menthol</t>
+  </si>
+  <si>
+    <t>quinine</t>
+  </si>
+  <si>
+    <t>1,3-Diacetin</t>
+  </si>
+  <si>
+    <t>fentanyl</t>
+  </si>
+  <si>
+    <t>diphenhydramine</t>
+  </si>
+  <si>
+    <t>caffeine</t>
+  </si>
+  <si>
+    <t>4-ANPP</t>
+  </si>
+  <si>
+    <t>1-phenethyl-4-propionyloxypiperidine</t>
+  </si>
+  <si>
+    <t>p-fluorofentanyl</t>
+  </si>
+  <si>
+    <t>N-ethyl-4-ANPP</t>
+  </si>
+  <si>
+    <t>tramadol</t>
+  </si>
+  <si>
+    <t>4-ANPP</t>
+  </si>
+  <si>
+    <t>N-phenylpropanamide</t>
+  </si>
+  <si>
+    <t>acetaminophen</t>
+  </si>
+  <si>
+    <t>N-ethyl-4-ANPP</t>
+  </si>
+  <si>
+    <t>methamphetamine</t>
+  </si>
+  <si>
+    <t>fentanyl</t>
+  </si>
+  <si>
+    <t>methamphetamine</t>
   </si>
   <si>
     <t>levamisole</t>
   </si>
   <si>
+    <t>cocaine</t>
+  </si>
+  <si>
+    <t>ecgonine methylester (EME)</t>
+  </si>
+  <si>
     <t>tropacocaine</t>
   </si>
   <si>
-    <t>phenacetin</t>
-  </si>
-  <si>
-    <t>benzoylecgonine (BZ)</t>
-  </si>
-  <si>
     <t>methyl ecgonidine (MED)</t>
   </si>
   <si>
-    <t>cocaine</t>
-  </si>
-  <si>
-    <t>norcocaine</t>
-  </si>
-  <si>
     <t>methamphetamine</t>
   </si>
   <si>
-    <t>p-fluoro phenethyl 4-ANPP</t>
-  </si>
-  <si>
-    <t>despropionyl p-fluorofentanyl</t>
-  </si>
-  <si>
-    <t>fentanyl</t>
-  </si>
-  <si>
-    <t>4-ANPP</t>
-  </si>
-  <si>
-    <t>tramadol</t>
-  </si>
-  <si>
-    <t>non-specific sugars</t>
-  </si>
-  <si>
-    <t>methamphetamine</t>
-  </si>
-  <si>
-    <t>caffeine</t>
-  </si>
-  <si>
-    <t>eutylone</t>
-  </si>
-  <si>
-    <t>urea</t>
-  </si>
-  <si>
-    <t>phenethyl 4-ANPP</t>
-  </si>
-  <si>
-    <t>xylazine</t>
-  </si>
-  <si>
-    <t>heroin</t>
-  </si>
-  <si>
-    <t>4-ANPP</t>
-  </si>
-  <si>
-    <t>non-specific sugars</t>
-  </si>
-  <si>
-    <t>6-monoacetylmorphine (6-MAM)</t>
-  </si>
-  <si>
-    <t>fentanyl</t>
-  </si>
-  <si>
-    <t>acetylcodeine</t>
-  </si>
-  <si>
-    <t>4-ANPP</t>
-  </si>
-  <si>
-    <t>fentanyl</t>
-  </si>
-  <si>
-    <t>caffeine</t>
-  </si>
-  <si>
-    <t>cocaine</t>
-  </si>
-  <si>
-    <t>1,3-Diacetin</t>
-  </si>
-  <si>
-    <t>N-ethyl-4-ANPP</t>
-  </si>
-  <si>
-    <t>heroin</t>
-  </si>
-  <si>
-    <t>6-monoacetylmorphine (6-MAM)</t>
-  </si>
-  <si>
-    <t>4-ANPP</t>
-  </si>
-  <si>
-    <t>tramadol</t>
-  </si>
-  <si>
-    <t>N-phenylpropanamide</t>
-  </si>
-  <si>
-    <t>fentanyl</t>
-  </si>
-  <si>
-    <t>acetylcodeine</t>
-  </si>
-  <si>
-    <t>xylazine</t>
-  </si>
-  <si>
-    <t>acetaminophen</t>
-  </si>
-  <si>
-    <t>lidocaine</t>
-  </si>
-  <si>
-    <t>dimethyl sulfone (methylsulfonylmethane MSM)</t>
-  </si>
-  <si>
-    <t>p-fluorofentanyl</t>
-  </si>
-  <si>
-    <t>phenethyl 4-ANPP</t>
-  </si>
-  <si>
-    <t>diphenhydramine</t>
-  </si>
-  <si>
-    <t>phenethyl 4-ANPP</t>
-  </si>
-  <si>
-    <t>gabapentin</t>
-  </si>
-  <si>
-    <t>methadone</t>
-  </si>
-  <si>
-    <t>inositol</t>
-  </si>
-  <si>
-    <t>quinine</t>
-  </si>
-  <si>
-    <t>N-piperidinyl etonitazene</t>
-  </si>
-  <si>
-    <t>non-specific sugars</t>
-  </si>
-  <si>
-    <t>methamphetamine</t>
-  </si>
-  <si>
-    <t>fentanyl</t>
-  </si>
-  <si>
-    <t>4-ANPP</t>
-  </si>
-  <si>
-    <t>1,3-Diacetin</t>
-  </si>
-  <si>
-    <t>heroin</t>
-  </si>
-  <si>
-    <t>metonitazene</t>
-  </si>
-  <si>
-    <t>acetylcodeine</t>
-  </si>
-  <si>
-    <t>fentanyl</t>
-  </si>
-  <si>
-    <t>non-specific organic acids</t>
-  </si>
-  <si>
-    <t>dimethyl sulfone (methylsulfonylmethane MSM)</t>
-  </si>
-  <si>
-    <t>methamphetamine</t>
-  </si>
-  <si>
-    <t>procaine</t>
-  </si>
-  <si>
-    <t>xylazine</t>
-  </si>
-  <si>
-    <t>4-ANPP</t>
-  </si>
-  <si>
-    <t>heroin</t>
-  </si>
-  <si>
-    <t>fentanyl</t>
-  </si>
-  <si>
-    <t>cocaine</t>
-  </si>
-  <si>
-    <t>1,3-Diacetin</t>
-  </si>
-  <si>
-    <t>nicotine</t>
-  </si>
-  <si>
-    <t>phenethylbromide</t>
-  </si>
-  <si>
-    <t>menthol</t>
-  </si>
-  <si>
-    <t>despropionyl p-fluorofentanyl</t>
-  </si>
-  <si>
-    <t>p-fluorofentanyl</t>
-  </si>
-  <si>
-    <t>p-fluoro phenethyl 4-ANPP</t>
-  </si>
-  <si>
-    <t>xylazine</t>
-  </si>
-  <si>
-    <t>phenethyl chloride</t>
-  </si>
-  <si>
-    <t>caffeine</t>
-  </si>
-  <si>
-    <t>p-fluorofentanyl</t>
-  </si>
-  <si>
-    <t>1,3-Diacetin</t>
-  </si>
-  <si>
-    <t>fentanyl</t>
-  </si>
-  <si>
-    <t>1-phenethyl-4-propionyloxypiperidine</t>
-  </si>
-  <si>
-    <t>N-ethyl-4-ANPP</t>
-  </si>
-  <si>
-    <t>diphenhydramine</t>
-  </si>
-  <si>
-    <t>quinine</t>
-  </si>
-  <si>
-    <t>4-ANPP</t>
-  </si>
-  <si>
-    <t>acetaminophen</t>
-  </si>
-  <si>
-    <t>tramadol</t>
-  </si>
-  <si>
-    <t>N-ethyl-4-ANPP</t>
-  </si>
-  <si>
-    <t>N-phenylpropanamide</t>
-  </si>
-  <si>
-    <t>4-ANPP</t>
-  </si>
-  <si>
-    <t>fentanyl</t>
-  </si>
-  <si>
-    <t>methamphetamine</t>
-  </si>
-  <si>
-    <t>fentanyl</t>
-  </si>
-  <si>
-    <t>levamisole</t>
-  </si>
-  <si>
-    <t>methyl ecgonidine (MED)</t>
-  </si>
-  <si>
-    <t>tropacocaine</t>
-  </si>
-  <si>
-    <t>cocaine</t>
-  </si>
-  <si>
-    <t>ecgonine methylester (EME)</t>
-  </si>
-  <si>
-    <t>methamphetamine</t>
-  </si>
-  <si>
     <t>no compounds of interest detected</t>
   </si>
   <si>
@@ -465,6 +465,9 @@
     <t/>
   </si>
   <si>
+    <t>trace</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
@@ -489,6 +492,12 @@
     <t/>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t>trace</t>
   </si>
   <si>
@@ -513,24 +522,48 @@
     <t/>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>trace</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>trace</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t>trace</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t>trace</t>
   </si>
   <si>
@@ -540,6 +573,9 @@
     <t/>
   </si>
   <si>
+    <t>trace</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
@@ -552,30 +588,66 @@
     <t/>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t>trace</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
+    <t>trace</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
+    <t>trace</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
     <t/>
   </si>
   <si>
+    <t>trace</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t>trace</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
+    <t>trace</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
@@ -585,6 +657,9 @@
     <t/>
   </si>
   <si>
+    <t>trace</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
@@ -594,6 +669,9 @@
     <t/>
   </si>
   <si>
+    <t>trace</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
@@ -603,93 +681,9 @@
     <t/>
   </si>
   <si>
-    <t>trace</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>trace</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>trace</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>trace</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>trace</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>trace</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>trace</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>trace</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>trace</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>trace</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
     <t>method</t>
   </si>
   <si>
@@ -739,9 +733,6 @@
   </si>
   <si>
     <t>Derivatized GCMS</t>
-  </si>
-  <si>
-    <t>GCMS</t>
   </si>
   <si>
     <t>date_complete</t>
@@ -905,109 +896,109 @@
         <v>134</v>
       </c>
       <c r="D1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F1" t="s">
+        <v>241</v>
+      </c>
+      <c r="G1" t="s">
+        <v>242</v>
+      </c>
+      <c r="H1" t="s">
         <v>243</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>244</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>245</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>246</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>247</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>248</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>249</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>250</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>251</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>252</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>253</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>254</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="T1" t="s">
         <v>255</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" t="s">
         <v>256</v>
       </c>
-      <c r="S1" t="s">
+      <c r="V1" t="s">
         <v>257</v>
       </c>
-      <c r="T1" t="s">
+      <c r="W1" t="s">
         <v>258</v>
       </c>
-      <c r="U1" t="s">
+      <c r="X1" t="s">
         <v>259</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Y1" t="s">
         <v>260</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Z1" t="s">
         <v>261</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AA1" t="s">
         <v>262</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AB1" t="s">
         <v>263</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AC1" t="s">
         <v>264</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AD1" t="s">
         <v>265</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AE1" t="s">
         <v>266</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AF1" t="s">
         <v>267</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AG1" t="s">
         <v>268</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AH1" t="s">
         <v>269</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AI1" t="s">
         <v>270</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AJ1" t="s">
         <v>271</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AK1" t="s">
         <v>272</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AL1" t="s">
         <v>273</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>274</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>275</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="2">
@@ -1021,7 +1012,7 @@
         <v>135</v>
       </c>
       <c r="D2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E2" s="1">
         <v>44603</v>
@@ -1091,7 +1082,7 @@
         <v>0</v>
       </c>
       <c r="AB2" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC2" s="2">
         <v>0</v>
@@ -1118,7 +1109,7 @@
         <v>0</v>
       </c>
       <c r="AK2" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL2" s="2">
         <v>0</v>
@@ -1135,7 +1126,7 @@
         <v>136</v>
       </c>
       <c r="D3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E3" s="1">
         <v>44603</v>
@@ -1160,10 +1151,10 @@
         <v>0</v>
       </c>
       <c r="M3" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N3" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O3" s="2">
         <v>0</v>
@@ -1249,7 +1240,7 @@
         <v>137</v>
       </c>
       <c r="D4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E4" s="1">
         <v>44603</v>
@@ -1268,10 +1259,10 @@
         <v>7</v>
       </c>
       <c r="K4" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L4" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M4" s="2">
         <v>0</v>
@@ -1363,7 +1354,7 @@
         <v>138</v>
       </c>
       <c r="D5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E5" s="1">
         <v>44603</v>
@@ -1433,7 +1424,7 @@
         <v>0</v>
       </c>
       <c r="AB5" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC5" s="2">
         <v>0</v>
@@ -1460,7 +1451,7 @@
         <v>0</v>
       </c>
       <c r="AK5" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL5" s="2">
         <v>0</v>
@@ -1477,7 +1468,7 @@
         <v>139</v>
       </c>
       <c r="D6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E6" s="1">
         <v>44603</v>
@@ -1502,10 +1493,10 @@
         <v>0</v>
       </c>
       <c r="M6" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N6" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O6" s="2">
         <v>0</v>
@@ -1591,7 +1582,7 @@
         <v>140</v>
       </c>
       <c r="D7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E7" s="1">
         <v>44603</v>
@@ -1610,10 +1601,10 @@
         <v>7</v>
       </c>
       <c r="K7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M7" s="2">
         <v>0</v>
@@ -1661,7 +1652,7 @@
         <v>0</v>
       </c>
       <c r="AB7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC7" s="2">
         <v>0</v>
@@ -1685,7 +1676,7 @@
         <v>0</v>
       </c>
       <c r="AJ7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK7" s="2">
         <v>0</v>
@@ -1705,7 +1696,7 @@
         <v>141</v>
       </c>
       <c r="D8" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E8" s="1">
         <v>44603</v>
@@ -1775,7 +1766,7 @@
         <v>0</v>
       </c>
       <c r="AB8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC8" s="2">
         <v>0</v>
@@ -1799,7 +1790,7 @@
         <v>0</v>
       </c>
       <c r="AJ8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK8" s="2">
         <v>0</v>
@@ -1819,7 +1810,7 @@
         <v>142</v>
       </c>
       <c r="D9" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E9" s="1">
         <v>44777</v>
@@ -1933,7 +1924,7 @@
         <v>143</v>
       </c>
       <c r="D10" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E10" s="1">
         <v>44777</v>
@@ -2047,7 +2038,7 @@
         <v>144</v>
       </c>
       <c r="D11" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E11" s="1">
         <v>44758</v>
@@ -2161,7 +2152,7 @@
         <v>145</v>
       </c>
       <c r="D12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E12" s="1">
         <v>44714</v>
@@ -2207,7 +2198,7 @@
         <v>0</v>
       </c>
       <c r="T12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U12" s="2">
         <v>0</v>
@@ -2246,7 +2237,7 @@
         <v>0</v>
       </c>
       <c r="AG12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH12" s="2">
         <v>0</v>
@@ -2272,7 +2263,7 @@
         <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D13" t="s">
         <v>226</v>
@@ -2281,10 +2272,10 @@
         <v>44714</v>
       </c>
       <c r="F13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2">
@@ -2357,10 +2348,10 @@
         <v>0</v>
       </c>
       <c r="AF13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH13" s="2">
         <v>0</v>
@@ -2386,10 +2377,10 @@
         <v>33</v>
       </c>
       <c r="C14" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D14" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E14" s="1">
         <v>44714</v>
@@ -2435,7 +2426,7 @@
         <v>0</v>
       </c>
       <c r="T14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U14" s="2">
         <v>0</v>
@@ -2500,7 +2491,7 @@
         <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D15" t="s">
         <v>227</v>
@@ -2588,7 +2579,7 @@
         <v>0</v>
       </c>
       <c r="AG15" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH15" s="2">
         <v>0</v>
@@ -2614,7 +2605,7 @@
         <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D16" t="s">
         <v>228</v>
@@ -2728,7 +2719,7 @@
         <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D17" t="s">
         <v>228</v>
@@ -2737,10 +2728,10 @@
         <v>44714</v>
       </c>
       <c r="F17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2">
@@ -2813,7 +2804,7 @@
         <v>0</v>
       </c>
       <c r="AF17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG17" s="2">
         <v>0</v>
@@ -2930,7 +2921,7 @@
         <v>1</v>
       </c>
       <c r="AG18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH18" s="2">
         <v>0</v>
@@ -2956,19 +2947,19 @@
         <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D19" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E19" s="1">
         <v>44759</v>
       </c>
       <c r="F19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2">
@@ -2978,10 +2969,10 @@
         <v>4</v>
       </c>
       <c r="K19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M19" s="2">
         <v>0</v>
@@ -2996,7 +2987,7 @@
         <v>0</v>
       </c>
       <c r="Q19" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R19" s="2">
         <v>0</v>
@@ -3029,7 +3020,7 @@
         <v>0</v>
       </c>
       <c r="AB19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC19" s="2">
         <v>0</v>
@@ -3070,19 +3061,19 @@
         <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D20" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E20" s="1">
         <v>44759</v>
       </c>
       <c r="F20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2">
@@ -3170,7 +3161,7 @@
         <v>1</v>
       </c>
       <c r="AK20" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL20" s="2">
         <v>0</v>
@@ -3184,19 +3175,19 @@
         <v>40</v>
       </c>
       <c r="C21" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D21" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E21" s="1">
         <v>44759</v>
       </c>
       <c r="F21" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2">
@@ -3239,7 +3230,7 @@
         <v>0</v>
       </c>
       <c r="V21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W21" s="2">
         <v>0</v>
@@ -3284,7 +3275,7 @@
         <v>0</v>
       </c>
       <c r="AK21" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL21" s="2">
         <v>0</v>
@@ -3298,19 +3289,19 @@
         <v>41</v>
       </c>
       <c r="C22" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D22" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E22" s="1">
         <v>44759</v>
       </c>
       <c r="F22" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="2">
@@ -3320,10 +3311,10 @@
         <v>4</v>
       </c>
       <c r="K22" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L22" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M22" s="2">
         <v>0</v>
@@ -3371,7 +3362,7 @@
         <v>0</v>
       </c>
       <c r="AB22" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC22" s="2">
         <v>0</v>
@@ -3395,10 +3386,10 @@
         <v>0</v>
       </c>
       <c r="AJ22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL22" s="2">
         <v>0</v>
@@ -3412,10 +3403,10 @@
         <v>42</v>
       </c>
       <c r="C23" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D23" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E23" s="1">
         <v>44759</v>
@@ -3500,7 +3491,7 @@
         <v>0</v>
       </c>
       <c r="AG23" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH23" s="2">
         <v>0</v>
@@ -3509,7 +3500,7 @@
         <v>0</v>
       </c>
       <c r="AJ23" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK23" s="2">
         <v>0</v>
@@ -3526,10 +3517,10 @@
         <v>43</v>
       </c>
       <c r="C24" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D24" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E24" s="1">
         <v>44759</v>
@@ -3566,7 +3557,7 @@
         <v>0</v>
       </c>
       <c r="Q24" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R24" s="2">
         <v>0</v>
@@ -3581,7 +3572,7 @@
         <v>0</v>
       </c>
       <c r="V24" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W24" s="2">
         <v>0</v>
@@ -3599,7 +3590,7 @@
         <v>0</v>
       </c>
       <c r="AB24" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC24" s="2">
         <v>0</v>
@@ -3640,10 +3631,10 @@
         <v>44</v>
       </c>
       <c r="C25" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D25" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E25" s="1">
         <v>44759</v>
@@ -3713,7 +3704,7 @@
         <v>0</v>
       </c>
       <c r="AB25" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC25" s="2">
         <v>0</v>
@@ -3728,7 +3719,7 @@
         <v>0</v>
       </c>
       <c r="AG25" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH25" s="2">
         <v>0</v>
@@ -3740,7 +3731,7 @@
         <v>0</v>
       </c>
       <c r="AK25" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL25" s="2">
         <v>0</v>
@@ -3754,10 +3745,10 @@
         <v>45</v>
       </c>
       <c r="C26" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D26" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E26" s="1">
         <v>44721</v>
@@ -3794,7 +3785,7 @@
         <v>0</v>
       </c>
       <c r="Q26" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R26" s="2">
         <v>0</v>
@@ -3857,7 +3848,7 @@
         <v>0</v>
       </c>
       <c r="AL26" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
@@ -3868,10 +3859,10 @@
         <v>46</v>
       </c>
       <c r="C27" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D27" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E27" s="1">
         <v>44721</v>
@@ -3982,10 +3973,10 @@
         <v>47</v>
       </c>
       <c r="C28" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D28" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E28" s="1">
         <v>44721</v>
@@ -4022,7 +4013,7 @@
         <v>0</v>
       </c>
       <c r="Q28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R28" s="2">
         <v>0</v>
@@ -4085,7 +4076,7 @@
         <v>0</v>
       </c>
       <c r="AL28" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -4096,19 +4087,19 @@
         <v>48</v>
       </c>
       <c r="C29" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D29" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E29" s="1">
         <v>44707</v>
       </c>
       <c r="F29" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G29" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H29" s="2"/>
       <c r="I29" s="2">
@@ -4169,7 +4160,7 @@
         <v>0</v>
       </c>
       <c r="AB29" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC29" s="2">
         <v>0</v>
@@ -4210,19 +4201,19 @@
         <v>49</v>
       </c>
       <c r="C30" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="D30" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E30" s="1">
         <v>44707</v>
       </c>
       <c r="F30" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G30" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H30" s="2"/>
       <c r="I30" s="2">
@@ -4232,10 +4223,10 @@
         <v>5</v>
       </c>
       <c r="K30" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L30" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M30" s="2">
         <v>0</v>
@@ -4283,7 +4274,7 @@
         <v>0</v>
       </c>
       <c r="AB30" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC30" s="2">
         <v>0</v>
@@ -4307,7 +4298,7 @@
         <v>0</v>
       </c>
       <c r="AJ30" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK30" s="2">
         <v>0</v>
@@ -4324,10 +4315,10 @@
         <v>50</v>
       </c>
       <c r="C31" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="D31" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="E31" s="1">
         <v>44707</v>
@@ -4438,10 +4429,10 @@
         <v>51</v>
       </c>
       <c r="C32" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="D32" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="E32" s="1">
         <v>44707</v>
@@ -4529,7 +4520,7 @@
         <v>0</v>
       </c>
       <c r="AH32" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI32" s="2">
         <v>0</v>
@@ -4552,10 +4543,10 @@
         <v>52</v>
       </c>
       <c r="C33" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="D33" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="E33" s="1">
         <v>44707</v>
@@ -4625,7 +4616,7 @@
         <v>0</v>
       </c>
       <c r="AB33" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC33" s="2">
         <v>0</v>
@@ -4649,7 +4640,7 @@
         <v>0</v>
       </c>
       <c r="AJ33" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK33" s="2">
         <v>0</v>
@@ -4666,19 +4657,19 @@
         <v>53</v>
       </c>
       <c r="C34" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D34" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="E34" s="1">
         <v>44707</v>
       </c>
       <c r="F34" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G34" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H34" s="2"/>
       <c r="I34" s="2">
@@ -4754,7 +4745,7 @@
         <v>0</v>
       </c>
       <c r="AG34" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH34" s="2">
         <v>0</v>
@@ -4763,7 +4754,7 @@
         <v>0</v>
       </c>
       <c r="AJ34" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK34" s="2">
         <v>0</v>
@@ -4780,10 +4771,10 @@
         <v>54</v>
       </c>
       <c r="C35" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D35" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="E35" s="1">
         <v>44707</v>
@@ -4853,7 +4844,7 @@
         <v>0</v>
       </c>
       <c r="AB35" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC35" s="2">
         <v>0</v>
@@ -4894,10 +4885,10 @@
         <v>55</v>
       </c>
       <c r="C36" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D36" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="E36" s="1">
         <v>44707</v>
@@ -4916,10 +4907,10 @@
         <v>5</v>
       </c>
       <c r="K36" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L36" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M36" s="2">
         <v>0</v>
@@ -4967,7 +4958,7 @@
         <v>0</v>
       </c>
       <c r="AB36" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC36" s="2">
         <v>0</v>
@@ -4982,7 +4973,7 @@
         <v>0</v>
       </c>
       <c r="AG36" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH36" s="2">
         <v>0</v>
@@ -5008,19 +4999,19 @@
         <v>56</v>
       </c>
       <c r="C37" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D37" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="E37" s="1">
         <v>44707</v>
       </c>
       <c r="F37" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G37" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H37" s="2"/>
       <c r="I37" s="2">
@@ -5081,7 +5072,7 @@
         <v>0</v>
       </c>
       <c r="AB37" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC37" s="2">
         <v>0</v>
@@ -5099,13 +5090,13 @@
         <v>0</v>
       </c>
       <c r="AH37" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI37" s="2">
         <v>0</v>
       </c>
       <c r="AJ37" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK37" s="2">
         <v>0</v>
@@ -5122,19 +5113,19 @@
         <v>57</v>
       </c>
       <c r="C38" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D38" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="E38" s="1">
         <v>44789</v>
       </c>
       <c r="F38" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G38" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H38" s="2"/>
       <c r="I38" s="2">
@@ -5165,7 +5156,7 @@
         <v>0</v>
       </c>
       <c r="R38" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S38" s="2">
         <v>0</v>
@@ -5210,7 +5201,7 @@
         <v>0</v>
       </c>
       <c r="AG38" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH38" s="2">
         <v>0</v>
@@ -5219,7 +5210,7 @@
         <v>0</v>
       </c>
       <c r="AJ38" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK38" s="2">
         <v>0</v>
@@ -5236,10 +5227,10 @@
         <v>58</v>
       </c>
       <c r="C39" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D39" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="E39" s="1">
         <v>44789</v>
@@ -5350,19 +5341,19 @@
         <v>59</v>
       </c>
       <c r="C40" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D40" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="E40" s="1">
         <v>44789</v>
       </c>
       <c r="F40" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G40" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H40" s="2"/>
       <c r="I40" s="2">
@@ -5393,7 +5384,7 @@
         <v>0</v>
       </c>
       <c r="R40" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S40" s="2">
         <v>0</v>
@@ -5438,7 +5429,7 @@
         <v>0</v>
       </c>
       <c r="AG40" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH40" s="2">
         <v>0</v>
@@ -5447,7 +5438,7 @@
         <v>0</v>
       </c>
       <c r="AJ40" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK40" s="2">
         <v>0</v>
@@ -5467,7 +5458,7 @@
         <v>166</v>
       </c>
       <c r="D41" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="E41" s="1">
         <v>44789</v>
@@ -5578,19 +5569,19 @@
         <v>61</v>
       </c>
       <c r="C42" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D42" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="E42" s="1">
         <v>44818</v>
       </c>
       <c r="F42" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G42" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H42" s="2"/>
       <c r="I42" s="2">
@@ -5600,10 +5591,10 @@
         <v>3</v>
       </c>
       <c r="K42" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L42" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M42" s="2">
         <v>0</v>
@@ -5651,7 +5642,7 @@
         <v>0</v>
       </c>
       <c r="AB42" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC42" s="2">
         <v>0</v>
@@ -5692,19 +5683,19 @@
         <v>62</v>
       </c>
       <c r="C43" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D43" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="E43" s="1">
         <v>44818</v>
       </c>
       <c r="F43" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G43" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H43" s="2"/>
       <c r="I43" s="2">
@@ -5720,10 +5711,10 @@
         <v>0</v>
       </c>
       <c r="M43" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N43" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O43" s="2">
         <v>0</v>
@@ -5806,19 +5797,19 @@
         <v>63</v>
       </c>
       <c r="C44" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="D44" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="E44" s="1">
         <v>44818</v>
       </c>
       <c r="F44" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G44" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H44" s="2"/>
       <c r="I44" s="2">
@@ -5879,7 +5870,7 @@
         <v>0</v>
       </c>
       <c r="AB44" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC44" s="2">
         <v>0</v>
@@ -5903,7 +5894,7 @@
         <v>0</v>
       </c>
       <c r="AJ44" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK44" s="2">
         <v>0</v>
@@ -5920,10 +5911,10 @@
         <v>64</v>
       </c>
       <c r="C45" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="D45" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="E45" s="1">
         <v>44818</v>
@@ -5975,7 +5966,7 @@
         <v>0</v>
       </c>
       <c r="V45" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W45" s="2">
         <v>0</v>
@@ -6034,19 +6025,19 @@
         <v>65</v>
       </c>
       <c r="C46" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="D46" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="E46" s="1">
         <v>44818</v>
       </c>
       <c r="F46" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G46" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H46" s="2"/>
       <c r="I46" s="2">
@@ -6107,7 +6098,7 @@
         <v>0</v>
       </c>
       <c r="AB46" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC46" s="2">
         <v>0</v>
@@ -6131,7 +6122,7 @@
         <v>0</v>
       </c>
       <c r="AJ46" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK46" s="2">
         <v>0</v>
@@ -6148,10 +6139,10 @@
         <v>66</v>
       </c>
       <c r="C47" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D47" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="E47" s="1">
         <v>44818</v>
@@ -6203,7 +6194,7 @@
         <v>0</v>
       </c>
       <c r="V47" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W47" s="2">
         <v>0</v>
@@ -6221,7 +6212,7 @@
         <v>0</v>
       </c>
       <c r="AB47" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC47" s="2">
         <v>0</v>
@@ -6245,7 +6236,7 @@
         <v>0</v>
       </c>
       <c r="AJ47" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK47" s="2">
         <v>0</v>
@@ -6262,10 +6253,10 @@
         <v>67</v>
       </c>
       <c r="C48" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D48" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="E48" s="1">
         <v>44818</v>
@@ -6335,7 +6326,7 @@
         <v>0</v>
       </c>
       <c r="AB48" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC48" s="2">
         <v>0</v>
@@ -6353,13 +6344,13 @@
         <v>0</v>
       </c>
       <c r="AH48" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI48" s="2">
         <v>0</v>
       </c>
       <c r="AJ48" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK48" s="2">
         <v>0</v>
@@ -6376,19 +6367,19 @@
         <v>68</v>
       </c>
       <c r="C49" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D49" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="E49" s="1">
         <v>44818</v>
       </c>
       <c r="F49" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G49" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H49" s="2"/>
       <c r="I49" s="2">
@@ -6398,10 +6389,10 @@
         <v>3</v>
       </c>
       <c r="K49" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L49" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M49" s="2">
         <v>0</v>
@@ -6449,7 +6440,7 @@
         <v>0</v>
       </c>
       <c r="AB49" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC49" s="2">
         <v>0</v>
@@ -6493,7 +6484,7 @@
         <v>170</v>
       </c>
       <c r="D50" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="E50" s="1">
         <v>44818</v>
@@ -6563,7 +6554,7 @@
         <v>0</v>
       </c>
       <c r="AB50" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC50" s="2">
         <v>0</v>
@@ -6581,13 +6572,13 @@
         <v>0</v>
       </c>
       <c r="AH50" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI50" s="2">
         <v>0</v>
       </c>
       <c r="AJ50" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK50" s="2">
         <v>0</v>
@@ -6604,19 +6595,19 @@
         <v>70</v>
       </c>
       <c r="C51" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D51" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="E51" s="1">
         <v>44818</v>
       </c>
       <c r="F51" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G51" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H51" s="2"/>
       <c r="I51" s="2">
@@ -6632,10 +6623,10 @@
         <v>0</v>
       </c>
       <c r="M51" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N51" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O51" s="2">
         <v>0</v>
@@ -6677,7 +6668,7 @@
         <v>0</v>
       </c>
       <c r="AB51" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC51" s="2">
         <v>0</v>
@@ -6701,7 +6692,7 @@
         <v>0</v>
       </c>
       <c r="AJ51" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK51" s="2">
         <v>0</v>
@@ -6718,10 +6709,10 @@
         <v>71</v>
       </c>
       <c r="C52" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D52" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="E52" s="1">
         <v>44818</v>
@@ -6815,7 +6806,7 @@
         <v>0</v>
       </c>
       <c r="AJ52" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK52" s="2">
         <v>0</v>
@@ -6832,10 +6823,10 @@
         <v>72</v>
       </c>
       <c r="C53" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D53" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="E53" s="1">
         <v>44818</v>
@@ -6946,10 +6937,10 @@
         <v>73</v>
       </c>
       <c r="C54" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D54" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="E54" s="1">
         <v>44818</v>
@@ -7060,10 +7051,10 @@
         <v>74</v>
       </c>
       <c r="C55" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D55" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="E55" s="1">
         <v>44818</v>
@@ -7133,7 +7124,7 @@
         <v>0</v>
       </c>
       <c r="AB55" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC55" s="2">
         <v>0</v>
@@ -7174,10 +7165,10 @@
         <v>75</v>
       </c>
       <c r="C56" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D56" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="E56" s="1">
         <v>44818</v>
@@ -7247,7 +7238,7 @@
         <v>0</v>
       </c>
       <c r="AB56" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC56" s="2">
         <v>0</v>
@@ -7271,7 +7262,7 @@
         <v>0</v>
       </c>
       <c r="AJ56" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK56" s="2">
         <v>0</v>
@@ -7288,19 +7279,19 @@
         <v>76</v>
       </c>
       <c r="C57" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D57" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="E57" s="1">
         <v>44771</v>
       </c>
       <c r="F57" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G57" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H57" s="2"/>
       <c r="I57" s="2">
@@ -7405,16 +7396,16 @@
         <v>172</v>
       </c>
       <c r="D58" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E58" s="1">
         <v>44771</v>
       </c>
       <c r="F58" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G58" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H58" s="2"/>
       <c r="I58" s="2">
@@ -7472,10 +7463,10 @@
         <v>0</v>
       </c>
       <c r="AA58" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB58" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC58" s="2">
         <v>0</v>
@@ -7499,7 +7490,7 @@
         <v>0</v>
       </c>
       <c r="AJ58" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK58" s="2">
         <v>0</v>
@@ -7519,16 +7510,16 @@
         <v>173</v>
       </c>
       <c r="D59" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E59" s="1">
         <v>44771</v>
       </c>
       <c r="F59" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G59" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H59" s="2"/>
       <c r="I59" s="2">
@@ -7562,7 +7553,7 @@
         <v>0</v>
       </c>
       <c r="S59" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T59" s="2">
         <v>0</v>
@@ -7613,7 +7604,7 @@
         <v>0</v>
       </c>
       <c r="AJ59" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK59" s="2">
         <v>0</v>
@@ -7633,7 +7624,7 @@
         <v>174</v>
       </c>
       <c r="D60" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E60" s="1">
         <v>44771</v>
@@ -7652,10 +7643,10 @@
         <v>11</v>
       </c>
       <c r="K60" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L60" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M60" s="2">
         <v>0</v>
@@ -7747,7 +7738,7 @@
         <v>175</v>
       </c>
       <c r="D61" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="E61" s="1">
         <v>44771</v>
@@ -7832,7 +7823,7 @@
         <v>0</v>
       </c>
       <c r="AG61" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH61" s="2">
         <v>0</v>
@@ -7841,7 +7832,7 @@
         <v>0</v>
       </c>
       <c r="AJ61" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK61" s="2">
         <v>0</v>
@@ -7861,7 +7852,7 @@
         <v>176</v>
       </c>
       <c r="D62" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="E62" s="1">
         <v>44771</v>
@@ -7931,7 +7922,7 @@
         <v>0</v>
       </c>
       <c r="AB62" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC62" s="2">
         <v>0</v>
@@ -7946,7 +7937,7 @@
         <v>0</v>
       </c>
       <c r="AG62" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH62" s="2">
         <v>0</v>
@@ -7975,7 +7966,7 @@
         <v>177</v>
       </c>
       <c r="D63" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="E63" s="1">
         <v>44771</v>
@@ -8042,10 +8033,10 @@
         <v>0</v>
       </c>
       <c r="AA63" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB63" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC63" s="2">
         <v>0</v>
@@ -8060,7 +8051,7 @@
         <v>0</v>
       </c>
       <c r="AG63" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH63" s="2">
         <v>0</v>
@@ -8089,7 +8080,7 @@
         <v>178</v>
       </c>
       <c r="D64" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E64" s="1">
         <v>44771</v>
@@ -8159,7 +8150,7 @@
         <v>0</v>
       </c>
       <c r="AB64" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC64" s="2">
         <v>0</v>
@@ -8174,7 +8165,7 @@
         <v>0</v>
       </c>
       <c r="AG64" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH64" s="2">
         <v>0</v>
@@ -8203,7 +8194,7 @@
         <v>179</v>
       </c>
       <c r="D65" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="E65" s="1">
         <v>44771</v>
@@ -8240,7 +8231,7 @@
         <v>0</v>
       </c>
       <c r="Q65" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R65" s="2">
         <v>0</v>
@@ -8273,7 +8264,7 @@
         <v>0</v>
       </c>
       <c r="AB65" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC65" s="2">
         <v>0</v>
@@ -8291,7 +8282,7 @@
         <v>0</v>
       </c>
       <c r="AH65" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI65" s="2">
         <v>0</v>
@@ -8317,7 +8308,7 @@
         <v>180</v>
       </c>
       <c r="D66" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="E66" s="1">
         <v>44771</v>
@@ -8336,10 +8327,10 @@
         <v>11</v>
       </c>
       <c r="K66" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L66" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M66" s="2">
         <v>0</v>
@@ -8387,7 +8378,7 @@
         <v>0</v>
       </c>
       <c r="AB66" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC66" s="2">
         <v>0</v>
@@ -8431,7 +8422,7 @@
         <v>181</v>
       </c>
       <c r="D67" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="E67" s="1">
         <v>44771</v>
@@ -8516,7 +8507,7 @@
         <v>0</v>
       </c>
       <c r="AG67" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH67" s="2">
         <v>0</v>
@@ -8525,7 +8516,7 @@
         <v>0</v>
       </c>
       <c r="AJ67" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK67" s="2">
         <v>0</v>
@@ -8545,7 +8536,7 @@
         <v>182</v>
       </c>
       <c r="D68" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E68" s="1">
         <v>44771</v>
@@ -8588,7 +8579,7 @@
         <v>0</v>
       </c>
       <c r="S68" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T68" s="2">
         <v>0</v>
@@ -8659,16 +8650,16 @@
         <v>183</v>
       </c>
       <c r="D69" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E69" s="1">
         <v>44771</v>
       </c>
       <c r="F69" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G69" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H69" s="2"/>
       <c r="I69" s="2">
@@ -8729,7 +8720,7 @@
         <v>0</v>
       </c>
       <c r="AB69" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC69" s="2">
         <v>0</v>
@@ -8744,7 +8735,7 @@
         <v>0</v>
       </c>
       <c r="AG69" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH69" s="2">
         <v>0</v>
@@ -8770,19 +8761,19 @@
         <v>89</v>
       </c>
       <c r="C70" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D70" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E70" s="1">
         <v>44771</v>
       </c>
       <c r="F70" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G70" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H70" s="2"/>
       <c r="I70" s="2">
@@ -8810,7 +8801,7 @@
         <v>0</v>
       </c>
       <c r="Q70" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R70" s="2">
         <v>0</v>
@@ -8840,10 +8831,10 @@
         <v>0</v>
       </c>
       <c r="AA70" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB70" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC70" s="2">
         <v>0</v>
@@ -8884,19 +8875,19 @@
         <v>90</v>
       </c>
       <c r="C71" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D71" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E71" s="1">
         <v>44771</v>
       </c>
       <c r="F71" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G71" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H71" s="2"/>
       <c r="I71" s="2">
@@ -8954,7 +8945,7 @@
         <v>0</v>
       </c>
       <c r="AA71" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB71" s="2">
         <v>1</v>
@@ -8975,7 +8966,7 @@
         <v>0</v>
       </c>
       <c r="AH71" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI71" s="2">
         <v>0</v>
@@ -8998,10 +8989,10 @@
         <v>91</v>
       </c>
       <c r="C72" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D72" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E72" s="1">
         <v>44845</v>
@@ -9112,19 +9103,19 @@
         <v>92</v>
       </c>
       <c r="C73" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D73" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E73" s="1">
         <v>44845</v>
       </c>
       <c r="F73" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G73" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H73" s="2"/>
       <c r="I73" s="2">
@@ -9226,19 +9217,19 @@
         <v>93</v>
       </c>
       <c r="C74" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D74" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E74" s="1">
         <v>44845</v>
       </c>
       <c r="F74" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G74" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H74" s="2"/>
       <c r="I74" s="2">
@@ -9340,10 +9331,10 @@
         <v>94</v>
       </c>
       <c r="C75" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D75" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E75" s="1">
         <v>44803</v>
@@ -9454,10 +9445,10 @@
         <v>95</v>
       </c>
       <c r="C76" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D76" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E76" s="1">
         <v>44840</v>
@@ -9568,10 +9559,10 @@
         <v>96</v>
       </c>
       <c r="C77" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D77" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E77" s="1">
         <v>44840</v>
@@ -9596,10 +9587,10 @@
         <v>0</v>
       </c>
       <c r="M77" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N77" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O77" s="2">
         <v>0</v>
@@ -9641,7 +9632,7 @@
         <v>0</v>
       </c>
       <c r="AB77" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC77" s="2">
         <v>0</v>
@@ -9665,7 +9656,7 @@
         <v>0</v>
       </c>
       <c r="AJ77" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK77" s="2">
         <v>0</v>
@@ -9682,10 +9673,10 @@
         <v>97</v>
       </c>
       <c r="C78" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D78" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E78" s="1">
         <v>44840</v>
@@ -9704,10 +9695,10 @@
         <v>6</v>
       </c>
       <c r="K78" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L78" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M78" s="2">
         <v>0</v>
@@ -9755,7 +9746,7 @@
         <v>0</v>
       </c>
       <c r="AB78" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC78" s="2">
         <v>0</v>
@@ -9779,7 +9770,7 @@
         <v>0</v>
       </c>
       <c r="AJ78" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK78" s="2">
         <v>0</v>
@@ -9796,10 +9787,10 @@
         <v>98</v>
       </c>
       <c r="C79" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D79" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E79" s="1">
         <v>44840</v>
@@ -9869,7 +9860,7 @@
         <v>0</v>
       </c>
       <c r="AB79" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC79" s="2">
         <v>0</v>
@@ -9910,10 +9901,10 @@
         <v>99</v>
       </c>
       <c r="C80" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D80" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E80" s="1">
         <v>44840</v>
@@ -9932,16 +9923,16 @@
         <v>6</v>
       </c>
       <c r="K80" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L80" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M80" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N80" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O80" s="2">
         <v>0</v>
@@ -9983,7 +9974,7 @@
         <v>0</v>
       </c>
       <c r="AB80" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC80" s="2">
         <v>0</v>
@@ -10007,7 +9998,7 @@
         <v>0</v>
       </c>
       <c r="AJ80" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK80" s="2">
         <v>0</v>
@@ -10024,10 +10015,10 @@
         <v>100</v>
       </c>
       <c r="C81" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D81" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E81" s="1">
         <v>44840</v>
@@ -10121,7 +10112,7 @@
         <v>0</v>
       </c>
       <c r="AJ81" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK81" s="2">
         <v>0</v>
@@ -10138,10 +10129,10 @@
         <v>101</v>
       </c>
       <c r="C82" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D82" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E82" s="1">
         <v>44894</v>
@@ -10252,10 +10243,10 @@
         <v>102</v>
       </c>
       <c r="C83" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D83" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E83" s="1">
         <v>44894</v>
@@ -10369,16 +10360,16 @@
         <v>196</v>
       </c>
       <c r="D84" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E84" s="1">
         <v>44894</v>
       </c>
       <c r="F84" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G84" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H84" s="2"/>
       <c r="I84" s="2">
@@ -10439,7 +10430,7 @@
         <v>0</v>
       </c>
       <c r="AB84" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC84" s="2">
         <v>0</v>
@@ -10483,16 +10474,16 @@
         <v>197</v>
       </c>
       <c r="D85" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E85" s="1">
         <v>44894</v>
       </c>
       <c r="F85" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G85" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H85" s="2"/>
       <c r="I85" s="2">
@@ -10577,10 +10568,10 @@
         <v>0</v>
       </c>
       <c r="AJ85" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK85" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL85" s="2">
         <v>0</v>
@@ -10597,7 +10588,7 @@
         <v>198</v>
       </c>
       <c r="D86" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E86" s="1">
         <v>44894</v>
@@ -10711,16 +10702,16 @@
         <v>199</v>
       </c>
       <c r="D87" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E87" s="1">
         <v>44894</v>
       </c>
       <c r="F87" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G87" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H87" s="2"/>
       <c r="I87" s="2">
@@ -10781,7 +10772,7 @@
         <v>0</v>
       </c>
       <c r="AB87" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC87" s="2">
         <v>0</v>
@@ -10822,10 +10813,10 @@
         <v>107</v>
       </c>
       <c r="C88" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D88" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E88" s="1">
         <v>44894</v>
@@ -10853,10 +10844,10 @@
         <v>0</v>
       </c>
       <c r="N88" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O88" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P88" s="2">
         <v>0</v>
@@ -10922,7 +10913,7 @@
         <v>1</v>
       </c>
       <c r="AK88" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL88" s="2">
         <v>0</v>
@@ -10939,16 +10930,16 @@
         <v>200</v>
       </c>
       <c r="D89" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E89" s="1">
         <v>44894</v>
       </c>
       <c r="F89" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G89" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H89" s="2"/>
       <c r="I89" s="2">
@@ -10967,10 +10958,10 @@
         <v>0</v>
       </c>
       <c r="N89" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O89" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P89" s="2">
         <v>0</v>
@@ -11053,7 +11044,7 @@
         <v>201</v>
       </c>
       <c r="D90" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E90" s="1">
         <v>44894</v>
@@ -11147,7 +11138,7 @@
         <v>0</v>
       </c>
       <c r="AJ90" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK90" s="2">
         <v>0</v>
@@ -11167,16 +11158,16 @@
         <v>202</v>
       </c>
       <c r="D91" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E91" s="1">
         <v>44865</v>
       </c>
       <c r="F91" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G91" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H91" s="2"/>
       <c r="I91" s="2">
@@ -11207,7 +11198,7 @@
         <v>0</v>
       </c>
       <c r="R91" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S91" s="2">
         <v>0</v>
@@ -11281,16 +11272,16 @@
         <v>203</v>
       </c>
       <c r="D92" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E92" s="1">
         <v>44865</v>
       </c>
       <c r="F92" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G92" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H92" s="2"/>
       <c r="I92" s="2">
@@ -11351,7 +11342,7 @@
         <v>0</v>
       </c>
       <c r="AB92" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC92" s="2">
         <v>0</v>
@@ -11395,7 +11386,7 @@
         <v>204</v>
       </c>
       <c r="D93" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E93" s="1">
         <v>44865</v>
@@ -11414,10 +11405,10 @@
         <v>5</v>
       </c>
       <c r="K93" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L93" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M93" s="2">
         <v>0</v>
@@ -11465,7 +11456,7 @@
         <v>0</v>
       </c>
       <c r="AB93" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC93" s="2">
         <v>0</v>
@@ -11509,7 +11500,7 @@
         <v>205</v>
       </c>
       <c r="D94" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E94" s="1">
         <v>44865</v>
@@ -11528,10 +11519,10 @@
         <v>5</v>
       </c>
       <c r="K94" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L94" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M94" s="2">
         <v>0</v>
@@ -11579,7 +11570,7 @@
         <v>0</v>
       </c>
       <c r="AB94" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC94" s="2">
         <v>0</v>
@@ -11594,7 +11585,7 @@
         <v>0</v>
       </c>
       <c r="AG94" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH94" s="2">
         <v>0</v>
@@ -11623,16 +11614,16 @@
         <v>206</v>
       </c>
       <c r="D95" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E95" s="1">
         <v>44865</v>
       </c>
       <c r="F95" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G95" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H95" s="2"/>
       <c r="I95" s="2">
@@ -11663,7 +11654,7 @@
         <v>0</v>
       </c>
       <c r="R95" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S95" s="2">
         <v>0</v>
@@ -11708,7 +11699,7 @@
         <v>0</v>
       </c>
       <c r="AG95" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH95" s="2">
         <v>0</v>
@@ -11734,19 +11725,19 @@
         <v>115</v>
       </c>
       <c r="C96" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D96" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E96" s="1">
         <v>44865</v>
       </c>
       <c r="F96" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G96" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H96" s="2"/>
       <c r="I96" s="2">
@@ -11848,19 +11839,19 @@
         <v>116</v>
       </c>
       <c r="C97" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D97" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E97" s="1">
         <v>44865</v>
       </c>
       <c r="F97" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G97" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H97" s="2"/>
       <c r="I97" s="2">
@@ -11936,7 +11927,7 @@
         <v>0</v>
       </c>
       <c r="AG97" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH97" s="2">
         <v>0</v>
@@ -11965,7 +11956,7 @@
         <v>208</v>
       </c>
       <c r="D98" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E98" s="1">
         <v>44865</v>
@@ -12035,7 +12026,7 @@
         <v>0</v>
       </c>
       <c r="AB98" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC98" s="2">
         <v>0</v>
@@ -12050,7 +12041,7 @@
         <v>0</v>
       </c>
       <c r="AG98" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH98" s="2">
         <v>0</v>
@@ -12076,19 +12067,19 @@
         <v>118</v>
       </c>
       <c r="C99" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D99" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E99" s="1">
         <v>44865</v>
       </c>
       <c r="F99" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G99" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H99" s="2"/>
       <c r="I99" s="2">
@@ -12190,19 +12181,19 @@
         <v>119</v>
       </c>
       <c r="C100" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D100" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E100" s="1">
         <v>44879</v>
       </c>
       <c r="F100" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G100" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H100" s="2"/>
       <c r="I100" s="2">
@@ -12245,7 +12236,7 @@
         <v>0</v>
       </c>
       <c r="V100" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W100" s="2">
         <v>0</v>
@@ -12263,7 +12254,7 @@
         <v>0</v>
       </c>
       <c r="AB100" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC100" s="2">
         <v>0</v>
@@ -12304,19 +12295,19 @@
         <v>120</v>
       </c>
       <c r="C101" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D101" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E101" s="1">
         <v>44879</v>
       </c>
       <c r="F101" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G101" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H101" s="2"/>
       <c r="I101" s="2">
@@ -12359,7 +12350,7 @@
         <v>0</v>
       </c>
       <c r="V101" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W101" s="2">
         <v>0</v>
@@ -12377,7 +12368,7 @@
         <v>0</v>
       </c>
       <c r="AB101" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC101" s="2">
         <v>0</v>
@@ -12401,7 +12392,7 @@
         <v>0</v>
       </c>
       <c r="AJ101" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK101" s="2">
         <v>0</v>
@@ -12418,10 +12409,10 @@
         <v>121</v>
       </c>
       <c r="C102" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D102" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E102" s="1">
         <v>44879</v>
@@ -12535,16 +12526,16 @@
         <v>211</v>
       </c>
       <c r="D103" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E103" s="1">
         <v>44879</v>
       </c>
       <c r="F103" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G103" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H103" s="2"/>
       <c r="I103" s="2">
@@ -12629,7 +12620,7 @@
         <v>0</v>
       </c>
       <c r="AJ103" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK103" s="2">
         <v>0</v>
@@ -12649,16 +12640,16 @@
         <v>212</v>
       </c>
       <c r="D104" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E104" s="1">
         <v>44879</v>
       </c>
       <c r="F104" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G104" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H104" s="2"/>
       <c r="I104" s="2">
@@ -12760,19 +12751,19 @@
         <v>124</v>
       </c>
       <c r="C105" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D105" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E105" s="1">
         <v>44879</v>
       </c>
       <c r="F105" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G105" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H105" s="2"/>
       <c r="I105" s="2">
@@ -12782,10 +12773,10 @@
         <v>3</v>
       </c>
       <c r="K105" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L105" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M105" s="2">
         <v>0</v>
@@ -12800,7 +12791,7 @@
         <v>0</v>
       </c>
       <c r="Q105" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R105" s="2">
         <v>0</v>
@@ -12833,7 +12824,7 @@
         <v>0</v>
       </c>
       <c r="AB105" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC105" s="2">
         <v>0</v>
@@ -12874,19 +12865,19 @@
         <v>125</v>
       </c>
       <c r="C106" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D106" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E106" s="1">
         <v>44879</v>
       </c>
       <c r="F106" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G106" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H106" s="2"/>
       <c r="I106" s="2">
@@ -12896,10 +12887,10 @@
         <v>3</v>
       </c>
       <c r="K106" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L106" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M106" s="2">
         <v>0</v>
@@ -12914,7 +12905,7 @@
         <v>0</v>
       </c>
       <c r="Q106" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R106" s="2">
         <v>0</v>
@@ -12947,7 +12938,7 @@
         <v>0</v>
       </c>
       <c r="AB106" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC106" s="2">
         <v>0</v>
@@ -12988,19 +12979,19 @@
         <v>125</v>
       </c>
       <c r="C107" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D107" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E107" s="1">
         <v>44893</v>
       </c>
       <c r="F107" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G107" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H107" s="2"/>
       <c r="I107" s="2">
@@ -13013,7 +13004,7 @@
         <v>0</v>
       </c>
       <c r="L107" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M107" s="2">
         <v>0</v>
@@ -13025,10 +13016,10 @@
         <v>0</v>
       </c>
       <c r="P107" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q107" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R107" s="2">
         <v>0</v>
@@ -13061,7 +13052,7 @@
         <v>0</v>
       </c>
       <c r="AB107" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC107" s="2">
         <v>0</v>
@@ -13102,19 +13093,19 @@
         <v>126</v>
       </c>
       <c r="C108" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D108" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E108" s="1">
         <v>44893</v>
       </c>
       <c r="F108" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G108" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H108" s="2"/>
       <c r="I108" s="2">
@@ -13127,7 +13118,7 @@
         <v>0</v>
       </c>
       <c r="L108" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M108" s="2">
         <v>0</v>
@@ -13139,10 +13130,10 @@
         <v>0</v>
       </c>
       <c r="P108" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q108" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R108" s="2">
         <v>0</v>
@@ -13175,7 +13166,7 @@
         <v>0</v>
       </c>
       <c r="AB108" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC108" s="2">
         <v>0</v>
@@ -13216,10 +13207,10 @@
         <v>127</v>
       </c>
       <c r="C109" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D109" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E109" s="1">
         <v>44887</v>
@@ -13330,10 +13321,10 @@
         <v>128</v>
       </c>
       <c r="C110" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D110" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E110" s="1">
         <v>44887</v>
@@ -13444,10 +13435,10 @@
         <v>129</v>
       </c>
       <c r="C111" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D111" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E111" s="1">
         <v>44887</v>
@@ -13529,10 +13520,10 @@
         <v>0</v>
       </c>
       <c r="AF111" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG111" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH111" s="2">
         <v>0</v>
@@ -13558,19 +13549,19 @@
         <v>130</v>
       </c>
       <c r="C112" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D112" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E112" s="1">
         <v>44887</v>
       </c>
       <c r="F112" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G112" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H112" s="2"/>
       <c r="I112" s="2">
@@ -13643,10 +13634,10 @@
         <v>0</v>
       </c>
       <c r="AF112" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG112" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH112" s="2">
         <v>0</v>
@@ -13672,19 +13663,19 @@
         <v>131</v>
       </c>
       <c r="C113" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D113" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E113" s="1">
         <v>44887</v>
       </c>
       <c r="F113" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G113" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H113" s="2"/>
       <c r="I113" s="2">
@@ -13786,10 +13777,10 @@
         <v>132</v>
       </c>
       <c r="C114" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D114" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E114" s="1">
         <v>44896</v>
@@ -13900,10 +13891,10 @@
         <v>133</v>
       </c>
       <c r="C115" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D115" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E115" s="1">
         <v>44714</v>
@@ -14016,10 +14007,10 @@
         <v>133</v>
       </c>
       <c r="C116" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D116" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="E116" s="1">
         <v>44714</v>

</xml_diff>

<commit_message>
update codebook and demo datasets
</commit_message>
<xml_diff>
--- a/datasets/lab_detail.xlsx
+++ b/datasets/lab_detail.xlsx
@@ -81,10 +81,16 @@
     <t>substance</t>
   </si>
   <si>
-    <t>p-fluorofentanyl</t>
+    <t>despropionyl p-fluorofentanyl</t>
   </si>
   <si>
     <t>xylazine</t>
+  </si>
+  <si>
+    <t>fentanyl</t>
+  </si>
+  <si>
+    <t>dimethyl sulfone (methylsulfonylmethane MSM)</t>
   </si>
   <si>
     <t>phenethyl 4-ANPP</t>
@@ -93,19 +99,16 @@
     <t>4-ANPP</t>
   </si>
   <si>
-    <t>dimethyl sulfone (methylsulfonylmethane MSM)</t>
+    <t>p-fluorofentanyl</t>
   </si>
   <si>
-    <t>despropionyl p-fluorofentanyl</t>
-  </si>
-  <si>
-    <t>fentanyl</t>
+    <t>3,4-methylenedioxy-N-benzylcathinone (BMDP)</t>
   </si>
   <si>
     <t>3,4-MDMA</t>
   </si>
   <si>
-    <t>3,4-methylenedioxy-N-benzylcathinone (BMDP)</t>
+    <t>levamisole</t>
   </si>
   <si>
     <t>tropacocaine</t>
@@ -114,37 +117,34 @@
     <t>phenacetin</t>
   </si>
   <si>
-    <t>norcocaine</t>
-  </si>
-  <si>
-    <t>levamisole</t>
-  </si>
-  <si>
-    <t>cocaine</t>
-  </si>
-  <si>
     <t>benzoylecgonine (BZ)</t>
   </si>
   <si>
     <t>methyl ecgonidine (MED)</t>
   </si>
   <si>
-    <t>tramadol</t>
+    <t>cocaine</t>
+  </si>
+  <si>
+    <t>norcocaine</t>
+  </si>
+  <si>
+    <t>methamphetamine</t>
   </si>
   <si>
     <t>p-fluoro phenethyl 4-ANPP</t>
   </si>
   <si>
+    <t>tramadol</t>
+  </si>
+  <si>
     <t>non-specific sugars</t>
   </si>
   <si>
-    <t>methamphetamine</t>
+    <t>caffeine</t>
   </si>
   <si>
     <t>eutylone</t>
-  </si>
-  <si>
-    <t>caffeine</t>
   </si>
   <si>
     <t>urea</t>
@@ -153,43 +153,43 @@
     <t>heroin</t>
   </si>
   <si>
+    <t>6-monoacetylmorphine (6-MAM)</t>
+  </si>
+  <si>
     <t>acetylcodeine</t>
   </si>
   <si>
-    <t>6-monoacetylmorphine (6-MAM)</t>
+    <t>1,3-Diacetin</t>
+  </si>
+  <si>
+    <t>N-ethyl-4-ANPP</t>
   </si>
   <si>
     <t>N-phenylpropanamide</t>
   </si>
   <si>
+    <t>acetaminophen</t>
+  </si>
+  <si>
     <t>lidocaine</t>
   </si>
   <si>
-    <t>N-ethyl-4-ANPP</t>
-  </si>
-  <si>
-    <t>acetaminophen</t>
-  </si>
-  <si>
-    <t>1,3-Diacetin</t>
+    <t>diphenhydramine</t>
   </si>
   <si>
     <t>gabapentin</t>
   </si>
   <si>
+    <t>methadone</t>
+  </si>
+  <si>
     <t>inositol</t>
   </si>
   <si>
-    <t>methadone</t>
+    <t>quinine</t>
   </si>
   <si>
     <t>N-piperidinyl etonitazene</t>
-  </si>
-  <si>
-    <t>diphenhydramine</t>
-  </si>
-  <si>
-    <t>quinine</t>
   </si>
   <si>
     <t>metonitazene</t>
@@ -201,16 +201,16 @@
     <t>procaine</t>
   </si>
   <si>
-    <t>phenethyl chloride</t>
+    <t>nicotine</t>
+  </si>
+  <si>
+    <t>phenethylbromide</t>
   </si>
   <si>
     <t>menthol</t>
   </si>
   <si>
-    <t>nicotine</t>
-  </si>
-  <si>
-    <t>phenethylbromide</t>
+    <t>phenethyl chloride</t>
   </si>
   <si>
     <t>1-phenethyl-4-propionyloxypiperidine</t>
@@ -614,7 +614,7 @@
         <v>0</v>
       </c>
       <c r="AK2" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL2" s="2">
         <v>0</v>
@@ -764,10 +764,10 @@
         <v>7</v>
       </c>
       <c r="K4" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M4" s="2">
         <v>0</v>
@@ -815,7 +815,7 @@
         <v>0</v>
       </c>
       <c r="AB4" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC4" s="2">
         <v>0</v>
@@ -839,7 +839,7 @@
         <v>0</v>
       </c>
       <c r="AJ4" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK4" s="2">
         <v>0</v>
@@ -953,7 +953,7 @@
         <v>0</v>
       </c>
       <c r="AJ5" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK5" s="2">
         <v>0</v>
@@ -1067,7 +1067,7 @@
         <v>0</v>
       </c>
       <c r="AJ6" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK6" s="2">
         <v>0</v>
@@ -1157,7 +1157,7 @@
         <v>0</v>
       </c>
       <c r="AB7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC7" s="2">
         <v>0</v>
@@ -1181,10 +1181,10 @@
         <v>0</v>
       </c>
       <c r="AJ7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL7" s="2">
         <v>0</v>
@@ -1220,10 +1220,10 @@
         <v>7</v>
       </c>
       <c r="K8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M8" s="2">
         <v>0</v>
@@ -1312,7 +1312,7 @@
         <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D9" t="s">
         <v>73</v>
@@ -1321,10 +1321,10 @@
         <v>44777</v>
       </c>
       <c r="F9" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2">
@@ -1364,7 +1364,7 @@
         <v>0</v>
       </c>
       <c r="U9" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V9" s="2">
         <v>0</v>
@@ -1426,7 +1426,7 @@
         <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D10" t="s">
         <v>73</v>
@@ -1435,10 +1435,10 @@
         <v>44777</v>
       </c>
       <c r="F10" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2">
@@ -1478,7 +1478,7 @@
         <v>0</v>
       </c>
       <c r="U10" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V10" s="2">
         <v>0</v>
@@ -1537,7 +1537,7 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
         <v>70</v>
@@ -1703,7 +1703,7 @@
         <v>0</v>
       </c>
       <c r="T12" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U12" s="2">
         <v>0</v>
@@ -1739,7 +1739,7 @@
         <v>0</v>
       </c>
       <c r="AF12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG12" s="2">
         <v>1</v>
@@ -1771,7 +1771,7 @@
         <v>71</v>
       </c>
       <c r="D13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E13" s="1">
         <v>44714</v>
@@ -1853,7 +1853,7 @@
         <v>0</v>
       </c>
       <c r="AF13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG13" s="2">
         <v>1</v>
@@ -1885,7 +1885,7 @@
         <v>71</v>
       </c>
       <c r="D14" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E14" s="1">
         <v>44714</v>
@@ -1967,10 +1967,10 @@
         <v>0</v>
       </c>
       <c r="AF14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH14" s="2">
         <v>0</v>
@@ -1999,7 +1999,7 @@
         <v>71</v>
       </c>
       <c r="D15" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E15" s="1">
         <v>44714</v>
@@ -2045,7 +2045,7 @@
         <v>0</v>
       </c>
       <c r="T15" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U15" s="2">
         <v>0</v>
@@ -2084,7 +2084,7 @@
         <v>0</v>
       </c>
       <c r="AG15" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH15" s="2">
         <v>0</v>
@@ -2110,7 +2110,7 @@
         <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D16" t="s">
         <v>73</v>
@@ -2119,10 +2119,10 @@
         <v>44714</v>
       </c>
       <c r="F16" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2">
@@ -2224,19 +2224,19 @@
         <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E17" s="1">
         <v>44714</v>
       </c>
       <c r="F17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2">
@@ -2423,7 +2423,7 @@
         <v>0</v>
       </c>
       <c r="AF18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG18" s="2">
         <v>0</v>
@@ -2449,22 +2449,22 @@
         <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D19" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E19" s="1">
         <v>44759</v>
       </c>
       <c r="F19" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2">
@@ -2474,10 +2474,10 @@
         <v>4</v>
       </c>
       <c r="K19" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L19" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M19" s="2">
         <v>0</v>
@@ -2492,7 +2492,7 @@
         <v>0</v>
       </c>
       <c r="Q19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R19" s="2">
         <v>0</v>
@@ -2525,7 +2525,7 @@
         <v>0</v>
       </c>
       <c r="AB19" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC19" s="2">
         <v>0</v>
@@ -2563,10 +2563,10 @@
         <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D20" t="s">
         <v>73</v>
@@ -2575,10 +2575,10 @@
         <v>44759</v>
       </c>
       <c r="F20" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2">
@@ -2666,7 +2666,7 @@
         <v>1</v>
       </c>
       <c r="AK20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL20" s="2">
         <v>0</v>
@@ -2677,7 +2677,7 @@
         <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C21" t="s">
         <v>70</v>
@@ -2791,10 +2791,10 @@
         <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D22" t="s">
         <v>73</v>
@@ -2803,10 +2803,10 @@
         <v>44759</v>
       </c>
       <c r="F22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="2">
@@ -2816,10 +2816,10 @@
         <v>4</v>
       </c>
       <c r="K22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M22" s="2">
         <v>0</v>
@@ -2849,7 +2849,7 @@
         <v>0</v>
       </c>
       <c r="V22" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W22" s="2">
         <v>0</v>
@@ -2905,10 +2905,10 @@
         <v>5</v>
       </c>
       <c r="B23" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="C23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D23" t="s">
         <v>73</v>
@@ -2917,10 +2917,10 @@
         <v>44759</v>
       </c>
       <c r="F23" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2">
@@ -3008,7 +3008,7 @@
         <v>1</v>
       </c>
       <c r="AK23" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL23" s="2">
         <v>0</v>
@@ -3022,19 +3022,19 @@
         <v>40</v>
       </c>
       <c r="C24" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E24" s="1">
         <v>44759</v>
       </c>
       <c r="F24" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G24" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2">
@@ -3077,7 +3077,7 @@
         <v>0</v>
       </c>
       <c r="V24" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W24" s="2">
         <v>0</v>
@@ -3095,7 +3095,7 @@
         <v>0</v>
       </c>
       <c r="AB24" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC24" s="2">
         <v>0</v>
@@ -3110,7 +3110,7 @@
         <v>0</v>
       </c>
       <c r="AG24" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH24" s="2">
         <v>0</v>
@@ -3136,7 +3136,7 @@
         <v>41</v>
       </c>
       <c r="C25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D25" t="s">
         <v>74</v>
@@ -3145,10 +3145,10 @@
         <v>44759</v>
       </c>
       <c r="F25" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H25" s="2"/>
       <c r="I25" s="2">
@@ -3176,7 +3176,7 @@
         <v>0</v>
       </c>
       <c r="Q25" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R25" s="2">
         <v>0</v>
@@ -3224,7 +3224,7 @@
         <v>0</v>
       </c>
       <c r="AG25" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH25" s="2">
         <v>0</v>
@@ -3247,7 +3247,7 @@
         <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C26" t="s">
         <v>71</v>
@@ -3290,7 +3290,7 @@
         <v>0</v>
       </c>
       <c r="Q26" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R26" s="2">
         <v>0</v>
@@ -3353,7 +3353,7 @@
         <v>0</v>
       </c>
       <c r="AL26" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -3361,7 +3361,7 @@
         <v>6</v>
       </c>
       <c r="B27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C27" t="s">
         <v>70</v>
@@ -3475,7 +3475,7 @@
         <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C28" t="s">
         <v>71</v>
@@ -3518,7 +3518,7 @@
         <v>0</v>
       </c>
       <c r="Q28" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R28" s="2">
         <v>0</v>
@@ -3581,7 +3581,7 @@
         <v>0</v>
       </c>
       <c r="AL28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
@@ -3703,22 +3703,22 @@
         <v>7</v>
       </c>
       <c r="B30" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="C30" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D30" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E30" s="1">
         <v>44707</v>
       </c>
       <c r="F30" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G30" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H30" s="2"/>
       <c r="I30" s="2">
@@ -3779,7 +3779,7 @@
         <v>0</v>
       </c>
       <c r="AB30" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC30" s="2">
         <v>0</v>
@@ -3803,7 +3803,7 @@
         <v>0</v>
       </c>
       <c r="AJ30" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK30" s="2">
         <v>0</v>
@@ -3817,22 +3817,22 @@
         <v>7</v>
       </c>
       <c r="B31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E31" s="1">
         <v>44707</v>
       </c>
       <c r="F31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G31" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H31" s="2"/>
       <c r="I31" s="2">
@@ -3848,10 +3848,10 @@
         <v>0</v>
       </c>
       <c r="M31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O31" s="2">
         <v>0</v>
@@ -3931,10 +3931,10 @@
         <v>7</v>
       </c>
       <c r="B32" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="C32" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D32" t="s">
         <v>73</v>
@@ -3943,10 +3943,10 @@
         <v>44707</v>
       </c>
       <c r="F32" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G32" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H32" s="2"/>
       <c r="I32" s="2">
@@ -4007,7 +4007,7 @@
         <v>0</v>
       </c>
       <c r="AB32" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC32" s="2">
         <v>0</v>
@@ -4031,7 +4031,7 @@
         <v>0</v>
       </c>
       <c r="AJ32" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK32" s="2">
         <v>0</v>
@@ -4045,10 +4045,10 @@
         <v>7</v>
       </c>
       <c r="B33" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C33" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D33" t="s">
         <v>73</v>
@@ -4057,10 +4057,10 @@
         <v>44707</v>
       </c>
       <c r="F33" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G33" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H33" s="2"/>
       <c r="I33" s="2">
@@ -4076,10 +4076,10 @@
         <v>0</v>
       </c>
       <c r="M33" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N33" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O33" s="2">
         <v>0</v>
@@ -4159,13 +4159,13 @@
         <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C34" t="s">
         <v>70</v>
       </c>
       <c r="D34" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E34" s="1">
         <v>44707</v>
@@ -4235,7 +4235,7 @@
         <v>0</v>
       </c>
       <c r="AB34" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC34" s="2">
         <v>0</v>
@@ -4250,10 +4250,10 @@
         <v>0</v>
       </c>
       <c r="AG34" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH34" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI34" s="2">
         <v>0</v>
@@ -4273,10 +4273,10 @@
         <v>7</v>
       </c>
       <c r="B35" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C35" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D35" t="s">
         <v>73</v>
@@ -4285,10 +4285,10 @@
         <v>44707</v>
       </c>
       <c r="F35" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G35" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H35" s="2"/>
       <c r="I35" s="2">
@@ -4298,10 +4298,10 @@
         <v>5</v>
       </c>
       <c r="K35" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L35" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M35" s="2">
         <v>0</v>
@@ -4387,13 +4387,13 @@
         <v>7</v>
       </c>
       <c r="B36" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="C36" t="s">
         <v>70</v>
       </c>
       <c r="D36" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E36" s="1">
         <v>44707</v>
@@ -4412,10 +4412,10 @@
         <v>5</v>
       </c>
       <c r="K36" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L36" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M36" s="2">
         <v>0</v>
@@ -4463,7 +4463,7 @@
         <v>0</v>
       </c>
       <c r="AB36" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC36" s="2">
         <v>0</v>
@@ -4478,7 +4478,7 @@
         <v>0</v>
       </c>
       <c r="AG36" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH36" s="2">
         <v>0</v>
@@ -4504,7 +4504,7 @@
         <v>47</v>
       </c>
       <c r="C37" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D37" t="s">
         <v>73</v>
@@ -4513,10 +4513,10 @@
         <v>44707</v>
       </c>
       <c r="F37" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G37" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H37" s="2"/>
       <c r="I37" s="2">
@@ -4595,7 +4595,7 @@
         <v>0</v>
       </c>
       <c r="AH37" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI37" s="2">
         <v>0</v>
@@ -4615,7 +4615,7 @@
         <v>8</v>
       </c>
       <c r="B38" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C38" t="s">
         <v>71</v>
@@ -4729,10 +4729,10 @@
         <v>8</v>
       </c>
       <c r="B39" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C39" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D39" t="s">
         <v>73</v>
@@ -4741,10 +4741,10 @@
         <v>44789</v>
       </c>
       <c r="F39" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G39" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H39" s="2"/>
       <c r="I39" s="2">
@@ -4754,10 +4754,10 @@
         <v>2</v>
       </c>
       <c r="K39" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L39" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M39" s="2">
         <v>0</v>
@@ -4805,7 +4805,7 @@
         <v>0</v>
       </c>
       <c r="AB39" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC39" s="2">
         <v>0</v>
@@ -4843,7 +4843,7 @@
         <v>8</v>
       </c>
       <c r="B40" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C40" t="s">
         <v>70</v>
@@ -4957,10 +4957,10 @@
         <v>8</v>
       </c>
       <c r="B41" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="C41" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D41" t="s">
         <v>73</v>
@@ -4969,10 +4969,10 @@
         <v>44789</v>
       </c>
       <c r="F41" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G41" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H41" s="2"/>
       <c r="I41" s="2">
@@ -4982,10 +4982,10 @@
         <v>2</v>
       </c>
       <c r="K41" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L41" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M41" s="2">
         <v>0</v>
@@ -5033,7 +5033,7 @@
         <v>0</v>
       </c>
       <c r="AB41" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC41" s="2">
         <v>0</v>
@@ -5071,7 +5071,7 @@
         <v>9</v>
       </c>
       <c r="B42" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C42" t="s">
         <v>71</v>
@@ -5147,7 +5147,7 @@
         <v>0</v>
       </c>
       <c r="AB42" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC42" s="2">
         <v>0</v>
@@ -5165,7 +5165,7 @@
         <v>0</v>
       </c>
       <c r="AH42" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI42" s="2">
         <v>0</v>
@@ -5185,7 +5185,7 @@
         <v>9</v>
       </c>
       <c r="B43" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="C43" t="s">
         <v>71</v>
@@ -5285,7 +5285,7 @@
         <v>0</v>
       </c>
       <c r="AJ43" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK43" s="2">
         <v>0</v>
@@ -5299,7 +5299,7 @@
         <v>9</v>
       </c>
       <c r="B44" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C44" t="s">
         <v>71</v>
@@ -5413,10 +5413,10 @@
         <v>9</v>
       </c>
       <c r="B45" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="C45" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D45" t="s">
         <v>73</v>
@@ -5425,10 +5425,10 @@
         <v>44818</v>
       </c>
       <c r="F45" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G45" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H45" s="2"/>
       <c r="I45" s="2">
@@ -5489,7 +5489,7 @@
         <v>0</v>
       </c>
       <c r="AB45" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC45" s="2">
         <v>0</v>
@@ -5513,7 +5513,7 @@
         <v>0</v>
       </c>
       <c r="AJ45" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK45" s="2">
         <v>0</v>
@@ -5527,10 +5527,10 @@
         <v>9</v>
       </c>
       <c r="B46" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="C46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D46" t="s">
         <v>73</v>
@@ -5539,10 +5539,10 @@
         <v>44818</v>
       </c>
       <c r="F46" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G46" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H46" s="2"/>
       <c r="I46" s="2">
@@ -5603,7 +5603,7 @@
         <v>0</v>
       </c>
       <c r="AB46" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC46" s="2">
         <v>0</v>
@@ -5627,7 +5627,7 @@
         <v>0</v>
       </c>
       <c r="AJ46" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK46" s="2">
         <v>0</v>
@@ -5641,7 +5641,7 @@
         <v>9</v>
       </c>
       <c r="B47" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C47" t="s">
         <v>71</v>
@@ -5699,7 +5699,7 @@
         <v>0</v>
       </c>
       <c r="V47" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W47" s="2">
         <v>0</v>
@@ -5717,7 +5717,7 @@
         <v>0</v>
       </c>
       <c r="AB47" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC47" s="2">
         <v>0</v>
@@ -5741,7 +5741,7 @@
         <v>0</v>
       </c>
       <c r="AJ47" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK47" s="2">
         <v>0</v>
@@ -5755,10 +5755,10 @@
         <v>9</v>
       </c>
       <c r="B48" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="C48" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D48" t="s">
         <v>73</v>
@@ -5767,10 +5767,10 @@
         <v>44818</v>
       </c>
       <c r="F48" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G48" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H48" s="2"/>
       <c r="I48" s="2">
@@ -5780,10 +5780,10 @@
         <v>3</v>
       </c>
       <c r="K48" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L48" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M48" s="2">
         <v>0</v>
@@ -5831,7 +5831,7 @@
         <v>0</v>
       </c>
       <c r="AB48" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC48" s="2">
         <v>0</v>
@@ -5855,7 +5855,7 @@
         <v>0</v>
       </c>
       <c r="AJ48" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK48" s="2">
         <v>0</v>
@@ -5872,7 +5872,7 @@
         <v>24</v>
       </c>
       <c r="C49" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D49" t="s">
         <v>73</v>
@@ -5881,10 +5881,10 @@
         <v>44818</v>
       </c>
       <c r="F49" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G49" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H49" s="2"/>
       <c r="I49" s="2">
@@ -5894,10 +5894,10 @@
         <v>3</v>
       </c>
       <c r="K49" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L49" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M49" s="2">
         <v>0</v>
@@ -5945,7 +5945,7 @@
         <v>0</v>
       </c>
       <c r="AB49" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC49" s="2">
         <v>0</v>
@@ -5969,7 +5969,7 @@
         <v>0</v>
       </c>
       <c r="AJ49" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK49" s="2">
         <v>0</v>
@@ -5983,7 +5983,7 @@
         <v>9</v>
       </c>
       <c r="B50" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C50" t="s">
         <v>71</v>
@@ -6059,7 +6059,7 @@
         <v>0</v>
       </c>
       <c r="AB50" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC50" s="2">
         <v>0</v>
@@ -6074,10 +6074,10 @@
         <v>0</v>
       </c>
       <c r="AG50" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH50" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI50" s="2">
         <v>0</v>
@@ -6097,10 +6097,10 @@
         <v>9</v>
       </c>
       <c r="B51" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C51" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D51" t="s">
         <v>73</v>
@@ -6109,10 +6109,10 @@
         <v>44818</v>
       </c>
       <c r="F51" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G51" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H51" s="2"/>
       <c r="I51" s="2">
@@ -6128,10 +6128,10 @@
         <v>0</v>
       </c>
       <c r="M51" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N51" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O51" s="2">
         <v>0</v>
@@ -6173,7 +6173,7 @@
         <v>0</v>
       </c>
       <c r="AB51" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC51" s="2">
         <v>0</v>
@@ -6197,7 +6197,7 @@
         <v>0</v>
       </c>
       <c r="AJ51" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK51" s="2">
         <v>0</v>
@@ -6211,10 +6211,10 @@
         <v>9</v>
       </c>
       <c r="B52" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="C52" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D52" t="s">
         <v>73</v>
@@ -6223,10 +6223,10 @@
         <v>44818</v>
       </c>
       <c r="F52" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G52" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H52" s="2"/>
       <c r="I52" s="2">
@@ -6242,10 +6242,10 @@
         <v>0</v>
       </c>
       <c r="M52" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N52" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O52" s="2">
         <v>0</v>
@@ -6311,7 +6311,7 @@
         <v>0</v>
       </c>
       <c r="AJ52" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK52" s="2">
         <v>0</v>
@@ -6325,7 +6325,7 @@
         <v>9</v>
       </c>
       <c r="B53" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="C53" t="s">
         <v>71</v>
@@ -6383,7 +6383,7 @@
         <v>0</v>
       </c>
       <c r="V53" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W53" s="2">
         <v>0</v>
@@ -6401,7 +6401,7 @@
         <v>0</v>
       </c>
       <c r="AB53" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC53" s="2">
         <v>0</v>
@@ -6416,7 +6416,7 @@
         <v>0</v>
       </c>
       <c r="AG53" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH53" s="2">
         <v>0</v>
@@ -6439,7 +6439,7 @@
         <v>9</v>
       </c>
       <c r="B54" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="C54" t="s">
         <v>71</v>
@@ -6539,7 +6539,7 @@
         <v>0</v>
       </c>
       <c r="AJ54" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK54" s="2">
         <v>0</v>
@@ -6553,7 +6553,7 @@
         <v>9</v>
       </c>
       <c r="B55" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="C55" t="s">
         <v>71</v>
@@ -6629,7 +6629,7 @@
         <v>0</v>
       </c>
       <c r="AB55" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC55" s="2">
         <v>0</v>
@@ -6667,7 +6667,7 @@
         <v>9</v>
       </c>
       <c r="B56" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="C56" t="s">
         <v>71</v>
@@ -6767,7 +6767,7 @@
         <v>0</v>
       </c>
       <c r="AJ56" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK56" s="2">
         <v>0</v>
@@ -6781,10 +6781,10 @@
         <v>10</v>
       </c>
       <c r="B57" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C57" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D57" t="s">
         <v>73</v>
@@ -6793,10 +6793,10 @@
         <v>44771</v>
       </c>
       <c r="F57" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G57" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H57" s="2"/>
       <c r="I57" s="2">
@@ -6872,7 +6872,7 @@
         <v>0</v>
       </c>
       <c r="AG57" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH57" s="2">
         <v>0</v>
@@ -6895,7 +6895,7 @@
         <v>10</v>
       </c>
       <c r="B58" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C58" t="s">
         <v>71</v>
@@ -7009,13 +7009,13 @@
         <v>10</v>
       </c>
       <c r="B59" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="C59" t="s">
         <v>70</v>
       </c>
       <c r="D59" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E59" s="1">
         <v>44771</v>
@@ -7058,7 +7058,7 @@
         <v>0</v>
       </c>
       <c r="S59" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T59" s="2">
         <v>0</v>
@@ -7100,7 +7100,7 @@
         <v>0</v>
       </c>
       <c r="AG59" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH59" s="2">
         <v>0</v>
@@ -7123,10 +7123,10 @@
         <v>10</v>
       </c>
       <c r="B60" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="C60" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D60" t="s">
         <v>73</v>
@@ -7135,10 +7135,10 @@
         <v>44771</v>
       </c>
       <c r="F60" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G60" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H60" s="2"/>
       <c r="I60" s="2">
@@ -7217,7 +7217,7 @@
         <v>0</v>
       </c>
       <c r="AH60" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI60" s="2">
         <v>0</v>
@@ -7237,13 +7237,13 @@
         <v>10</v>
       </c>
       <c r="B61" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C61" t="s">
         <v>70</v>
       </c>
       <c r="D61" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E61" s="1">
         <v>44771</v>
@@ -7286,7 +7286,7 @@
         <v>0</v>
       </c>
       <c r="S61" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T61" s="2">
         <v>0</v>
@@ -7328,7 +7328,7 @@
         <v>0</v>
       </c>
       <c r="AG61" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH61" s="2">
         <v>0</v>
@@ -7351,7 +7351,7 @@
         <v>10</v>
       </c>
       <c r="B62" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C62" t="s">
         <v>70</v>
@@ -7465,7 +7465,7 @@
         <v>10</v>
       </c>
       <c r="B63" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="C63" t="s">
         <v>70</v>
@@ -7538,10 +7538,10 @@
         <v>0</v>
       </c>
       <c r="AA63" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB63" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC63" s="2">
         <v>0</v>
@@ -7565,7 +7565,7 @@
         <v>0</v>
       </c>
       <c r="AJ63" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK63" s="2">
         <v>0</v>
@@ -7582,19 +7582,19 @@
         <v>41</v>
       </c>
       <c r="C64" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D64" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E64" s="1">
         <v>44771</v>
       </c>
       <c r="F64" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G64" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H64" s="2"/>
       <c r="I64" s="2">
@@ -7622,7 +7622,7 @@
         <v>0</v>
       </c>
       <c r="Q64" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R64" s="2">
         <v>0</v>
@@ -7670,7 +7670,7 @@
         <v>0</v>
       </c>
       <c r="AG64" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH64" s="2">
         <v>0</v>
@@ -7693,10 +7693,10 @@
         <v>10</v>
       </c>
       <c r="B65" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="C65" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D65" t="s">
         <v>73</v>
@@ -7705,10 +7705,10 @@
         <v>44771</v>
       </c>
       <c r="F65" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G65" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H65" s="2"/>
       <c r="I65" s="2">
@@ -7736,7 +7736,7 @@
         <v>0</v>
       </c>
       <c r="Q65" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R65" s="2">
         <v>0</v>
@@ -7769,7 +7769,7 @@
         <v>0</v>
       </c>
       <c r="AB65" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC65" s="2">
         <v>0</v>
@@ -7807,7 +7807,7 @@
         <v>10</v>
       </c>
       <c r="B66" t="s">
-        <v>56</v>
+        <v>24</v>
       </c>
       <c r="C66" t="s">
         <v>70</v>
@@ -7832,10 +7832,10 @@
         <v>11</v>
       </c>
       <c r="K66" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L66" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M66" s="2">
         <v>0</v>
@@ -7880,7 +7880,7 @@
         <v>0</v>
       </c>
       <c r="AA66" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB66" s="2">
         <v>1</v>
@@ -7921,7 +7921,7 @@
         <v>10</v>
       </c>
       <c r="B67" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="C67" t="s">
         <v>70</v>
@@ -7997,7 +7997,7 @@
         <v>0</v>
       </c>
       <c r="AB67" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC67" s="2">
         <v>0</v>
@@ -8021,7 +8021,7 @@
         <v>0</v>
       </c>
       <c r="AJ67" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK67" s="2">
         <v>0</v>
@@ -8035,7 +8035,7 @@
         <v>10</v>
       </c>
       <c r="B68" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="C68" t="s">
         <v>70</v>
@@ -8060,10 +8060,10 @@
         <v>11</v>
       </c>
       <c r="K68" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L68" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M68" s="2">
         <v>0</v>
@@ -8111,7 +8111,7 @@
         <v>0</v>
       </c>
       <c r="AB68" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC68" s="2">
         <v>0</v>
@@ -8149,10 +8149,10 @@
         <v>10</v>
       </c>
       <c r="B69" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="C69" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D69" t="s">
         <v>73</v>
@@ -8161,10 +8161,10 @@
         <v>44771</v>
       </c>
       <c r="F69" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G69" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H69" s="2"/>
       <c r="I69" s="2">
@@ -8225,7 +8225,7 @@
         <v>0</v>
       </c>
       <c r="AB69" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC69" s="2">
         <v>0</v>
@@ -8240,7 +8240,7 @@
         <v>0</v>
       </c>
       <c r="AG69" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH69" s="2">
         <v>0</v>
@@ -8263,13 +8263,13 @@
         <v>10</v>
       </c>
       <c r="B70" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C70" t="s">
         <v>70</v>
       </c>
       <c r="D70" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E70" s="1">
         <v>44771</v>
@@ -8336,10 +8336,10 @@
         <v>0</v>
       </c>
       <c r="AA70" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB70" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC70" s="2">
         <v>0</v>
@@ -8354,7 +8354,7 @@
         <v>0</v>
       </c>
       <c r="AG70" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH70" s="2">
         <v>0</v>
@@ -8377,10 +8377,10 @@
         <v>10</v>
       </c>
       <c r="B71" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C71" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D71" t="s">
         <v>73</v>
@@ -8389,10 +8389,10 @@
         <v>44771</v>
       </c>
       <c r="F71" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G71" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H71" s="2"/>
       <c r="I71" s="2">
@@ -8450,7 +8450,7 @@
         <v>0</v>
       </c>
       <c r="AA71" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB71" s="2">
         <v>1</v>
@@ -8471,7 +8471,7 @@
         <v>0</v>
       </c>
       <c r="AH71" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI71" s="2">
         <v>0</v>
@@ -8491,7 +8491,7 @@
         <v>11</v>
       </c>
       <c r="B72" t="s">
-        <v>60</v>
+        <v>24</v>
       </c>
       <c r="C72" t="s">
         <v>70</v>
@@ -8516,10 +8516,10 @@
         <v>2</v>
       </c>
       <c r="K72" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L72" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M72" s="2">
         <v>0</v>
@@ -8567,7 +8567,7 @@
         <v>0</v>
       </c>
       <c r="AB72" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC72" s="2">
         <v>0</v>
@@ -8605,10 +8605,10 @@
         <v>11</v>
       </c>
       <c r="B73" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="C73" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D73" t="s">
         <v>73</v>
@@ -8617,10 +8617,10 @@
         <v>44845</v>
       </c>
       <c r="F73" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G73" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H73" s="2"/>
       <c r="I73" s="2">
@@ -8719,10 +8719,10 @@
         <v>11</v>
       </c>
       <c r="B74" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C74" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D74" t="s">
         <v>73</v>
@@ -8731,10 +8731,10 @@
         <v>44845</v>
       </c>
       <c r="F74" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G74" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H74" s="2"/>
       <c r="I74" s="2">
@@ -8744,10 +8744,10 @@
         <v>2</v>
       </c>
       <c r="K74" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L74" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M74" s="2">
         <v>0</v>
@@ -8795,7 +8795,7 @@
         <v>0</v>
       </c>
       <c r="AB74" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC74" s="2">
         <v>0</v>
@@ -8833,7 +8833,7 @@
         <v>12</v>
       </c>
       <c r="B75" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C75" t="s">
         <v>70</v>
@@ -9061,7 +9061,7 @@
         <v>13</v>
       </c>
       <c r="B77" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="C77" t="s">
         <v>70</v>
@@ -9092,10 +9092,10 @@
         <v>0</v>
       </c>
       <c r="M77" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N77" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O77" s="2">
         <v>0</v>
@@ -9137,7 +9137,7 @@
         <v>0</v>
       </c>
       <c r="AB77" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC77" s="2">
         <v>0</v>
@@ -9161,7 +9161,7 @@
         <v>0</v>
       </c>
       <c r="AJ77" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK77" s="2">
         <v>0</v>
@@ -9175,7 +9175,7 @@
         <v>13</v>
       </c>
       <c r="B78" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C78" t="s">
         <v>70</v>
@@ -9275,7 +9275,7 @@
         <v>0</v>
       </c>
       <c r="AJ78" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK78" s="2">
         <v>0</v>
@@ -9289,7 +9289,7 @@
         <v>13</v>
       </c>
       <c r="B79" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="C79" t="s">
         <v>70</v>
@@ -9320,10 +9320,10 @@
         <v>0</v>
       </c>
       <c r="M79" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N79" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O79" s="2">
         <v>0</v>
@@ -9365,7 +9365,7 @@
         <v>0</v>
       </c>
       <c r="AB79" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC79" s="2">
         <v>0</v>
@@ -9389,7 +9389,7 @@
         <v>0</v>
       </c>
       <c r="AJ79" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK79" s="2">
         <v>0</v>
@@ -9403,7 +9403,7 @@
         <v>13</v>
       </c>
       <c r="B80" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C80" t="s">
         <v>70</v>
@@ -9517,7 +9517,7 @@
         <v>13</v>
       </c>
       <c r="B81" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="C81" t="s">
         <v>70</v>
@@ -9617,7 +9617,7 @@
         <v>0</v>
       </c>
       <c r="AJ81" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK81" s="2">
         <v>0</v>
@@ -9631,10 +9631,10 @@
         <v>14</v>
       </c>
       <c r="B82" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="C82" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D82" t="s">
         <v>73</v>
@@ -9643,10 +9643,10 @@
         <v>44894</v>
       </c>
       <c r="F82" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G82" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H82" s="2"/>
       <c r="I82" s="2">
@@ -9731,7 +9731,7 @@
         <v>0</v>
       </c>
       <c r="AJ82" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK82" s="2">
         <v>0</v>
@@ -9745,10 +9745,10 @@
         <v>14</v>
       </c>
       <c r="B83" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="C83" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D83" t="s">
         <v>73</v>
@@ -9757,10 +9757,10 @@
         <v>44894</v>
       </c>
       <c r="F83" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G83" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H83" s="2"/>
       <c r="I83" s="2">
@@ -9821,7 +9821,7 @@
         <v>0</v>
       </c>
       <c r="AB83" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC83" s="2">
         <v>0</v>
@@ -9848,7 +9848,7 @@
         <v>0</v>
       </c>
       <c r="AK83" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL83" s="2">
         <v>0</v>
@@ -9862,7 +9862,7 @@
         <v>63</v>
       </c>
       <c r="C84" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D84" t="s">
         <v>73</v>
@@ -9871,10 +9871,10 @@
         <v>44894</v>
       </c>
       <c r="F84" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G84" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H84" s="2"/>
       <c r="I84" s="2">
@@ -9973,10 +9973,10 @@
         <v>14</v>
       </c>
       <c r="B85" t="s">
-        <v>23</v>
+        <v>64</v>
       </c>
       <c r="C85" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D85" t="s">
         <v>73</v>
@@ -9985,10 +9985,10 @@
         <v>44894</v>
       </c>
       <c r="F85" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G85" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H85" s="2"/>
       <c r="I85" s="2">
@@ -10007,10 +10007,10 @@
         <v>0</v>
       </c>
       <c r="N85" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O85" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P85" s="2">
         <v>0</v>
@@ -10073,7 +10073,7 @@
         <v>0</v>
       </c>
       <c r="AJ85" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK85" s="2">
         <v>0</v>
@@ -10087,10 +10087,10 @@
         <v>14</v>
       </c>
       <c r="B86" t="s">
-        <v>64</v>
+        <v>22</v>
       </c>
       <c r="C86" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D86" t="s">
         <v>73</v>
@@ -10099,10 +10099,10 @@
         <v>44894</v>
       </c>
       <c r="F86" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G86" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H86" s="2"/>
       <c r="I86" s="2">
@@ -10163,7 +10163,7 @@
         <v>0</v>
       </c>
       <c r="AB86" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC86" s="2">
         <v>0</v>
@@ -10190,7 +10190,7 @@
         <v>0</v>
       </c>
       <c r="AK86" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL86" s="2">
         <v>0</v>
@@ -10201,10 +10201,10 @@
         <v>14</v>
       </c>
       <c r="B87" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="C87" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D87" t="s">
         <v>73</v>
@@ -10213,10 +10213,10 @@
         <v>44894</v>
       </c>
       <c r="F87" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G87" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H87" s="2"/>
       <c r="I87" s="2">
@@ -10277,7 +10277,7 @@
         <v>0</v>
       </c>
       <c r="AB87" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC87" s="2">
         <v>0</v>
@@ -10301,10 +10301,10 @@
         <v>0</v>
       </c>
       <c r="AJ87" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK87" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL87" s="2">
         <v>0</v>
@@ -10315,10 +10315,10 @@
         <v>14</v>
       </c>
       <c r="B88" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="C88" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D88" t="s">
         <v>73</v>
@@ -10327,10 +10327,10 @@
         <v>44894</v>
       </c>
       <c r="F88" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G88" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H88" s="2"/>
       <c r="I88" s="2">
@@ -10391,7 +10391,7 @@
         <v>0</v>
       </c>
       <c r="AB88" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC88" s="2">
         <v>0</v>
@@ -10415,10 +10415,10 @@
         <v>0</v>
       </c>
       <c r="AJ88" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK88" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL88" s="2">
         <v>0</v>
@@ -10429,7 +10429,7 @@
         <v>14</v>
       </c>
       <c r="B89" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="C89" t="s">
         <v>71</v>
@@ -10463,10 +10463,10 @@
         <v>0</v>
       </c>
       <c r="N89" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O89" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P89" s="2">
         <v>0</v>
@@ -10529,7 +10529,7 @@
         <v>0</v>
       </c>
       <c r="AJ89" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK89" s="2">
         <v>0</v>
@@ -10543,10 +10543,10 @@
         <v>14</v>
       </c>
       <c r="B90" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="C90" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D90" t="s">
         <v>73</v>
@@ -10555,10 +10555,10 @@
         <v>44894</v>
       </c>
       <c r="F90" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G90" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H90" s="2"/>
       <c r="I90" s="2">
@@ -10643,7 +10643,7 @@
         <v>0</v>
       </c>
       <c r="AJ90" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK90" s="2">
         <v>0</v>
@@ -10657,10 +10657,10 @@
         <v>15</v>
       </c>
       <c r="B91" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="C91" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D91" t="s">
         <v>73</v>
@@ -10669,10 +10669,10 @@
         <v>44865</v>
       </c>
       <c r="F91" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G91" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H91" s="2"/>
       <c r="I91" s="2">
@@ -10703,7 +10703,7 @@
         <v>0</v>
       </c>
       <c r="R91" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S91" s="2">
         <v>0</v>
@@ -10748,7 +10748,7 @@
         <v>0</v>
       </c>
       <c r="AG91" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH91" s="2">
         <v>0</v>
@@ -10771,7 +10771,7 @@
         <v>15</v>
       </c>
       <c r="B92" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C92" t="s">
         <v>71</v>
@@ -10885,7 +10885,7 @@
         <v>15</v>
       </c>
       <c r="B93" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C93" t="s">
         <v>70</v>
@@ -10931,7 +10931,7 @@
         <v>0</v>
       </c>
       <c r="R93" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S93" s="2">
         <v>0</v>
@@ -10976,7 +10976,7 @@
         <v>0</v>
       </c>
       <c r="AG93" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH93" s="2">
         <v>0</v>
@@ -10999,7 +10999,7 @@
         <v>15</v>
       </c>
       <c r="B94" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="C94" t="s">
         <v>70</v>
@@ -11024,10 +11024,10 @@
         <v>5</v>
       </c>
       <c r="K94" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L94" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M94" s="2">
         <v>0</v>
@@ -11075,7 +11075,7 @@
         <v>0</v>
       </c>
       <c r="AB94" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC94" s="2">
         <v>0</v>
@@ -11113,7 +11113,7 @@
         <v>15</v>
       </c>
       <c r="B95" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="C95" t="s">
         <v>71</v>
@@ -11213,7 +11213,7 @@
         <v>0</v>
       </c>
       <c r="AJ95" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK95" s="2">
         <v>0</v>
@@ -11227,10 +11227,10 @@
         <v>15</v>
       </c>
       <c r="B96" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="C96" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D96" t="s">
         <v>73</v>
@@ -11239,10 +11239,10 @@
         <v>44865</v>
       </c>
       <c r="F96" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G96" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H96" s="2"/>
       <c r="I96" s="2">
@@ -11252,10 +11252,10 @@
         <v>5</v>
       </c>
       <c r="K96" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L96" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M96" s="2">
         <v>0</v>
@@ -11303,7 +11303,7 @@
         <v>0</v>
       </c>
       <c r="AB96" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC96" s="2">
         <v>0</v>
@@ -11327,7 +11327,7 @@
         <v>0</v>
       </c>
       <c r="AJ96" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK96" s="2">
         <v>0</v>
@@ -11341,7 +11341,7 @@
         <v>15</v>
       </c>
       <c r="B97" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="C97" t="s">
         <v>70</v>
@@ -11432,7 +11432,7 @@
         <v>0</v>
       </c>
       <c r="AG97" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH97" s="2">
         <v>0</v>
@@ -11441,7 +11441,7 @@
         <v>0</v>
       </c>
       <c r="AJ97" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK97" s="2">
         <v>0</v>
@@ -11458,7 +11458,7 @@
         <v>57</v>
       </c>
       <c r="C98" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D98" t="s">
         <v>73</v>
@@ -11467,10 +11467,10 @@
         <v>44865</v>
       </c>
       <c r="F98" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G98" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H98" s="2"/>
       <c r="I98" s="2">
@@ -11569,10 +11569,10 @@
         <v>15</v>
       </c>
       <c r="B99" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="C99" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D99" t="s">
         <v>73</v>
@@ -11581,10 +11581,10 @@
         <v>44865</v>
       </c>
       <c r="F99" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G99" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H99" s="2"/>
       <c r="I99" s="2">
@@ -11660,7 +11660,7 @@
         <v>0</v>
       </c>
       <c r="AG99" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH99" s="2">
         <v>0</v>
@@ -11669,7 +11669,7 @@
         <v>0</v>
       </c>
       <c r="AJ99" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK99" s="2">
         <v>0</v>
@@ -11683,10 +11683,10 @@
         <v>16</v>
       </c>
       <c r="B100" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="C100" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D100" t="s">
         <v>73</v>
@@ -11695,10 +11695,10 @@
         <v>44879</v>
       </c>
       <c r="F100" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G100" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H100" s="2"/>
       <c r="I100" s="2">
@@ -11741,7 +11741,7 @@
         <v>0</v>
       </c>
       <c r="V100" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W100" s="2">
         <v>0</v>
@@ -11759,7 +11759,7 @@
         <v>0</v>
       </c>
       <c r="AB100" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC100" s="2">
         <v>0</v>
@@ -11797,10 +11797,10 @@
         <v>16</v>
       </c>
       <c r="B101" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C101" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D101" t="s">
         <v>73</v>
@@ -11809,10 +11809,10 @@
         <v>44879</v>
       </c>
       <c r="F101" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G101" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H101" s="2"/>
       <c r="I101" s="2">
@@ -11855,7 +11855,7 @@
         <v>0</v>
       </c>
       <c r="V101" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W101" s="2">
         <v>0</v>
@@ -11873,7 +11873,7 @@
         <v>0</v>
       </c>
       <c r="AB101" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC101" s="2">
         <v>0</v>
@@ -11897,7 +11897,7 @@
         <v>0</v>
       </c>
       <c r="AJ101" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK101" s="2">
         <v>0</v>
@@ -11911,7 +11911,7 @@
         <v>16</v>
       </c>
       <c r="B102" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C102" t="s">
         <v>71</v>
@@ -12025,10 +12025,10 @@
         <v>16</v>
       </c>
       <c r="B103" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C103" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D103" t="s">
         <v>73</v>
@@ -12037,10 +12037,10 @@
         <v>44879</v>
       </c>
       <c r="F103" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G103" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H103" s="2"/>
       <c r="I103" s="2">
@@ -12125,7 +12125,7 @@
         <v>0</v>
       </c>
       <c r="AJ103" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK103" s="2">
         <v>0</v>
@@ -12139,10 +12139,10 @@
         <v>16</v>
       </c>
       <c r="B104" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="C104" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D104" t="s">
         <v>73</v>
@@ -12151,10 +12151,10 @@
         <v>44879</v>
       </c>
       <c r="F104" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G104" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H104" s="2"/>
       <c r="I104" s="2">
@@ -12253,7 +12253,7 @@
         <v>16</v>
       </c>
       <c r="B105" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C105" t="s">
         <v>70</v>
@@ -12367,7 +12367,7 @@
         <v>16</v>
       </c>
       <c r="B106" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C106" t="s">
         <v>71</v>
@@ -12481,7 +12481,7 @@
         <v>17</v>
       </c>
       <c r="B107" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C107" t="s">
         <v>70</v>
@@ -12595,7 +12595,7 @@
         <v>17</v>
       </c>
       <c r="B108" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C108" t="s">
         <v>71</v>
@@ -12712,7 +12712,7 @@
         <v>31</v>
       </c>
       <c r="C109" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D109" t="s">
         <v>73</v>
@@ -12721,10 +12721,10 @@
         <v>44887</v>
       </c>
       <c r="F109" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G109" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H109" s="2"/>
       <c r="I109" s="2">
@@ -12761,7 +12761,7 @@
         <v>0</v>
       </c>
       <c r="T109" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U109" s="2">
         <v>0</v>
@@ -12797,7 +12797,7 @@
         <v>0</v>
       </c>
       <c r="AF109" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG109" s="2">
         <v>1</v>
@@ -12823,7 +12823,7 @@
         <v>18</v>
       </c>
       <c r="B110" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C110" t="s">
         <v>70</v>
@@ -12937,7 +12937,7 @@
         <v>18</v>
       </c>
       <c r="B111" t="s">
-        <v>67</v>
+        <v>32</v>
       </c>
       <c r="C111" t="s">
         <v>71</v>
@@ -13025,10 +13025,10 @@
         <v>0</v>
       </c>
       <c r="AF111" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG111" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH111" s="2">
         <v>0</v>
@@ -13051,7 +13051,7 @@
         <v>18</v>
       </c>
       <c r="B112" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C112" t="s">
         <v>70</v>
@@ -13103,7 +13103,7 @@
         <v>0</v>
       </c>
       <c r="T112" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U112" s="2">
         <v>0</v>
@@ -13142,7 +13142,7 @@
         <v>0</v>
       </c>
       <c r="AG112" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH112" s="2">
         <v>0</v>
@@ -13165,10 +13165,10 @@
         <v>18</v>
       </c>
       <c r="B113" t="s">
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="C113" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D113" t="s">
         <v>73</v>
@@ -13177,10 +13177,10 @@
         <v>44887</v>
       </c>
       <c r="F113" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G113" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H113" s="2"/>
       <c r="I113" s="2">
@@ -13279,7 +13279,7 @@
         <v>19</v>
       </c>
       <c r="B114" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C114" t="s">
         <v>70</v>
@@ -13399,7 +13399,7 @@
         <v>70</v>
       </c>
       <c r="D115" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E115" s="1">
         <v>44714</v>
@@ -13515,7 +13515,7 @@
         <v>70</v>
       </c>
       <c r="D116" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E116" s="1">
         <v>44714</v>

</xml_diff>

<commit_message>
update geo for TN
</commit_message>
<xml_diff>
--- a/datasets/lab_detail.xlsx
+++ b/datasets/lab_detail.xlsx
@@ -81,22 +81,22 @@
     <t>substance</t>
   </si>
   <si>
-    <t>fentanyl</t>
+    <t>p-fluorofentanyl</t>
   </si>
   <si>
     <t>despropionyl p-fluorofentanyl</t>
   </si>
   <si>
-    <t>p-fluorofentanyl</t>
+    <t>fentanyl</t>
   </si>
   <si>
     <t>dimethyl sulfone (methylsulfonylmethane MSM)</t>
   </si>
   <si>
-    <t>4-ANPP</t>
+    <t>xylazine</t>
   </si>
   <si>
-    <t>xylazine</t>
+    <t>4-ANPP</t>
   </si>
   <si>
     <t>phenethyl 4-ANPP</t>
@@ -108,25 +108,25 @@
     <t>3,4-methylenedioxy-N-benzylcathinone (BMDP)</t>
   </si>
   <si>
-    <t>norcocaine</t>
-  </si>
-  <si>
     <t>phenacetin</t>
   </si>
   <si>
     <t>methyl ecgonidine (MED)</t>
   </si>
   <si>
-    <t>benzoylecgonine (BZ)</t>
+    <t>norcocaine</t>
   </si>
   <si>
     <t>levamisole</t>
   </si>
   <si>
-    <t>tropacocaine</t>
+    <t>cocaine</t>
   </si>
   <si>
-    <t>cocaine</t>
+    <t>benzoylecgonine (BZ)</t>
+  </si>
+  <si>
+    <t>tropacocaine</t>
   </si>
   <si>
     <t>p-fluoro phenethyl 4-ANPP</t>
@@ -147,10 +147,10 @@
     <t>caffeine</t>
   </si>
   <si>
-    <t>heroin</t>
+    <t>6-monoacetylmorphine (6-MAM)</t>
   </si>
   <si>
-    <t>6-monoacetylmorphine (6-MAM)</t>
+    <t>heroin</t>
   </si>
   <si>
     <t>urea</t>
@@ -159,40 +159,40 @@
     <t>acetylcodeine</t>
   </si>
   <si>
+    <t>lidocaine</t>
+  </si>
+  <si>
+    <t>acetaminophen</t>
+  </si>
+  <si>
     <t>N-phenylpropanamide</t>
   </si>
   <si>
     <t>1,3-Diacetin</t>
   </si>
   <si>
-    <t>acetaminophen</t>
+    <t>N-ethyl-4-ANPP</t>
   </si>
   <si>
-    <t>lidocaine</t>
+    <t>metonitazene</t>
   </si>
   <si>
-    <t>N-ethyl-4-ANPP</t>
+    <t>diphenhydramine</t>
   </si>
   <si>
     <t>gabapentin</t>
   </si>
   <si>
-    <t>diphenhydramine</t>
+    <t>inositol</t>
   </si>
   <si>
-    <t>metonitazene</t>
-  </si>
-  <si>
-    <t>methadone</t>
+    <t>N-piperidinyl etonitazene</t>
   </si>
   <si>
     <t>quinine</t>
   </si>
   <si>
-    <t>N-piperidinyl etonitazene</t>
-  </si>
-  <si>
-    <t>inositol</t>
+    <t>methadone</t>
   </si>
   <si>
     <t>non-specific organic acids</t>
@@ -548,10 +548,10 @@
         <v>7</v>
       </c>
       <c r="K2" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L2" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M2" s="2">
         <v>0</v>
@@ -788,10 +788,10 @@
         <v>7</v>
       </c>
       <c r="K4" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M4" s="2">
         <v>0</v>
@@ -1034,10 +1034,10 @@
         <v>0</v>
       </c>
       <c r="M6" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N6" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O6" s="2">
         <v>0</v>
@@ -1154,10 +1154,10 @@
         <v>0</v>
       </c>
       <c r="M7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O7" s="2">
         <v>0</v>
@@ -1729,7 +1729,7 @@
         <v>71</v>
       </c>
       <c r="D12" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E12" s="1">
         <v>44714</v>
@@ -1817,10 +1817,10 @@
         <v>0</v>
       </c>
       <c r="AH12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI12" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ12" s="2">
         <v>0</v>
@@ -1849,7 +1849,7 @@
         <v>71</v>
       </c>
       <c r="D13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E13" s="1">
         <v>44714</v>
@@ -1940,7 +1940,7 @@
         <v>0</v>
       </c>
       <c r="AI13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ13" s="2">
         <v>0</v>
@@ -2057,7 +2057,7 @@
         <v>0</v>
       </c>
       <c r="AH14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI14" s="2">
         <v>0</v>
@@ -2089,7 +2089,7 @@
         <v>71</v>
       </c>
       <c r="D15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E15" s="1">
         <v>44714</v>
@@ -2141,7 +2141,7 @@
         <v>0</v>
       </c>
       <c r="V15" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W15" s="2">
         <v>0</v>
@@ -2180,7 +2180,7 @@
         <v>0</v>
       </c>
       <c r="AI15" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ15" s="2">
         <v>0</v>
@@ -2206,7 +2206,7 @@
         <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D16" t="s">
         <v>73</v>
@@ -2215,10 +2215,10 @@
         <v>44714</v>
       </c>
       <c r="F16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2">
@@ -2249,10 +2249,10 @@
         <v>0</v>
       </c>
       <c r="R16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T16" s="2">
         <v>0</v>
@@ -2261,7 +2261,7 @@
         <v>0</v>
       </c>
       <c r="V16" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W16" s="2">
         <v>0</v>
@@ -2300,7 +2300,7 @@
         <v>0</v>
       </c>
       <c r="AI16" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ16" s="2">
         <v>0</v>
@@ -2329,7 +2329,7 @@
         <v>71</v>
       </c>
       <c r="D17" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E17" s="1">
         <v>44714</v>
@@ -2417,10 +2417,10 @@
         <v>0</v>
       </c>
       <c r="AH17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ17" s="2">
         <v>0</v>
@@ -2446,7 +2446,7 @@
         <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D18" t="s">
         <v>73</v>
@@ -2455,10 +2455,10 @@
         <v>44714</v>
       </c>
       <c r="F18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18" s="2"/>
       <c r="I18" s="2">
@@ -2489,10 +2489,10 @@
         <v>0</v>
       </c>
       <c r="R18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T18" s="2">
         <v>0</v>
@@ -2537,10 +2537,10 @@
         <v>0</v>
       </c>
       <c r="AH18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ18" s="2">
         <v>0</v>
@@ -2563,10 +2563,10 @@
         <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D19" t="s">
         <v>73</v>
@@ -2575,10 +2575,10 @@
         <v>44759</v>
       </c>
       <c r="F19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2">
@@ -2672,7 +2672,7 @@
         <v>1</v>
       </c>
       <c r="AM19" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN19" s="2">
         <v>0</v>
@@ -2683,13 +2683,13 @@
         <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="C20" t="s">
         <v>70</v>
       </c>
       <c r="D20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E20" s="1">
         <v>44759</v>
@@ -2765,7 +2765,7 @@
         <v>0</v>
       </c>
       <c r="AD20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE20" s="2">
         <v>0</v>
@@ -2780,7 +2780,7 @@
         <v>0</v>
       </c>
       <c r="AI20" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ20" s="2">
         <v>0</v>
@@ -2792,7 +2792,7 @@
         <v>0</v>
       </c>
       <c r="AM20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN20" s="2">
         <v>0</v>
@@ -2803,10 +2803,10 @@
         <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="C21" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D21" t="s">
         <v>73</v>
@@ -2815,10 +2815,10 @@
         <v>44759</v>
       </c>
       <c r="F21" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2">
@@ -2912,7 +2912,7 @@
         <v>1</v>
       </c>
       <c r="AM21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN21" s="2">
         <v>0</v>
@@ -2923,13 +2923,13 @@
         <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="C22" t="s">
         <v>70</v>
       </c>
       <c r="D22" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E22" s="1">
         <v>44759</v>
@@ -3005,7 +3005,7 @@
         <v>0</v>
       </c>
       <c r="AD22" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE22" s="2">
         <v>0</v>
@@ -3020,7 +3020,7 @@
         <v>0</v>
       </c>
       <c r="AI22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ22" s="2">
         <v>0</v>
@@ -3032,7 +3032,7 @@
         <v>0</v>
       </c>
       <c r="AM22" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN22" s="2">
         <v>0</v>
@@ -3163,10 +3163,10 @@
         <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="C24" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D24" t="s">
         <v>73</v>
@@ -3175,10 +3175,10 @@
         <v>44759</v>
       </c>
       <c r="F24" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G24" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2">
@@ -3188,10 +3188,10 @@
         <v>4</v>
       </c>
       <c r="K24" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L24" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M24" s="2">
         <v>0</v>
@@ -3227,7 +3227,7 @@
         <v>0</v>
       </c>
       <c r="X24" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y24" s="2">
         <v>0</v>
@@ -3283,10 +3283,10 @@
         <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D25" t="s">
         <v>73</v>
@@ -3295,10 +3295,10 @@
         <v>44759</v>
       </c>
       <c r="F25" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H25" s="2"/>
       <c r="I25" s="2">
@@ -3308,10 +3308,10 @@
         <v>4</v>
       </c>
       <c r="K25" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L25" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M25" s="2">
         <v>0</v>
@@ -3347,7 +3347,7 @@
         <v>0</v>
       </c>
       <c r="X25" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y25" s="2">
         <v>0</v>
@@ -3403,7 +3403,7 @@
         <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C26" t="s">
         <v>71</v>
@@ -3446,7 +3446,7 @@
         <v>0</v>
       </c>
       <c r="Q26" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R26" s="2">
         <v>0</v>
@@ -3515,7 +3515,7 @@
         <v>0</v>
       </c>
       <c r="AN26" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -3523,10 +3523,10 @@
         <v>6</v>
       </c>
       <c r="B27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C27" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D27" t="s">
         <v>73</v>
@@ -3535,10 +3535,10 @@
         <v>44721</v>
       </c>
       <c r="F27" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G27" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H27" s="2"/>
       <c r="I27" s="2">
@@ -3575,7 +3575,7 @@
         <v>0</v>
       </c>
       <c r="T27" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U27" s="2">
         <v>0</v>
@@ -3620,7 +3620,7 @@
         <v>0</v>
       </c>
       <c r="AI27" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ27" s="2">
         <v>0</v>
@@ -3635,7 +3635,7 @@
         <v>0</v>
       </c>
       <c r="AN27" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28">
@@ -3643,10 +3643,10 @@
         <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D28" t="s">
         <v>73</v>
@@ -3655,10 +3655,10 @@
         <v>44721</v>
       </c>
       <c r="F28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G28" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H28" s="2"/>
       <c r="I28" s="2">
@@ -3686,7 +3686,7 @@
         <v>0</v>
       </c>
       <c r="Q28" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R28" s="2">
         <v>0</v>
@@ -3695,7 +3695,7 @@
         <v>0</v>
       </c>
       <c r="T28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U28" s="2">
         <v>0</v>
@@ -3740,7 +3740,7 @@
         <v>0</v>
       </c>
       <c r="AI28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ28" s="2">
         <v>0</v>
@@ -3763,22 +3763,22 @@
         <v>7</v>
       </c>
       <c r="B29" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E29" s="1">
         <v>44707</v>
       </c>
       <c r="F29" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G29" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H29" s="2"/>
       <c r="I29" s="2">
@@ -3794,10 +3794,10 @@
         <v>0</v>
       </c>
       <c r="M29" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N29" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O29" s="2">
         <v>0</v>
@@ -3886,7 +3886,7 @@
         <v>44</v>
       </c>
       <c r="C30" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D30" t="s">
         <v>73</v>
@@ -3895,10 +3895,10 @@
         <v>44707</v>
       </c>
       <c r="F30" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G30" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H30" s="2"/>
       <c r="I30" s="2">
@@ -4003,7 +4003,7 @@
         <v>7</v>
       </c>
       <c r="B31" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C31" t="s">
         <v>70</v>
@@ -4123,13 +4123,13 @@
         <v>7</v>
       </c>
       <c r="B32" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C32" t="s">
         <v>71</v>
       </c>
       <c r="D32" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E32" s="1">
         <v>44707</v>
@@ -4205,7 +4205,7 @@
         <v>0</v>
       </c>
       <c r="AD32" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE32" s="2">
         <v>0</v>
@@ -4229,7 +4229,7 @@
         <v>0</v>
       </c>
       <c r="AL32" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM32" s="2">
         <v>0</v>
@@ -4363,7 +4363,7 @@
         <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="C34" t="s">
         <v>70</v>
@@ -4394,10 +4394,10 @@
         <v>0</v>
       </c>
       <c r="M34" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N34" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O34" s="2">
         <v>0</v>
@@ -4445,7 +4445,7 @@
         <v>0</v>
       </c>
       <c r="AD34" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE34" s="2">
         <v>0</v>
@@ -4469,7 +4469,7 @@
         <v>0</v>
       </c>
       <c r="AL34" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM34" s="2">
         <v>0</v>
@@ -4483,7 +4483,7 @@
         <v>7</v>
       </c>
       <c r="B35" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C35" t="s">
         <v>71</v>
@@ -4963,10 +4963,10 @@
         <v>8</v>
       </c>
       <c r="B39" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C39" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D39" t="s">
         <v>73</v>
@@ -4975,10 +4975,10 @@
         <v>44789</v>
       </c>
       <c r="F39" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G39" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H39" s="2"/>
       <c r="I39" s="2">
@@ -4988,10 +4988,10 @@
         <v>2</v>
       </c>
       <c r="K39" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L39" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M39" s="2">
         <v>0</v>
@@ -5045,7 +5045,7 @@
         <v>0</v>
       </c>
       <c r="AD39" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE39" s="2">
         <v>0</v>
@@ -5069,7 +5069,7 @@
         <v>0</v>
       </c>
       <c r="AL39" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM39" s="2">
         <v>0</v>
@@ -5083,7 +5083,7 @@
         <v>8</v>
       </c>
       <c r="B40" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C40" t="s">
         <v>71</v>
@@ -5203,10 +5203,10 @@
         <v>8</v>
       </c>
       <c r="B41" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C41" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D41" t="s">
         <v>73</v>
@@ -5215,10 +5215,10 @@
         <v>44789</v>
       </c>
       <c r="F41" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G41" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H41" s="2"/>
       <c r="I41" s="2">
@@ -5228,10 +5228,10 @@
         <v>2</v>
       </c>
       <c r="K41" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L41" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M41" s="2">
         <v>0</v>
@@ -5285,7 +5285,7 @@
         <v>0</v>
       </c>
       <c r="AD41" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE41" s="2">
         <v>0</v>
@@ -5309,7 +5309,7 @@
         <v>0</v>
       </c>
       <c r="AL41" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM41" s="2">
         <v>0</v>
@@ -5420,7 +5420,7 @@
         <v>0</v>
       </c>
       <c r="AI42" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ42" s="2">
         <v>0</v>
@@ -5429,7 +5429,7 @@
         <v>0</v>
       </c>
       <c r="AL42" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM42" s="2">
         <v>0</v>
@@ -5563,7 +5563,7 @@
         <v>9</v>
       </c>
       <c r="B44" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="C44" t="s">
         <v>71</v>
@@ -5645,7 +5645,7 @@
         <v>0</v>
       </c>
       <c r="AD44" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE44" s="2">
         <v>0</v>
@@ -5683,7 +5683,7 @@
         <v>9</v>
       </c>
       <c r="B45" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="C45" t="s">
         <v>71</v>
@@ -5765,7 +5765,7 @@
         <v>0</v>
       </c>
       <c r="AD45" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE45" s="2">
         <v>0</v>
@@ -5789,7 +5789,7 @@
         <v>0</v>
       </c>
       <c r="AL45" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM45" s="2">
         <v>0</v>
@@ -5803,7 +5803,7 @@
         <v>9</v>
       </c>
       <c r="B46" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C46" t="s">
         <v>71</v>
@@ -5885,7 +5885,7 @@
         <v>0</v>
       </c>
       <c r="AD46" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE46" s="2">
         <v>0</v>
@@ -5900,7 +5900,7 @@
         <v>0</v>
       </c>
       <c r="AI46" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ46" s="2">
         <v>0</v>
@@ -5923,10 +5923,10 @@
         <v>9</v>
       </c>
       <c r="B47" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="C47" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D47" t="s">
         <v>73</v>
@@ -5935,10 +5935,10 @@
         <v>44818</v>
       </c>
       <c r="F47" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G47" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H47" s="2"/>
       <c r="I47" s="2">
@@ -5948,10 +5948,10 @@
         <v>3</v>
       </c>
       <c r="K47" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L47" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M47" s="2">
         <v>0</v>
@@ -6043,10 +6043,10 @@
         <v>9</v>
       </c>
       <c r="B48" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="C48" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D48" t="s">
         <v>73</v>
@@ -6055,10 +6055,10 @@
         <v>44818</v>
       </c>
       <c r="F48" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G48" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H48" s="2"/>
       <c r="I48" s="2">
@@ -6068,10 +6068,10 @@
         <v>3</v>
       </c>
       <c r="K48" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L48" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M48" s="2">
         <v>0</v>
@@ -6143,7 +6143,7 @@
         <v>0</v>
       </c>
       <c r="AJ48" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK48" s="2">
         <v>0</v>
@@ -6163,7 +6163,7 @@
         <v>9</v>
       </c>
       <c r="B49" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C49" t="s">
         <v>71</v>
@@ -6269,7 +6269,7 @@
         <v>0</v>
       </c>
       <c r="AL49" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM49" s="2">
         <v>0</v>
@@ -6283,10 +6283,10 @@
         <v>9</v>
       </c>
       <c r="B50" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C50" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D50" t="s">
         <v>73</v>
@@ -6295,10 +6295,10 @@
         <v>44818</v>
       </c>
       <c r="F50" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G50" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H50" s="2"/>
       <c r="I50" s="2">
@@ -6403,10 +6403,10 @@
         <v>9</v>
       </c>
       <c r="B51" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="C51" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D51" t="s">
         <v>73</v>
@@ -6415,10 +6415,10 @@
         <v>44818</v>
       </c>
       <c r="F51" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G51" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H51" s="2"/>
       <c r="I51" s="2">
@@ -6434,10 +6434,10 @@
         <v>0</v>
       </c>
       <c r="M51" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N51" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O51" s="2">
         <v>0</v>
@@ -6485,7 +6485,7 @@
         <v>0</v>
       </c>
       <c r="AD51" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE51" s="2">
         <v>0</v>
@@ -6509,7 +6509,7 @@
         <v>0</v>
       </c>
       <c r="AL51" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM51" s="2">
         <v>0</v>
@@ -6523,7 +6523,7 @@
         <v>9</v>
       </c>
       <c r="B52" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C52" t="s">
         <v>71</v>
@@ -6587,7 +6587,7 @@
         <v>0</v>
       </c>
       <c r="X52" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y52" s="2">
         <v>0</v>
@@ -6623,7 +6623,7 @@
         <v>0</v>
       </c>
       <c r="AJ52" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK52" s="2">
         <v>0</v>
@@ -6643,10 +6643,10 @@
         <v>9</v>
       </c>
       <c r="B53" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="C53" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D53" t="s">
         <v>73</v>
@@ -6655,10 +6655,10 @@
         <v>44818</v>
       </c>
       <c r="F53" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G53" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H53" s="2"/>
       <c r="I53" s="2">
@@ -6707,7 +6707,7 @@
         <v>0</v>
       </c>
       <c r="X53" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y53" s="2">
         <v>0</v>
@@ -6725,7 +6725,7 @@
         <v>0</v>
       </c>
       <c r="AD53" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE53" s="2">
         <v>0</v>
@@ -6749,7 +6749,7 @@
         <v>0</v>
       </c>
       <c r="AL53" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM53" s="2">
         <v>0</v>
@@ -6763,7 +6763,7 @@
         <v>9</v>
       </c>
       <c r="B54" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="C54" t="s">
         <v>71</v>
@@ -6845,7 +6845,7 @@
         <v>0</v>
       </c>
       <c r="AD54" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE54" s="2">
         <v>0</v>
@@ -6883,10 +6883,10 @@
         <v>9</v>
       </c>
       <c r="B55" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C55" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D55" t="s">
         <v>73</v>
@@ -6895,10 +6895,10 @@
         <v>44818</v>
       </c>
       <c r="F55" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G55" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H55" s="2"/>
       <c r="I55" s="2">
@@ -6914,10 +6914,10 @@
         <v>0</v>
       </c>
       <c r="M55" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N55" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O55" s="2">
         <v>0</v>
@@ -6989,7 +6989,7 @@
         <v>0</v>
       </c>
       <c r="AL55" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM55" s="2">
         <v>0</v>
@@ -7003,7 +7003,7 @@
         <v>9</v>
       </c>
       <c r="B56" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="C56" t="s">
         <v>71</v>
@@ -7178,7 +7178,7 @@
         <v>0</v>
       </c>
       <c r="U57" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V57" s="2">
         <v>0</v>
@@ -7202,10 +7202,10 @@
         <v>0</v>
       </c>
       <c r="AC57" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD57" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE57" s="2">
         <v>0</v>
@@ -7243,7 +7243,7 @@
         <v>10</v>
       </c>
       <c r="B58" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C58" t="s">
         <v>70</v>
@@ -7538,7 +7538,7 @@
         <v>0</v>
       </c>
       <c r="U60" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V60" s="2">
         <v>0</v>
@@ -7562,10 +7562,10 @@
         <v>0</v>
       </c>
       <c r="AC60" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD60" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE60" s="2">
         <v>0</v>
@@ -7723,10 +7723,10 @@
         <v>10</v>
       </c>
       <c r="B62" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="C62" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D62" t="s">
         <v>73</v>
@@ -7735,10 +7735,10 @@
         <v>44771</v>
       </c>
       <c r="F62" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G62" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H62" s="2"/>
       <c r="I62" s="2">
@@ -7766,7 +7766,7 @@
         <v>0</v>
       </c>
       <c r="Q62" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R62" s="2">
         <v>0</v>
@@ -7805,7 +7805,7 @@
         <v>0</v>
       </c>
       <c r="AD62" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE62" s="2">
         <v>0</v>
@@ -7843,22 +7843,22 @@
         <v>10</v>
       </c>
       <c r="B63" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="C63" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D63" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E63" s="1">
         <v>44771</v>
       </c>
       <c r="F63" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G63" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H63" s="2"/>
       <c r="I63" s="2">
@@ -7886,7 +7886,7 @@
         <v>0</v>
       </c>
       <c r="Q63" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R63" s="2">
         <v>0</v>
@@ -7940,7 +7940,7 @@
         <v>0</v>
       </c>
       <c r="AI63" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ63" s="2">
         <v>0</v>
@@ -7963,22 +7963,22 @@
         <v>10</v>
       </c>
       <c r="B64" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="C64" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D64" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E64" s="1">
         <v>44771</v>
       </c>
       <c r="F64" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G64" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H64" s="2"/>
       <c r="I64" s="2">
@@ -8045,7 +8045,7 @@
         <v>0</v>
       </c>
       <c r="AD64" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE64" s="2">
         <v>0</v>
@@ -8060,10 +8060,10 @@
         <v>0</v>
       </c>
       <c r="AI64" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ64" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK64" s="2">
         <v>0</v>
@@ -8083,7 +8083,7 @@
         <v>10</v>
       </c>
       <c r="B65" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="C65" t="s">
         <v>70</v>
@@ -8108,10 +8108,10 @@
         <v>11</v>
       </c>
       <c r="K65" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L65" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M65" s="2">
         <v>0</v>
@@ -8162,7 +8162,7 @@
         <v>0</v>
       </c>
       <c r="AC65" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD65" s="2">
         <v>1</v>
@@ -8203,10 +8203,10 @@
         <v>10</v>
       </c>
       <c r="B66" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C66" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D66" t="s">
         <v>73</v>
@@ -8215,10 +8215,10 @@
         <v>44771</v>
       </c>
       <c r="F66" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G66" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H66" s="2"/>
       <c r="I66" s="2">
@@ -8285,7 +8285,7 @@
         <v>0</v>
       </c>
       <c r="AD66" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE66" s="2">
         <v>0</v>
@@ -8309,7 +8309,7 @@
         <v>0</v>
       </c>
       <c r="AL66" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM66" s="2">
         <v>0</v>
@@ -8323,13 +8323,13 @@
         <v>10</v>
       </c>
       <c r="B67" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="C67" t="s">
         <v>70</v>
       </c>
       <c r="D67" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E67" s="1">
         <v>44771</v>
@@ -8405,7 +8405,7 @@
         <v>0</v>
       </c>
       <c r="AD67" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE67" s="2">
         <v>0</v>
@@ -8420,7 +8420,7 @@
         <v>0</v>
       </c>
       <c r="AI67" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ67" s="2">
         <v>0</v>
@@ -8443,10 +8443,10 @@
         <v>10</v>
       </c>
       <c r="B68" t="s">
-        <v>58</v>
+        <v>28</v>
       </c>
       <c r="C68" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D68" t="s">
         <v>73</v>
@@ -8455,10 +8455,10 @@
         <v>44771</v>
       </c>
       <c r="F68" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G68" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H68" s="2"/>
       <c r="I68" s="2">
@@ -8522,10 +8522,10 @@
         <v>0</v>
       </c>
       <c r="AC68" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD68" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE68" s="2">
         <v>0</v>
@@ -8549,7 +8549,7 @@
         <v>0</v>
       </c>
       <c r="AL68" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM68" s="2">
         <v>0</v>
@@ -8563,13 +8563,13 @@
         <v>10</v>
       </c>
       <c r="B69" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C69" t="s">
         <v>70</v>
       </c>
       <c r="D69" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E69" s="1">
         <v>44771</v>
@@ -8660,7 +8660,7 @@
         <v>0</v>
       </c>
       <c r="AI69" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ69" s="2">
         <v>0</v>
@@ -8683,10 +8683,10 @@
         <v>10</v>
       </c>
       <c r="B70" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="C70" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D70" t="s">
         <v>73</v>
@@ -8695,10 +8695,10 @@
         <v>44771</v>
       </c>
       <c r="F70" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G70" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H70" s="2"/>
       <c r="I70" s="2">
@@ -8708,10 +8708,10 @@
         <v>11</v>
       </c>
       <c r="K70" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L70" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M70" s="2">
         <v>0</v>
@@ -8783,7 +8783,7 @@
         <v>0</v>
       </c>
       <c r="AJ70" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK70" s="2">
         <v>0</v>
@@ -8803,7 +8803,7 @@
         <v>10</v>
       </c>
       <c r="B71" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="C71" t="s">
         <v>70</v>
@@ -8885,7 +8885,7 @@
         <v>0</v>
       </c>
       <c r="AD71" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE71" s="2">
         <v>0</v>
@@ -8923,10 +8923,10 @@
         <v>11</v>
       </c>
       <c r="B72" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="C72" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D72" t="s">
         <v>73</v>
@@ -8935,10 +8935,10 @@
         <v>44845</v>
       </c>
       <c r="F72" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G72" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H72" s="2"/>
       <c r="I72" s="2">
@@ -9043,10 +9043,10 @@
         <v>11</v>
       </c>
       <c r="B73" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="C73" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D73" t="s">
         <v>73</v>
@@ -9055,10 +9055,10 @@
         <v>44845</v>
       </c>
       <c r="F73" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G73" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H73" s="2"/>
       <c r="I73" s="2">
@@ -9163,7 +9163,7 @@
         <v>11</v>
       </c>
       <c r="B74" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C74" t="s">
         <v>70</v>
@@ -9403,7 +9403,7 @@
         <v>13</v>
       </c>
       <c r="B76" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="C76" t="s">
         <v>70</v>
@@ -9500,7 +9500,7 @@
         <v>0</v>
       </c>
       <c r="AI76" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ76" s="2">
         <v>0</v>
@@ -9509,7 +9509,7 @@
         <v>0</v>
       </c>
       <c r="AL76" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM76" s="2">
         <v>0</v>
@@ -9523,7 +9523,7 @@
         <v>13</v>
       </c>
       <c r="B77" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="C77" t="s">
         <v>70</v>
@@ -9569,10 +9569,10 @@
         <v>0</v>
       </c>
       <c r="R77" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S77" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T77" s="2">
         <v>0</v>
@@ -9620,7 +9620,7 @@
         <v>0</v>
       </c>
       <c r="AI77" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ77" s="2">
         <v>0</v>
@@ -9643,7 +9643,7 @@
         <v>13</v>
       </c>
       <c r="B78" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C78" t="s">
         <v>70</v>
@@ -9668,10 +9668,10 @@
         <v>6</v>
       </c>
       <c r="K78" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L78" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M78" s="2">
         <v>0</v>
@@ -9725,7 +9725,7 @@
         <v>0</v>
       </c>
       <c r="AD78" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE78" s="2">
         <v>0</v>
@@ -9749,7 +9749,7 @@
         <v>0</v>
       </c>
       <c r="AL78" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM78" s="2">
         <v>0</v>
@@ -9763,7 +9763,7 @@
         <v>13</v>
       </c>
       <c r="B79" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="C79" t="s">
         <v>70</v>
@@ -9788,10 +9788,10 @@
         <v>6</v>
       </c>
       <c r="K79" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L79" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M79" s="2">
         <v>0</v>
@@ -9809,10 +9809,10 @@
         <v>0</v>
       </c>
       <c r="R79" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S79" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T79" s="2">
         <v>0</v>
@@ -9845,7 +9845,7 @@
         <v>0</v>
       </c>
       <c r="AD79" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE79" s="2">
         <v>0</v>
@@ -9883,7 +9883,7 @@
         <v>13</v>
       </c>
       <c r="B80" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="C80" t="s">
         <v>70</v>
@@ -9914,10 +9914,10 @@
         <v>0</v>
       </c>
       <c r="M80" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N80" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O80" s="2">
         <v>0</v>
@@ -9965,7 +9965,7 @@
         <v>0</v>
       </c>
       <c r="AD80" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE80" s="2">
         <v>0</v>
@@ -9989,7 +9989,7 @@
         <v>0</v>
       </c>
       <c r="AL80" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM80" s="2">
         <v>0</v>
@@ -10003,7 +10003,7 @@
         <v>13</v>
       </c>
       <c r="B81" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="C81" t="s">
         <v>70</v>
@@ -10034,10 +10034,10 @@
         <v>0</v>
       </c>
       <c r="M81" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N81" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O81" s="2">
         <v>0</v>
@@ -10085,7 +10085,7 @@
         <v>0</v>
       </c>
       <c r="AD81" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE81" s="2">
         <v>0</v>
@@ -10109,7 +10109,7 @@
         <v>0</v>
       </c>
       <c r="AL81" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM81" s="2">
         <v>0</v>
@@ -10123,10 +10123,10 @@
         <v>14</v>
       </c>
       <c r="B82" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="C82" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D82" t="s">
         <v>73</v>
@@ -10135,10 +10135,10 @@
         <v>44894</v>
       </c>
       <c r="F82" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G82" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H82" s="2"/>
       <c r="I82" s="2">
@@ -10229,10 +10229,10 @@
         <v>0</v>
       </c>
       <c r="AL82" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM82" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN82" s="2">
         <v>0</v>
@@ -10243,7 +10243,7 @@
         <v>14</v>
       </c>
       <c r="B83" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C83" t="s">
         <v>70</v>
@@ -10349,7 +10349,7 @@
         <v>0</v>
       </c>
       <c r="AL83" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM83" s="2">
         <v>0</v>
@@ -10363,10 +10363,10 @@
         <v>14</v>
       </c>
       <c r="B84" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="C84" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D84" t="s">
         <v>73</v>
@@ -10375,10 +10375,10 @@
         <v>44894</v>
       </c>
       <c r="F84" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G84" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H84" s="2"/>
       <c r="I84" s="2">
@@ -10445,7 +10445,7 @@
         <v>0</v>
       </c>
       <c r="AD84" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE84" s="2">
         <v>0</v>
@@ -10469,7 +10469,7 @@
         <v>0</v>
       </c>
       <c r="AL84" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM84" s="2">
         <v>1</v>
@@ -10483,7 +10483,7 @@
         <v>14</v>
       </c>
       <c r="B85" t="s">
-        <v>63</v>
+        <v>23</v>
       </c>
       <c r="C85" t="s">
         <v>70</v>
@@ -10565,7 +10565,7 @@
         <v>0</v>
       </c>
       <c r="AD85" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE85" s="2">
         <v>0</v>
@@ -10589,10 +10589,10 @@
         <v>0</v>
       </c>
       <c r="AL85" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM85" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN85" s="2">
         <v>0</v>
@@ -10603,7 +10603,7 @@
         <v>14</v>
       </c>
       <c r="B86" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="C86" t="s">
         <v>71</v>
@@ -10637,10 +10637,10 @@
         <v>0</v>
       </c>
       <c r="N86" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O86" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P86" s="2">
         <v>0</v>
@@ -10709,7 +10709,7 @@
         <v>0</v>
       </c>
       <c r="AL86" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM86" s="2">
         <v>0</v>
@@ -10723,7 +10723,7 @@
         <v>14</v>
       </c>
       <c r="B87" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="C87" t="s">
         <v>71</v>
@@ -10757,10 +10757,10 @@
         <v>0</v>
       </c>
       <c r="N87" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O87" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P87" s="2">
         <v>0</v>
@@ -10829,7 +10829,7 @@
         <v>0</v>
       </c>
       <c r="AL87" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM87" s="2">
         <v>0</v>
@@ -10843,10 +10843,10 @@
         <v>14</v>
       </c>
       <c r="B88" t="s">
-        <v>24</v>
+        <v>65</v>
       </c>
       <c r="C88" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D88" t="s">
         <v>73</v>
@@ -10855,10 +10855,10 @@
         <v>44894</v>
       </c>
       <c r="F88" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G88" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H88" s="2"/>
       <c r="I88" s="2">
@@ -10925,7 +10925,7 @@
         <v>0</v>
       </c>
       <c r="AD88" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE88" s="2">
         <v>0</v>
@@ -10963,10 +10963,10 @@
         <v>14</v>
       </c>
       <c r="B89" t="s">
-        <v>64</v>
+        <v>22</v>
       </c>
       <c r="C89" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D89" t="s">
         <v>73</v>
@@ -10975,10 +10975,10 @@
         <v>44894</v>
       </c>
       <c r="F89" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G89" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H89" s="2"/>
       <c r="I89" s="2">
@@ -11045,7 +11045,7 @@
         <v>0</v>
       </c>
       <c r="AD89" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE89" s="2">
         <v>0</v>
@@ -11083,7 +11083,7 @@
         <v>14</v>
       </c>
       <c r="B90" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="C90" t="s">
         <v>71</v>
@@ -11203,7 +11203,7 @@
         <v>15</v>
       </c>
       <c r="B91" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="C91" t="s">
         <v>70</v>
@@ -11255,7 +11255,7 @@
         <v>0</v>
       </c>
       <c r="T91" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U91" s="2">
         <v>0</v>
@@ -11300,7 +11300,7 @@
         <v>0</v>
       </c>
       <c r="AI91" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ91" s="2">
         <v>0</v>
@@ -11309,7 +11309,7 @@
         <v>0</v>
       </c>
       <c r="AL91" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM91" s="2">
         <v>0</v>
@@ -11323,10 +11323,10 @@
         <v>15</v>
       </c>
       <c r="B92" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C92" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D92" t="s">
         <v>73</v>
@@ -11335,10 +11335,10 @@
         <v>44865</v>
       </c>
       <c r="F92" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G92" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H92" s="2"/>
       <c r="I92" s="2">
@@ -11375,7 +11375,7 @@
         <v>0</v>
       </c>
       <c r="T92" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U92" s="2">
         <v>0</v>
@@ -11420,7 +11420,7 @@
         <v>0</v>
       </c>
       <c r="AI92" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ92" s="2">
         <v>0</v>
@@ -11429,7 +11429,7 @@
         <v>0</v>
       </c>
       <c r="AL92" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM92" s="2">
         <v>0</v>
@@ -11443,10 +11443,10 @@
         <v>15</v>
       </c>
       <c r="B93" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="C93" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D93" t="s">
         <v>73</v>
@@ -11455,10 +11455,10 @@
         <v>44865</v>
       </c>
       <c r="F93" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G93" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H93" s="2"/>
       <c r="I93" s="2">
@@ -11525,7 +11525,7 @@
         <v>0</v>
       </c>
       <c r="AD93" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE93" s="2">
         <v>0</v>
@@ -11563,10 +11563,10 @@
         <v>15</v>
       </c>
       <c r="B94" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="C94" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D94" t="s">
         <v>73</v>
@@ -11575,10 +11575,10 @@
         <v>44865</v>
       </c>
       <c r="F94" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G94" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H94" s="2"/>
       <c r="I94" s="2">
@@ -11645,7 +11645,7 @@
         <v>0</v>
       </c>
       <c r="AD94" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE94" s="2">
         <v>0</v>
@@ -11683,10 +11683,10 @@
         <v>15</v>
       </c>
       <c r="B95" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="C95" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D95" t="s">
         <v>73</v>
@@ -11695,10 +11695,10 @@
         <v>44865</v>
       </c>
       <c r="F95" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G95" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H95" s="2"/>
       <c r="I95" s="2">
@@ -11803,10 +11803,10 @@
         <v>15</v>
       </c>
       <c r="B96" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="C96" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D96" t="s">
         <v>73</v>
@@ -11815,10 +11815,10 @@
         <v>44865</v>
       </c>
       <c r="F96" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G96" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H96" s="2"/>
       <c r="I96" s="2">
@@ -11828,10 +11828,10 @@
         <v>5</v>
       </c>
       <c r="K96" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L96" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M96" s="2">
         <v>0</v>
@@ -11885,7 +11885,7 @@
         <v>0</v>
       </c>
       <c r="AD96" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE96" s="2">
         <v>0</v>
@@ -11900,7 +11900,7 @@
         <v>0</v>
       </c>
       <c r="AI96" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ96" s="2">
         <v>0</v>
@@ -11923,10 +11923,10 @@
         <v>15</v>
       </c>
       <c r="B97" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="C97" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D97" t="s">
         <v>73</v>
@@ -11935,10 +11935,10 @@
         <v>44865</v>
       </c>
       <c r="F97" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G97" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H97" s="2"/>
       <c r="I97" s="2">
@@ -12020,7 +12020,7 @@
         <v>0</v>
       </c>
       <c r="AI97" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ97" s="2">
         <v>0</v>
@@ -12043,10 +12043,10 @@
         <v>15</v>
       </c>
       <c r="B98" t="s">
-        <v>66</v>
+        <v>24</v>
       </c>
       <c r="C98" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D98" t="s">
         <v>73</v>
@@ -12055,10 +12055,10 @@
         <v>44865</v>
       </c>
       <c r="F98" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G98" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H98" s="2"/>
       <c r="I98" s="2">
@@ -12068,10 +12068,10 @@
         <v>5</v>
       </c>
       <c r="K98" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L98" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M98" s="2">
         <v>0</v>
@@ -12125,7 +12125,7 @@
         <v>0</v>
       </c>
       <c r="AD98" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE98" s="2">
         <v>0</v>
@@ -12163,10 +12163,10 @@
         <v>15</v>
       </c>
       <c r="B99" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C99" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D99" t="s">
         <v>73</v>
@@ -12175,10 +12175,10 @@
         <v>44865</v>
       </c>
       <c r="F99" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G99" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H99" s="2"/>
       <c r="I99" s="2">
@@ -12283,10 +12283,10 @@
         <v>16</v>
       </c>
       <c r="B100" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C100" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D100" t="s">
         <v>73</v>
@@ -12295,10 +12295,10 @@
         <v>44879</v>
       </c>
       <c r="F100" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G100" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H100" s="2"/>
       <c r="I100" s="2">
@@ -12389,7 +12389,7 @@
         <v>0</v>
       </c>
       <c r="AL100" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM100" s="2">
         <v>0</v>
@@ -12403,7 +12403,7 @@
         <v>16</v>
       </c>
       <c r="B101" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="C101" t="s">
         <v>70</v>
@@ -12428,10 +12428,10 @@
         <v>3</v>
       </c>
       <c r="K101" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L101" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M101" s="2">
         <v>0</v>
@@ -12485,7 +12485,7 @@
         <v>0</v>
       </c>
       <c r="AD101" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE101" s="2">
         <v>0</v>
@@ -12523,7 +12523,7 @@
         <v>16</v>
       </c>
       <c r="B102" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C102" t="s">
         <v>70</v>
@@ -12548,10 +12548,10 @@
         <v>3</v>
       </c>
       <c r="K102" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L102" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M102" s="2">
         <v>0</v>
@@ -12605,7 +12605,7 @@
         <v>0</v>
       </c>
       <c r="AD102" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE102" s="2">
         <v>0</v>
@@ -12629,7 +12629,7 @@
         <v>0</v>
       </c>
       <c r="AL102" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM102" s="2">
         <v>0</v>
@@ -12643,10 +12643,10 @@
         <v>16</v>
       </c>
       <c r="B103" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="C103" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D103" t="s">
         <v>73</v>
@@ -12655,10 +12655,10 @@
         <v>44879</v>
       </c>
       <c r="F103" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G103" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H103" s="2"/>
       <c r="I103" s="2">
@@ -12763,7 +12763,7 @@
         <v>16</v>
       </c>
       <c r="B104" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C104" t="s">
         <v>71</v>
@@ -13123,7 +13123,7 @@
         <v>17</v>
       </c>
       <c r="B107" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C107" t="s">
         <v>71</v>
@@ -13363,10 +13363,10 @@
         <v>18</v>
       </c>
       <c r="B109" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C109" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D109" t="s">
         <v>73</v>
@@ -13375,10 +13375,10 @@
         <v>44887</v>
       </c>
       <c r="F109" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G109" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H109" s="2"/>
       <c r="I109" s="2">
@@ -13457,10 +13457,10 @@
         <v>0</v>
       </c>
       <c r="AH109" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI109" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ109" s="2">
         <v>0</v>
@@ -13486,7 +13486,7 @@
         <v>37</v>
       </c>
       <c r="C110" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D110" t="s">
         <v>73</v>
@@ -13495,10 +13495,10 @@
         <v>44887</v>
       </c>
       <c r="F110" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G110" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H110" s="2"/>
       <c r="I110" s="2">
@@ -13529,10 +13529,10 @@
         <v>0</v>
       </c>
       <c r="R110" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S110" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T110" s="2">
         <v>0</v>
@@ -13577,10 +13577,10 @@
         <v>0</v>
       </c>
       <c r="AH110" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI110" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ110" s="2">
         <v>0</v>
@@ -13649,10 +13649,10 @@
         <v>0</v>
       </c>
       <c r="R111" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S111" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T111" s="2">
         <v>0</v>
@@ -13661,7 +13661,7 @@
         <v>0</v>
       </c>
       <c r="V111" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W111" s="2">
         <v>0</v>
@@ -13700,7 +13700,7 @@
         <v>0</v>
       </c>
       <c r="AI111" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ111" s="2">
         <v>0</v>
@@ -13723,7 +13723,7 @@
         <v>18</v>
       </c>
       <c r="B112" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C112" t="s">
         <v>70</v>
@@ -13781,7 +13781,7 @@
         <v>0</v>
       </c>
       <c r="V112" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W112" s="2">
         <v>0</v>
@@ -13820,7 +13820,7 @@
         <v>0</v>
       </c>
       <c r="AI112" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ112" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
fix float number issues
</commit_message>
<xml_diff>
--- a/datasets/lab_detail.xlsx
+++ b/datasets/lab_detail.xlsx
@@ -81,55 +81,58 @@
     <t>substance</t>
   </si>
   <si>
+    <t>4-ANPP</t>
+  </si>
+  <si>
     <t>dimethyl sulfone (methylsulfonylmethane MSM)</t>
+  </si>
+  <si>
+    <t>phenethyl 4-ANPP</t>
+  </si>
+  <si>
+    <t>xylazine</t>
+  </si>
+  <si>
+    <t>p-fluorofentanyl</t>
   </si>
   <si>
     <t>despropionyl p-fluorofentanyl</t>
   </si>
   <si>
-    <t>p-fluorofentanyl</t>
-  </si>
-  <si>
-    <t>xylazine</t>
-  </si>
-  <si>
     <t>fentanyl</t>
   </si>
   <si>
-    <t>4-ANPP</t>
-  </si>
-  <si>
-    <t>phenethyl 4-ANPP</t>
+    <t>3,4-methylenedioxy-N-benzylcathinone (BMDP)</t>
   </si>
   <si>
     <t>3,4-MDMA</t>
   </si>
   <si>
-    <t>3,4-methylenedioxy-N-benzylcathinone (BMDP)</t>
+    <t>benzoylecgonine (BZ)</t>
   </si>
   <si>
-    <t>benzoylecgonine (BZ)</t>
+    <t>levamisole</t>
   </si>
   <si>
     <t>tropacocaine</t>
   </si>
   <si>
-    <t>methyl ecgonidine (MED)</t>
+    <t>phenacetin</t>
   </si>
   <si>
     <t>cocaine</t>
   </si>
   <si>
-    <t>levamisole</t>
-  </si>
-  <si>
     <t>norcocaine</t>
   </si>
   <si>
-    <t>phenacetin</t>
+    <t>methyl ecgonidine (MED)</t>
   </si>
   <si>
     <t>tramadol</t>
+  </si>
+  <si>
+    <t>methamphetamine</t>
   </si>
   <si>
     <t>p-fluoro phenethyl 4-ANPP</t>
@@ -138,61 +141,58 @@
     <t>non-specific sugars</t>
   </si>
   <si>
-    <t>methamphetamine</t>
+    <t>caffeine</t>
   </si>
   <si>
     <t>eutylone</t>
   </si>
   <si>
-    <t>caffeine</t>
+    <t>acetylcodeine</t>
+  </si>
+  <si>
+    <t>urea</t>
+  </si>
+  <si>
+    <t>6-monoacetylmorphine (6-MAM)</t>
   </si>
   <si>
     <t>heroin</t>
   </si>
   <si>
-    <t>acetylcodeine</t>
+    <t>N-phenylpropanamide</t>
   </si>
   <si>
-    <t>6-monoacetylmorphine (6-MAM)</t>
-  </si>
-  <si>
-    <t>urea</t>
+    <t>acetaminophen</t>
   </si>
   <si>
     <t>lidocaine</t>
   </si>
   <si>
-    <t>N-phenylpropanamide</t>
-  </si>
-  <si>
     <t>N-ethyl-4-ANPP</t>
-  </si>
-  <si>
-    <t>acetaminophen</t>
   </si>
   <si>
     <t>1,3-Diacetin</t>
   </si>
   <si>
-    <t>quinine</t>
+    <t>N-piperidinyl etonitazene</t>
+  </si>
+  <si>
+    <t>gabapentin</t>
   </si>
   <si>
     <t>inositol</t>
   </si>
   <si>
-    <t>N-piperidinyl etonitazene</t>
+    <t>methadone</t>
   </si>
   <si>
     <t>metonitazene</t>
   </si>
   <si>
-    <t>diphenhydramine</t>
+    <t>quinine</t>
   </si>
   <si>
-    <t>methadone</t>
-  </si>
-  <si>
-    <t>gabapentin</t>
+    <t>diphenhydramine</t>
   </si>
   <si>
     <t>non-specific organic acids</t>
@@ -201,16 +201,16 @@
     <t>procaine</t>
   </si>
   <si>
-    <t>phenethyl chloride</t>
+    <t>nicotine</t>
+  </si>
+  <si>
+    <t>menthol</t>
   </si>
   <si>
     <t>phenethylbromide</t>
   </si>
   <si>
-    <t>nicotine</t>
-  </si>
-  <si>
-    <t>menthol</t>
+    <t>phenethyl chloride</t>
   </si>
   <si>
     <t>1-phenethyl-4-propionyloxypiperidine</t>
@@ -638,7 +638,7 @@
         <v>0</v>
       </c>
       <c r="AM2" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN2" s="2">
         <v>0</v>
@@ -737,7 +737,7 @@
         <v>0</v>
       </c>
       <c r="AE3" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF3" s="2">
         <v>0</v>
@@ -764,7 +764,7 @@
         <v>0</v>
       </c>
       <c r="AN3" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO3" s="2">
         <v>0</v>
@@ -860,7 +860,7 @@
         <v>0</v>
       </c>
       <c r="AE4" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF4" s="2">
         <v>0</v>
@@ -884,7 +884,7 @@
         <v>0</v>
       </c>
       <c r="AM4" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN4" s="2">
         <v>0</v>
@@ -1049,10 +1049,10 @@
         <v>0</v>
       </c>
       <c r="L6" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M6" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N6" s="2">
         <v>0</v>
@@ -1229,7 +1229,7 @@
         <v>0</v>
       </c>
       <c r="AE7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF7" s="2">
         <v>0</v>
@@ -1253,10 +1253,10 @@
         <v>0</v>
       </c>
       <c r="AM7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO7" s="2">
         <v>0</v>
@@ -1295,10 +1295,10 @@
         <v>0</v>
       </c>
       <c r="L8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N8" s="2">
         <v>0</v>
@@ -1352,7 +1352,7 @@
         <v>0</v>
       </c>
       <c r="AE8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF8" s="2">
         <v>0</v>
@@ -1376,7 +1376,7 @@
         <v>0</v>
       </c>
       <c r="AM8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN8" s="2">
         <v>0</v>
@@ -1393,7 +1393,7 @@
         <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D9" t="s">
         <v>73</v>
@@ -1402,10 +1402,10 @@
         <v>44777</v>
       </c>
       <c r="F9" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2">
@@ -1454,7 +1454,7 @@
         <v>0</v>
       </c>
       <c r="X9" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y9" s="2">
         <v>0</v>
@@ -1516,7 +1516,7 @@
         <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D10" t="s">
         <v>73</v>
@@ -1525,10 +1525,10 @@
         <v>44777</v>
       </c>
       <c r="F10" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2">
@@ -1577,7 +1577,7 @@
         <v>0</v>
       </c>
       <c r="X10" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y10" s="2">
         <v>0</v>
@@ -1636,7 +1636,7 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
         <v>70</v>
@@ -1943,7 +1943,7 @@
         <v>0</v>
       </c>
       <c r="W13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X13" s="2">
         <v>0</v>
@@ -1979,7 +1979,7 @@
         <v>0</v>
       </c>
       <c r="AI13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ13" s="2">
         <v>1</v>
@@ -2102,10 +2102,10 @@
         <v>0</v>
       </c>
       <c r="AI14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK14" s="2">
         <v>0</v>
@@ -2131,19 +2131,19 @@
         <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D15" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E15" s="1">
         <v>44714</v>
       </c>
       <c r="F15" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2">
@@ -2177,10 +2177,10 @@
         <v>0</v>
       </c>
       <c r="S15" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T15" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U15" s="2">
         <v>0</v>
@@ -2228,7 +2228,7 @@
         <v>0</v>
       </c>
       <c r="AJ15" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK15" s="2">
         <v>0</v>
@@ -2254,7 +2254,7 @@
         <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D16" t="s">
         <v>73</v>
@@ -2263,10 +2263,10 @@
         <v>44714</v>
       </c>
       <c r="F16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2">
@@ -2300,10 +2300,10 @@
         <v>0</v>
       </c>
       <c r="S16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U16" s="2">
         <v>0</v>
@@ -2312,7 +2312,7 @@
         <v>0</v>
       </c>
       <c r="W16" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X16" s="2">
         <v>0</v>
@@ -2351,7 +2351,7 @@
         <v>0</v>
       </c>
       <c r="AJ16" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK16" s="2">
         <v>0</v>
@@ -2503,7 +2503,7 @@
         <v>71</v>
       </c>
       <c r="D18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E18" s="1">
         <v>44714</v>
@@ -2597,7 +2597,7 @@
         <v>0</v>
       </c>
       <c r="AJ18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK18" s="2">
         <v>0</v>
@@ -2749,7 +2749,7 @@
         <v>71</v>
       </c>
       <c r="D20" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E20" s="1">
         <v>44759</v>
@@ -2789,7 +2789,7 @@
         <v>0</v>
       </c>
       <c r="R20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S20" s="2">
         <v>0</v>
@@ -2852,10 +2852,10 @@
         <v>0</v>
       </c>
       <c r="AM20" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN20" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO20" s="2">
         <v>0</v>
@@ -2866,10 +2866,10 @@
         <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="C21" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D21" t="s">
         <v>73</v>
@@ -2878,10 +2878,10 @@
         <v>44759</v>
       </c>
       <c r="F21" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2">
@@ -2978,7 +2978,7 @@
         <v>1</v>
       </c>
       <c r="AN21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO21" s="2">
         <v>0</v>
@@ -2989,13 +2989,13 @@
         <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="C22" t="s">
         <v>70</v>
       </c>
       <c r="D22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E22" s="1">
         <v>44759</v>
@@ -3089,7 +3089,7 @@
         <v>0</v>
       </c>
       <c r="AJ22" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK22" s="2">
         <v>0</v>
@@ -3098,7 +3098,7 @@
         <v>0</v>
       </c>
       <c r="AM22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN22" s="2">
         <v>0</v>
@@ -3112,22 +3112,22 @@
         <v>5</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E23" s="1">
         <v>44759</v>
       </c>
       <c r="F23" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2">
@@ -3140,10 +3140,10 @@
         <v>0</v>
       </c>
       <c r="L23" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M23" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N23" s="2">
         <v>0</v>
@@ -3158,7 +3158,7 @@
         <v>0</v>
       </c>
       <c r="R23" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S23" s="2">
         <v>0</v>
@@ -3197,7 +3197,7 @@
         <v>0</v>
       </c>
       <c r="AE23" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF23" s="2">
         <v>0</v>
@@ -3235,7 +3235,7 @@
         <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C24" t="s">
         <v>70</v>
@@ -3263,10 +3263,10 @@
         <v>0</v>
       </c>
       <c r="L24" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M24" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N24" s="2">
         <v>0</v>
@@ -3347,7 +3347,7 @@
         <v>0</v>
       </c>
       <c r="AN24" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO24" s="2">
         <v>0</v>
@@ -3358,13 +3358,13 @@
         <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="C25" t="s">
         <v>70</v>
       </c>
       <c r="D25" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E25" s="1">
         <v>44759</v>
@@ -3443,7 +3443,7 @@
         <v>0</v>
       </c>
       <c r="AE25" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF25" s="2">
         <v>0</v>
@@ -3458,7 +3458,7 @@
         <v>0</v>
       </c>
       <c r="AJ25" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK25" s="2">
         <v>0</v>
@@ -3470,7 +3470,7 @@
         <v>0</v>
       </c>
       <c r="AN25" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO25" s="2">
         <v>0</v>
@@ -3481,10 +3481,10 @@
         <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D26" t="s">
         <v>73</v>
@@ -3493,10 +3493,10 @@
         <v>44721</v>
       </c>
       <c r="F26" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G26" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H26" s="2"/>
       <c r="I26" s="2">
@@ -3527,7 +3527,7 @@
         <v>0</v>
       </c>
       <c r="R26" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S26" s="2">
         <v>0</v>
@@ -3536,7 +3536,7 @@
         <v>0</v>
       </c>
       <c r="U26" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V26" s="2">
         <v>0</v>
@@ -3581,7 +3581,7 @@
         <v>0</v>
       </c>
       <c r="AJ26" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK26" s="2">
         <v>0</v>
@@ -3604,7 +3604,7 @@
         <v>6</v>
       </c>
       <c r="B27" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C27" t="s">
         <v>71</v>
@@ -3727,10 +3727,10 @@
         <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C28" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D28" t="s">
         <v>73</v>
@@ -3739,10 +3739,10 @@
         <v>44721</v>
       </c>
       <c r="F28" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H28" s="2"/>
       <c r="I28" s="2">
@@ -3773,7 +3773,7 @@
         <v>0</v>
       </c>
       <c r="R28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S28" s="2">
         <v>0</v>
@@ -3782,7 +3782,7 @@
         <v>0</v>
       </c>
       <c r="U28" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V28" s="2">
         <v>0</v>
@@ -3827,7 +3827,7 @@
         <v>0</v>
       </c>
       <c r="AJ28" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK28" s="2">
         <v>0</v>
@@ -3850,10 +3850,10 @@
         <v>7</v>
       </c>
       <c r="B29" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C29" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D29" t="s">
         <v>73</v>
@@ -3862,10 +3862,10 @@
         <v>44707</v>
       </c>
       <c r="F29" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G29" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H29" s="2"/>
       <c r="I29" s="2">
@@ -3884,10 +3884,10 @@
         <v>0</v>
       </c>
       <c r="N29" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O29" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P29" s="2">
         <v>0</v>
@@ -3973,10 +3973,10 @@
         <v>7</v>
       </c>
       <c r="B30" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D30" t="s">
         <v>73</v>
@@ -3985,10 +3985,10 @@
         <v>44707</v>
       </c>
       <c r="F30" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G30" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H30" s="2"/>
       <c r="I30" s="2">
@@ -4007,10 +4007,10 @@
         <v>0</v>
       </c>
       <c r="N30" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O30" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P30" s="2">
         <v>0</v>
@@ -4096,10 +4096,10 @@
         <v>7</v>
       </c>
       <c r="B31" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D31" t="s">
         <v>74</v>
@@ -4108,10 +4108,10 @@
         <v>44707</v>
       </c>
       <c r="F31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G31" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H31" s="2"/>
       <c r="I31" s="2">
@@ -4196,7 +4196,7 @@
         <v>0</v>
       </c>
       <c r="AJ31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK31" s="2">
         <v>0</v>
@@ -4205,7 +4205,7 @@
         <v>0</v>
       </c>
       <c r="AM31" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN31" s="2">
         <v>0</v>
@@ -4322,7 +4322,7 @@
         <v>0</v>
       </c>
       <c r="AK32" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL32" s="2">
         <v>0</v>
@@ -4345,19 +4345,19 @@
         <v>45</v>
       </c>
       <c r="C33" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D33" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E33" s="1">
         <v>44707</v>
       </c>
       <c r="F33" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G33" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H33" s="2"/>
       <c r="I33" s="2">
@@ -4427,7 +4427,7 @@
         <v>0</v>
       </c>
       <c r="AE33" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF33" s="2">
         <v>0</v>
@@ -4445,7 +4445,7 @@
         <v>0</v>
       </c>
       <c r="AK33" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL33" s="2">
         <v>0</v>
@@ -4588,13 +4588,13 @@
         <v>7</v>
       </c>
       <c r="B35" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="C35" t="s">
         <v>70</v>
       </c>
       <c r="D35" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E35" s="1">
         <v>44707</v>
@@ -4616,10 +4616,10 @@
         <v>0</v>
       </c>
       <c r="L35" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M35" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N35" s="2">
         <v>0</v>
@@ -4673,7 +4673,7 @@
         <v>0</v>
       </c>
       <c r="AE35" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF35" s="2">
         <v>0</v>
@@ -4688,7 +4688,7 @@
         <v>0</v>
       </c>
       <c r="AJ35" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK35" s="2">
         <v>0</v>
@@ -4711,7 +4711,7 @@
         <v>7</v>
       </c>
       <c r="B36" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="C36" t="s">
         <v>70</v>
@@ -4739,10 +4739,10 @@
         <v>0</v>
       </c>
       <c r="L36" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M36" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N36" s="2">
         <v>0</v>
@@ -4834,7 +4834,7 @@
         <v>7</v>
       </c>
       <c r="B37" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="C37" t="s">
         <v>71</v>
@@ -4943,7 +4943,7 @@
         <v>0</v>
       </c>
       <c r="AM37" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN37" s="2">
         <v>0</v>
@@ -4957,10 +4957,10 @@
         <v>8</v>
       </c>
       <c r="B38" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C38" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D38" t="s">
         <v>73</v>
@@ -4969,10 +4969,10 @@
         <v>44789</v>
       </c>
       <c r="F38" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G38" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H38" s="2"/>
       <c r="I38" s="2">
@@ -4985,10 +4985,10 @@
         <v>0</v>
       </c>
       <c r="L38" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M38" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N38" s="2">
         <v>0</v>
@@ -5042,7 +5042,7 @@
         <v>0</v>
       </c>
       <c r="AE38" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF38" s="2">
         <v>0</v>
@@ -5066,7 +5066,7 @@
         <v>0</v>
       </c>
       <c r="AM38" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN38" s="2">
         <v>0</v>
@@ -5080,7 +5080,7 @@
         <v>8</v>
       </c>
       <c r="B39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C39" t="s">
         <v>70</v>
@@ -5203,7 +5203,7 @@
         <v>8</v>
       </c>
       <c r="B40" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C40" t="s">
         <v>71</v>
@@ -5326,10 +5326,10 @@
         <v>8</v>
       </c>
       <c r="B41" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C41" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D41" t="s">
         <v>73</v>
@@ -5338,10 +5338,10 @@
         <v>44789</v>
       </c>
       <c r="F41" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G41" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H41" s="2"/>
       <c r="I41" s="2">
@@ -5354,10 +5354,10 @@
         <v>0</v>
       </c>
       <c r="L41" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M41" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N41" s="2">
         <v>0</v>
@@ -5411,7 +5411,7 @@
         <v>0</v>
       </c>
       <c r="AE41" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF41" s="2">
         <v>0</v>
@@ -5435,7 +5435,7 @@
         <v>0</v>
       </c>
       <c r="AM41" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN41" s="2">
         <v>0</v>
@@ -5449,7 +5449,7 @@
         <v>9</v>
       </c>
       <c r="B42" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C42" t="s">
         <v>71</v>
@@ -5534,7 +5534,7 @@
         <v>0</v>
       </c>
       <c r="AE42" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF42" s="2">
         <v>0</v>
@@ -5572,7 +5572,7 @@
         <v>9</v>
       </c>
       <c r="B43" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C43" t="s">
         <v>71</v>
@@ -5695,10 +5695,10 @@
         <v>9</v>
       </c>
       <c r="B44" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="C44" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D44" t="s">
         <v>73</v>
@@ -5707,10 +5707,10 @@
         <v>44818</v>
       </c>
       <c r="F44" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G44" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H44" s="2"/>
       <c r="I44" s="2">
@@ -5723,10 +5723,10 @@
         <v>0</v>
       </c>
       <c r="L44" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M44" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N44" s="2">
         <v>0</v>
@@ -5780,7 +5780,7 @@
         <v>0</v>
       </c>
       <c r="AE44" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF44" s="2">
         <v>0</v>
@@ -5804,7 +5804,7 @@
         <v>0</v>
       </c>
       <c r="AM44" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN44" s="2">
         <v>0</v>
@@ -5818,7 +5818,7 @@
         <v>9</v>
       </c>
       <c r="B45" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C45" t="s">
         <v>71</v>
@@ -5927,7 +5927,7 @@
         <v>0</v>
       </c>
       <c r="AM45" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN45" s="2">
         <v>0</v>
@@ -5941,10 +5941,10 @@
         <v>9</v>
       </c>
       <c r="B46" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="C46" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D46" t="s">
         <v>73</v>
@@ -5953,10 +5953,10 @@
         <v>44818</v>
       </c>
       <c r="F46" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G46" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H46" s="2"/>
       <c r="I46" s="2">
@@ -5975,10 +5975,10 @@
         <v>0</v>
       </c>
       <c r="N46" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O46" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P46" s="2">
         <v>0</v>
@@ -6026,7 +6026,7 @@
         <v>0</v>
       </c>
       <c r="AE46" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF46" s="2">
         <v>0</v>
@@ -6044,13 +6044,13 @@
         <v>0</v>
       </c>
       <c r="AK46" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL46" s="2">
         <v>0</v>
       </c>
       <c r="AM46" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN46" s="2">
         <v>0</v>
@@ -6064,7 +6064,7 @@
         <v>9</v>
       </c>
       <c r="B47" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="C47" t="s">
         <v>71</v>
@@ -6131,7 +6131,7 @@
         <v>0</v>
       </c>
       <c r="Y47" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z47" s="2">
         <v>0</v>
@@ -6149,7 +6149,7 @@
         <v>0</v>
       </c>
       <c r="AE47" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF47" s="2">
         <v>0</v>
@@ -6187,7 +6187,7 @@
         <v>9</v>
       </c>
       <c r="B48" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C48" t="s">
         <v>71</v>
@@ -6310,7 +6310,7 @@
         <v>9</v>
       </c>
       <c r="B49" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="C49" t="s">
         <v>71</v>
@@ -6433,7 +6433,7 @@
         <v>9</v>
       </c>
       <c r="B50" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C50" t="s">
         <v>71</v>
@@ -6556,7 +6556,7 @@
         <v>9</v>
       </c>
       <c r="B51" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C51" t="s">
         <v>71</v>
@@ -6665,7 +6665,7 @@
         <v>0</v>
       </c>
       <c r="AM51" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN51" s="2">
         <v>0</v>
@@ -6679,7 +6679,7 @@
         <v>9</v>
       </c>
       <c r="B52" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="C52" t="s">
         <v>71</v>
@@ -6764,7 +6764,7 @@
         <v>0</v>
       </c>
       <c r="AE52" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF52" s="2">
         <v>0</v>
@@ -6788,7 +6788,7 @@
         <v>0</v>
       </c>
       <c r="AM52" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN52" s="2">
         <v>0</v>
@@ -6802,10 +6802,10 @@
         <v>9</v>
       </c>
       <c r="B53" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="C53" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D53" t="s">
         <v>73</v>
@@ -6814,10 +6814,10 @@
         <v>44818</v>
       </c>
       <c r="F53" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G53" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H53" s="2"/>
       <c r="I53" s="2">
@@ -6836,10 +6836,10 @@
         <v>0</v>
       </c>
       <c r="N53" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O53" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P53" s="2">
         <v>0</v>
@@ -6911,7 +6911,7 @@
         <v>0</v>
       </c>
       <c r="AM53" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN53" s="2">
         <v>0</v>
@@ -6925,10 +6925,10 @@
         <v>9</v>
       </c>
       <c r="B54" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="C54" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D54" t="s">
         <v>73</v>
@@ -6937,10 +6937,10 @@
         <v>44818</v>
       </c>
       <c r="F54" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G54" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H54" s="2"/>
       <c r="I54" s="2">
@@ -7010,7 +7010,7 @@
         <v>0</v>
       </c>
       <c r="AE54" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF54" s="2">
         <v>0</v>
@@ -7028,13 +7028,13 @@
         <v>0</v>
       </c>
       <c r="AK54" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL54" s="2">
         <v>0</v>
       </c>
       <c r="AM54" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN54" s="2">
         <v>0</v>
@@ -7048,7 +7048,7 @@
         <v>9</v>
       </c>
       <c r="B55" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="C55" t="s">
         <v>71</v>
@@ -7115,7 +7115,7 @@
         <v>0</v>
       </c>
       <c r="Y55" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z55" s="2">
         <v>0</v>
@@ -7133,7 +7133,7 @@
         <v>0</v>
       </c>
       <c r="AE55" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF55" s="2">
         <v>0</v>
@@ -7171,7 +7171,7 @@
         <v>9</v>
       </c>
       <c r="B56" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C56" t="s">
         <v>70</v>
@@ -7199,10 +7199,10 @@
         <v>0</v>
       </c>
       <c r="L56" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M56" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N56" s="2">
         <v>0</v>
@@ -7256,7 +7256,7 @@
         <v>0</v>
       </c>
       <c r="AE56" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF56" s="2">
         <v>0</v>
@@ -7280,7 +7280,7 @@
         <v>0</v>
       </c>
       <c r="AM56" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN56" s="2">
         <v>0</v>
@@ -7294,10 +7294,10 @@
         <v>10</v>
       </c>
       <c r="B57" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="C57" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D57" t="s">
         <v>73</v>
@@ -7306,10 +7306,10 @@
         <v>44771</v>
       </c>
       <c r="F57" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G57" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H57" s="2"/>
       <c r="I57" s="2">
@@ -7376,10 +7376,10 @@
         <v>0</v>
       </c>
       <c r="AD57" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE57" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF57" s="2">
         <v>0</v>
@@ -7403,7 +7403,7 @@
         <v>0</v>
       </c>
       <c r="AM57" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN57" s="2">
         <v>0</v>
@@ -7417,7 +7417,7 @@
         <v>10</v>
       </c>
       <c r="B58" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="C58" t="s">
         <v>70</v>
@@ -7540,7 +7540,7 @@
         <v>10</v>
       </c>
       <c r="B59" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C59" t="s">
         <v>70</v>
@@ -7625,7 +7625,7 @@
         <v>0</v>
       </c>
       <c r="AE59" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF59" s="2">
         <v>0</v>
@@ -7663,22 +7663,22 @@
         <v>10</v>
       </c>
       <c r="B60" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="C60" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D60" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E60" s="1">
         <v>44771</v>
       </c>
       <c r="F60" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G60" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H60" s="2"/>
       <c r="I60" s="2">
@@ -7709,7 +7709,7 @@
         <v>0</v>
       </c>
       <c r="R60" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S60" s="2">
         <v>0</v>
@@ -7763,7 +7763,7 @@
         <v>0</v>
       </c>
       <c r="AJ60" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK60" s="2">
         <v>0</v>
@@ -7786,7 +7786,7 @@
         <v>10</v>
       </c>
       <c r="B61" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C61" t="s">
         <v>70</v>
@@ -7844,7 +7844,7 @@
         <v>0</v>
       </c>
       <c r="V61" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W61" s="2">
         <v>0</v>
@@ -7868,10 +7868,10 @@
         <v>0</v>
       </c>
       <c r="AD61" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE61" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF61" s="2">
         <v>0</v>
@@ -7909,10 +7909,10 @@
         <v>10</v>
       </c>
       <c r="B62" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C62" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D62" t="s">
         <v>73</v>
@@ -7921,10 +7921,10 @@
         <v>44771</v>
       </c>
       <c r="F62" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G62" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H62" s="2"/>
       <c r="I62" s="2">
@@ -7937,10 +7937,10 @@
         <v>0</v>
       </c>
       <c r="L62" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M62" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N62" s="2">
         <v>0</v>
@@ -8012,7 +8012,7 @@
         <v>0</v>
       </c>
       <c r="AK62" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL62" s="2">
         <v>0</v>
@@ -8032,13 +8032,13 @@
         <v>10</v>
       </c>
       <c r="B63" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="C63" t="s">
         <v>70</v>
       </c>
       <c r="D63" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E63" s="1">
         <v>44771</v>
@@ -8060,10 +8060,10 @@
         <v>0</v>
       </c>
       <c r="L63" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M63" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N63" s="2">
         <v>0</v>
@@ -8117,7 +8117,7 @@
         <v>0</v>
       </c>
       <c r="AE63" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF63" s="2">
         <v>0</v>
@@ -8132,7 +8132,7 @@
         <v>0</v>
       </c>
       <c r="AJ63" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK63" s="2">
         <v>0</v>
@@ -8155,7 +8155,7 @@
         <v>10</v>
       </c>
       <c r="B64" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="C64" t="s">
         <v>70</v>
@@ -8237,7 +8237,7 @@
         <v>0</v>
       </c>
       <c r="AD64" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE64" s="2">
         <v>1</v>
@@ -8278,7 +8278,7 @@
         <v>10</v>
       </c>
       <c r="B65" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="C65" t="s">
         <v>70</v>
@@ -8363,7 +8363,7 @@
         <v>0</v>
       </c>
       <c r="AE65" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF65" s="2">
         <v>0</v>
@@ -8387,7 +8387,7 @@
         <v>0</v>
       </c>
       <c r="AM65" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN65" s="2">
         <v>0</v>
@@ -8401,10 +8401,10 @@
         <v>10</v>
       </c>
       <c r="B66" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="C66" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D66" t="s">
         <v>73</v>
@@ -8413,10 +8413,10 @@
         <v>44771</v>
       </c>
       <c r="F66" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G66" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H66" s="2"/>
       <c r="I66" s="2">
@@ -8447,7 +8447,7 @@
         <v>0</v>
       </c>
       <c r="R66" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S66" s="2">
         <v>0</v>
@@ -8483,10 +8483,10 @@
         <v>0</v>
       </c>
       <c r="AD66" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE66" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF66" s="2">
         <v>0</v>
@@ -8524,10 +8524,10 @@
         <v>10</v>
       </c>
       <c r="B67" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C67" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D67" t="s">
         <v>73</v>
@@ -8536,10 +8536,10 @@
         <v>44771</v>
       </c>
       <c r="F67" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G67" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H67" s="2"/>
       <c r="I67" s="2">
@@ -8609,7 +8609,7 @@
         <v>0</v>
       </c>
       <c r="AE67" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF67" s="2">
         <v>0</v>
@@ -8627,7 +8627,7 @@
         <v>0</v>
       </c>
       <c r="AK67" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL67" s="2">
         <v>0</v>
@@ -8647,22 +8647,22 @@
         <v>10</v>
       </c>
       <c r="B68" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C68" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D68" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E68" s="1">
         <v>44771</v>
       </c>
       <c r="F68" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G68" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H68" s="2"/>
       <c r="I68" s="2">
@@ -8770,10 +8770,10 @@
         <v>10</v>
       </c>
       <c r="B69" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C69" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D69" t="s">
         <v>73</v>
@@ -8782,10 +8782,10 @@
         <v>44771</v>
       </c>
       <c r="F69" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G69" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H69" s="2"/>
       <c r="I69" s="2">
@@ -8855,7 +8855,7 @@
         <v>0</v>
       </c>
       <c r="AE69" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF69" s="2">
         <v>0</v>
@@ -8870,7 +8870,7 @@
         <v>0</v>
       </c>
       <c r="AJ69" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK69" s="2">
         <v>0</v>
@@ -8893,10 +8893,10 @@
         <v>10</v>
       </c>
       <c r="B70" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
       <c r="C70" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D70" t="s">
         <v>73</v>
@@ -8905,10 +8905,10 @@
         <v>44771</v>
       </c>
       <c r="F70" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G70" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H70" s="2"/>
       <c r="I70" s="2">
@@ -8951,7 +8951,7 @@
         <v>0</v>
       </c>
       <c r="V70" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W70" s="2">
         <v>0</v>
@@ -9002,7 +9002,7 @@
         <v>0</v>
       </c>
       <c r="AM70" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN70" s="2">
         <v>0</v>
@@ -9016,13 +9016,13 @@
         <v>10</v>
       </c>
       <c r="B71" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="C71" t="s">
         <v>70</v>
       </c>
       <c r="D71" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E71" s="1">
         <v>44771</v>
@@ -9116,7 +9116,7 @@
         <v>0</v>
       </c>
       <c r="AJ71" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK71" s="2">
         <v>0</v>
@@ -9125,7 +9125,7 @@
         <v>0</v>
       </c>
       <c r="AM71" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN71" s="2">
         <v>0</v>
@@ -9139,10 +9139,10 @@
         <v>11</v>
       </c>
       <c r="B72" t="s">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="C72" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D72" t="s">
         <v>73</v>
@@ -9151,10 +9151,10 @@
         <v>44845</v>
       </c>
       <c r="F72" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G72" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H72" s="2"/>
       <c r="I72" s="2">
@@ -9262,7 +9262,7 @@
         <v>11</v>
       </c>
       <c r="B73" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C73" t="s">
         <v>70</v>
@@ -9385,10 +9385,10 @@
         <v>11</v>
       </c>
       <c r="B74" t="s">
-        <v>60</v>
+        <v>23</v>
       </c>
       <c r="C74" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D74" t="s">
         <v>73</v>
@@ -9397,10 +9397,10 @@
         <v>44845</v>
       </c>
       <c r="F74" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G74" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H74" s="2"/>
       <c r="I74" s="2">
@@ -9508,7 +9508,7 @@
         <v>12</v>
       </c>
       <c r="B75" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C75" t="s">
         <v>70</v>
@@ -9631,7 +9631,7 @@
         <v>13</v>
       </c>
       <c r="B76" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="C76" t="s">
         <v>70</v>
@@ -9659,10 +9659,10 @@
         <v>0</v>
       </c>
       <c r="L76" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M76" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N76" s="2">
         <v>0</v>
@@ -9754,7 +9754,7 @@
         <v>13</v>
       </c>
       <c r="B77" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="C77" t="s">
         <v>70</v>
@@ -9803,10 +9803,10 @@
         <v>0</v>
       </c>
       <c r="S77" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T77" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U77" s="2">
         <v>0</v>
@@ -9863,7 +9863,7 @@
         <v>0</v>
       </c>
       <c r="AM77" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN77" s="2">
         <v>0</v>
@@ -9877,7 +9877,7 @@
         <v>13</v>
       </c>
       <c r="B78" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C78" t="s">
         <v>70</v>
@@ -9905,16 +9905,16 @@
         <v>0</v>
       </c>
       <c r="L78" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M78" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N78" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O78" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P78" s="2">
         <v>0</v>
@@ -9962,7 +9962,7 @@
         <v>0</v>
       </c>
       <c r="AE78" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF78" s="2">
         <v>0</v>
@@ -9986,7 +9986,7 @@
         <v>0</v>
       </c>
       <c r="AM78" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN78" s="2">
         <v>0</v>
@@ -10000,7 +10000,7 @@
         <v>13</v>
       </c>
       <c r="B79" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C79" t="s">
         <v>70</v>
@@ -10049,10 +10049,10 @@
         <v>0</v>
       </c>
       <c r="S79" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T79" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U79" s="2">
         <v>0</v>
@@ -10109,7 +10109,7 @@
         <v>0</v>
       </c>
       <c r="AM79" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN79" s="2">
         <v>0</v>
@@ -10123,7 +10123,7 @@
         <v>13</v>
       </c>
       <c r="B80" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="C80" t="s">
         <v>70</v>
@@ -10157,10 +10157,10 @@
         <v>0</v>
       </c>
       <c r="N80" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O80" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P80" s="2">
         <v>0</v>
@@ -10208,7 +10208,7 @@
         <v>0</v>
       </c>
       <c r="AE80" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF80" s="2">
         <v>0</v>
@@ -10232,7 +10232,7 @@
         <v>0</v>
       </c>
       <c r="AM80" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN80" s="2">
         <v>0</v>
@@ -10372,7 +10372,7 @@
         <v>62</v>
       </c>
       <c r="C82" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D82" t="s">
         <v>73</v>
@@ -10381,10 +10381,10 @@
         <v>44894</v>
       </c>
       <c r="F82" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G82" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H82" s="2"/>
       <c r="I82" s="2">
@@ -10478,7 +10478,7 @@
         <v>0</v>
       </c>
       <c r="AM82" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN82" s="2">
         <v>0</v>
@@ -10492,7 +10492,7 @@
         <v>14</v>
       </c>
       <c r="B83" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C83" t="s">
         <v>70</v>
@@ -10615,7 +10615,7 @@
         <v>14</v>
       </c>
       <c r="B84" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="C84" t="s">
         <v>71</v>
@@ -10724,10 +10724,10 @@
         <v>0</v>
       </c>
       <c r="AM84" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN84" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO84" s="2">
         <v>0</v>
@@ -10741,7 +10741,7 @@
         <v>63</v>
       </c>
       <c r="C85" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D85" t="s">
         <v>73</v>
@@ -10750,10 +10750,10 @@
         <v>44894</v>
       </c>
       <c r="F85" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G85" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H85" s="2"/>
       <c r="I85" s="2">
@@ -10861,7 +10861,7 @@
         <v>14</v>
       </c>
       <c r="B86" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C86" t="s">
         <v>70</v>
@@ -11339,7 +11339,7 @@
         <v>0</v>
       </c>
       <c r="AM89" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN89" s="2">
         <v>0</v>
@@ -11353,7 +11353,7 @@
         <v>14</v>
       </c>
       <c r="B90" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="C90" t="s">
         <v>71</v>
@@ -11462,10 +11462,10 @@
         <v>0</v>
       </c>
       <c r="AM90" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN90" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO90" s="2">
         <v>0</v>
@@ -11476,7 +11476,7 @@
         <v>15</v>
       </c>
       <c r="B91" t="s">
-        <v>66</v>
+        <v>26</v>
       </c>
       <c r="C91" t="s">
         <v>71</v>
@@ -11561,7 +11561,7 @@
         <v>0</v>
       </c>
       <c r="AE91" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF91" s="2">
         <v>0</v>
@@ -11599,7 +11599,7 @@
         <v>15</v>
       </c>
       <c r="B92" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="C92" t="s">
         <v>70</v>
@@ -11654,7 +11654,7 @@
         <v>0</v>
       </c>
       <c r="U92" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V92" s="2">
         <v>0</v>
@@ -11722,10 +11722,10 @@
         <v>15</v>
       </c>
       <c r="B93" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C93" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D93" t="s">
         <v>73</v>
@@ -11734,10 +11734,10 @@
         <v>44865</v>
       </c>
       <c r="F93" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G93" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H93" s="2"/>
       <c r="I93" s="2">
@@ -11807,7 +11807,7 @@
         <v>0</v>
       </c>
       <c r="AE93" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF93" s="2">
         <v>0</v>
@@ -11831,7 +11831,7 @@
         <v>0</v>
       </c>
       <c r="AM93" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN93" s="2">
         <v>0</v>
@@ -11845,10 +11845,10 @@
         <v>15</v>
       </c>
       <c r="B94" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="C94" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D94" t="s">
         <v>73</v>
@@ -11857,10 +11857,10 @@
         <v>44865</v>
       </c>
       <c r="F94" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G94" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H94" s="2"/>
       <c r="I94" s="2">
@@ -11945,7 +11945,7 @@
         <v>0</v>
       </c>
       <c r="AJ94" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK94" s="2">
         <v>0</v>
@@ -11954,7 +11954,7 @@
         <v>0</v>
       </c>
       <c r="AM94" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN94" s="2">
         <v>0</v>
@@ -11968,7 +11968,7 @@
         <v>15</v>
       </c>
       <c r="B95" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C95" t="s">
         <v>71</v>
@@ -12068,7 +12068,7 @@
         <v>0</v>
       </c>
       <c r="AJ95" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK95" s="2">
         <v>0</v>
@@ -12077,7 +12077,7 @@
         <v>0</v>
       </c>
       <c r="AM95" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN95" s="2">
         <v>0</v>
@@ -12091,7 +12091,7 @@
         <v>15</v>
       </c>
       <c r="B96" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C96" t="s">
         <v>70</v>
@@ -12191,7 +12191,7 @@
         <v>0</v>
       </c>
       <c r="AJ96" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK96" s="2">
         <v>0</v>
@@ -12214,7 +12214,7 @@
         <v>15</v>
       </c>
       <c r="B97" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C97" t="s">
         <v>70</v>
@@ -12337,10 +12337,10 @@
         <v>15</v>
       </c>
       <c r="B98" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="C98" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D98" t="s">
         <v>73</v>
@@ -12349,10 +12349,10 @@
         <v>44865</v>
       </c>
       <c r="F98" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G98" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H98" s="2"/>
       <c r="I98" s="2">
@@ -12460,10 +12460,10 @@
         <v>15</v>
       </c>
       <c r="B99" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C99" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D99" t="s">
         <v>73</v>
@@ -12472,10 +12472,10 @@
         <v>44865</v>
       </c>
       <c r="F99" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G99" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H99" s="2"/>
       <c r="I99" s="2">
@@ -12515,7 +12515,7 @@
         <v>0</v>
       </c>
       <c r="U99" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V99" s="2">
         <v>0</v>
@@ -12560,7 +12560,7 @@
         <v>0</v>
       </c>
       <c r="AJ99" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK99" s="2">
         <v>0</v>
@@ -12569,7 +12569,7 @@
         <v>0</v>
       </c>
       <c r="AM99" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN99" s="2">
         <v>0</v>
@@ -12583,7 +12583,7 @@
         <v>16</v>
       </c>
       <c r="B100" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C100" t="s">
         <v>71</v>
@@ -12629,7 +12629,7 @@
         <v>0</v>
       </c>
       <c r="R100" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S100" s="2">
         <v>0</v>
@@ -12650,7 +12650,7 @@
         <v>0</v>
       </c>
       <c r="Y100" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z100" s="2">
         <v>0</v>
@@ -12668,7 +12668,7 @@
         <v>0</v>
       </c>
       <c r="AE100" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF100" s="2">
         <v>0</v>
@@ -12706,7 +12706,7 @@
         <v>16</v>
       </c>
       <c r="B101" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C101" t="s">
         <v>70</v>
@@ -12734,10 +12734,10 @@
         <v>0</v>
       </c>
       <c r="L101" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M101" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N101" s="2">
         <v>0</v>
@@ -12791,7 +12791,7 @@
         <v>0</v>
       </c>
       <c r="AE101" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF101" s="2">
         <v>0</v>
@@ -12815,7 +12815,7 @@
         <v>0</v>
       </c>
       <c r="AM101" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN101" s="2">
         <v>0</v>
@@ -12832,7 +12832,7 @@
         <v>51</v>
       </c>
       <c r="C102" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D102" t="s">
         <v>73</v>
@@ -12841,10 +12841,10 @@
         <v>44879</v>
       </c>
       <c r="F102" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G102" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H102" s="2"/>
       <c r="I102" s="2">
@@ -12938,7 +12938,7 @@
         <v>0</v>
       </c>
       <c r="AM102" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN102" s="2">
         <v>0</v>
@@ -12952,7 +12952,7 @@
         <v>16</v>
       </c>
       <c r="B103" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C103" t="s">
         <v>70</v>
@@ -12980,10 +12980,10 @@
         <v>0</v>
       </c>
       <c r="L103" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M103" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N103" s="2">
         <v>0</v>
@@ -13037,7 +13037,7 @@
         <v>0</v>
       </c>
       <c r="AE103" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF103" s="2">
         <v>0</v>
@@ -13061,7 +13061,7 @@
         <v>0</v>
       </c>
       <c r="AM103" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN103" s="2">
         <v>0</v>
@@ -13075,7 +13075,7 @@
         <v>16</v>
       </c>
       <c r="B104" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="C104" t="s">
         <v>71</v>
@@ -13142,7 +13142,7 @@
         <v>0</v>
       </c>
       <c r="Y104" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z104" s="2">
         <v>0</v>
@@ -13160,7 +13160,7 @@
         <v>0</v>
       </c>
       <c r="AE104" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF104" s="2">
         <v>0</v>
@@ -13184,7 +13184,7 @@
         <v>0</v>
       </c>
       <c r="AM104" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN104" s="2">
         <v>0</v>
@@ -13198,10 +13198,10 @@
         <v>16</v>
       </c>
       <c r="B105" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C105" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D105" t="s">
         <v>73</v>
@@ -13210,10 +13210,10 @@
         <v>44879</v>
       </c>
       <c r="F105" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G105" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H105" s="2"/>
       <c r="I105" s="2">
@@ -13307,7 +13307,7 @@
         <v>0</v>
       </c>
       <c r="AM105" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN105" s="2">
         <v>0</v>
@@ -13321,7 +13321,7 @@
         <v>16</v>
       </c>
       <c r="B106" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C106" t="s">
         <v>71</v>
@@ -13367,7 +13367,7 @@
         <v>0</v>
       </c>
       <c r="R106" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S106" s="2">
         <v>0</v>
@@ -13430,7 +13430,7 @@
         <v>0</v>
       </c>
       <c r="AM106" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN106" s="2">
         <v>0</v>
@@ -13444,7 +13444,7 @@
         <v>17</v>
       </c>
       <c r="B107" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C107" t="s">
         <v>71</v>
@@ -13567,7 +13567,7 @@
         <v>17</v>
       </c>
       <c r="B108" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C108" t="s">
         <v>70</v>
@@ -13690,10 +13690,10 @@
         <v>18</v>
       </c>
       <c r="B109" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C109" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D109" t="s">
         <v>73</v>
@@ -13702,10 +13702,10 @@
         <v>44887</v>
       </c>
       <c r="F109" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G109" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H109" s="2"/>
       <c r="I109" s="2">
@@ -13751,7 +13751,7 @@
         <v>0</v>
       </c>
       <c r="W109" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X109" s="2">
         <v>0</v>
@@ -13787,7 +13787,7 @@
         <v>0</v>
       </c>
       <c r="AI109" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ109" s="2">
         <v>1</v>
@@ -13813,10 +13813,10 @@
         <v>18</v>
       </c>
       <c r="B110" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C110" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D110" t="s">
         <v>73</v>
@@ -13825,10 +13825,10 @@
         <v>44887</v>
       </c>
       <c r="F110" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G110" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H110" s="2"/>
       <c r="I110" s="2">
@@ -13910,10 +13910,10 @@
         <v>0</v>
       </c>
       <c r="AI110" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ110" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK110" s="2">
         <v>0</v>
@@ -13936,7 +13936,7 @@
         <v>18</v>
       </c>
       <c r="B111" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C111" t="s">
         <v>70</v>
@@ -13985,10 +13985,10 @@
         <v>0</v>
       </c>
       <c r="S111" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T111" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U111" s="2">
         <v>0</v>
@@ -14059,10 +14059,10 @@
         <v>18</v>
       </c>
       <c r="B112" t="s">
-        <v>67</v>
+        <v>32</v>
       </c>
       <c r="C112" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D112" t="s">
         <v>73</v>
@@ -14071,10 +14071,10 @@
         <v>44887</v>
       </c>
       <c r="F112" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G112" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H112" s="2"/>
       <c r="I112" s="2">
@@ -14120,7 +14120,7 @@
         <v>0</v>
       </c>
       <c r="W112" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X112" s="2">
         <v>0</v>
@@ -14159,7 +14159,7 @@
         <v>0</v>
       </c>
       <c r="AJ112" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK112" s="2">
         <v>0</v>
@@ -14182,10 +14182,10 @@
         <v>18</v>
       </c>
       <c r="B113" t="s">
-        <v>34</v>
+        <v>67</v>
       </c>
       <c r="C113" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D113" t="s">
         <v>73</v>
@@ -14194,10 +14194,10 @@
         <v>44887</v>
       </c>
       <c r="F113" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G113" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H113" s="2"/>
       <c r="I113" s="2">
@@ -14231,10 +14231,10 @@
         <v>0</v>
       </c>
       <c r="S113" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T113" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U113" s="2">
         <v>0</v>
@@ -14305,7 +14305,7 @@
         <v>19</v>
       </c>
       <c r="B114" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C114" t="s">
         <v>70</v>
@@ -14434,7 +14434,7 @@
         <v>70</v>
       </c>
       <c r="D115" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E115" s="1">
         <v>44714</v>
@@ -14559,7 +14559,7 @@
         <v>70</v>
       </c>
       <c r="D116" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E116" s="1">
         <v>44714</v>

</xml_diff>

<commit_message>
update results and pending
</commit_message>
<xml_diff>
--- a/datasets/lab_detail.xlsx
+++ b/datasets/lab_detail.xlsx
@@ -81,40 +81,43 @@
     <t>substance</t>
   </si>
   <si>
-    <t>4-ANPP</t>
+    <t>p-fluorofentanyl</t>
+  </si>
+  <si>
+    <t>dimethyl sulfone (methylsulfonylmethane MSM)</t>
+  </si>
+  <si>
+    <t>fentanyl</t>
   </si>
   <si>
     <t>despropionyl p-fluorofentanyl</t>
   </si>
   <si>
-    <t>dimethyl sulfone (methylsulfonylmethane MSM)</t>
+    <t>4-ANPP</t>
+  </si>
+  <si>
+    <t>xylazine</t>
   </si>
   <si>
     <t>phenethyl 4-ANPP</t>
   </si>
   <si>
-    <t>fentanyl</t>
-  </si>
-  <si>
-    <t>p-fluorofentanyl</t>
-  </si>
-  <si>
-    <t>xylazine</t>
+    <t>3,4-MDMA</t>
   </si>
   <si>
     <t>3,4-methylenedioxy-N-benzylcathinone (BMDP)</t>
   </si>
   <si>
-    <t>3,4-MDMA</t>
+    <t>methyl ecgonidine (MED)</t>
   </si>
   <si>
-    <t>phenacetin</t>
+    <t>levamisole</t>
+  </si>
+  <si>
+    <t>norcocaine</t>
   </si>
   <si>
     <t>tropacocaine</t>
-  </si>
-  <si>
-    <t>levamisole</t>
   </si>
   <si>
     <t>cocaine</t>
@@ -123,10 +126,13 @@
     <t>benzoylecgonine (BZ)</t>
   </si>
   <si>
-    <t>norcocaine</t>
+    <t>phenacetin</t>
   </si>
   <si>
-    <t>methyl ecgonidine (MED)</t>
+    <t>p-fluoro phenethyl 4-ANPP</t>
+  </si>
+  <si>
+    <t>methamphetamine</t>
   </si>
   <si>
     <t>tramadol</t>
@@ -135,55 +141,46 @@
     <t>non-specific sugars</t>
   </si>
   <si>
-    <t>methamphetamine</t>
-  </si>
-  <si>
-    <t>p-fluoro phenethyl 4-ANPP</t>
+    <t>eutylone</t>
   </si>
   <si>
     <t>caffeine</t>
   </si>
   <si>
-    <t>eutylone</t>
+    <t>heroin</t>
   </si>
   <si>
-    <t>heroin</t>
+    <t>6-monoacetylmorphine (6-MAM)</t>
+  </si>
+  <si>
+    <t>acetylcodeine</t>
   </si>
   <si>
     <t>urea</t>
   </si>
   <si>
-    <t>acetylcodeine</t>
-  </si>
-  <si>
-    <t>6-monoacetylmorphine (6-MAM)</t>
-  </si>
-  <si>
     <t>1,3-Diacetin</t>
   </si>
   <si>
-    <t>N-phenylpropanamide</t>
+    <t>lidocaine</t>
   </si>
   <si>
     <t>N-ethyl-4-ANPP</t>
   </si>
   <si>
-    <t>lidocaine</t>
-  </si>
-  <si>
     <t>acetaminophen</t>
   </si>
   <si>
-    <t>N-piperidinyl etonitazene</t>
-  </si>
-  <si>
-    <t>quinine</t>
+    <t>N-phenylpropanamide</t>
   </si>
   <si>
     <t>diphenhydramine</t>
   </si>
   <si>
     <t>gabapentin</t>
+  </si>
+  <si>
+    <t>N-piperidinyl etonitazene</t>
   </si>
   <si>
     <t>methadone</t>
@@ -193,6 +190,9 @@
   </si>
   <si>
     <t>metonitazene</t>
+  </si>
+  <si>
+    <t>quinine</t>
   </si>
   <si>
     <t>non-specific organic acids</t>
@@ -207,10 +207,10 @@
     <t>menthol</t>
   </si>
   <si>
-    <t>phenethyl chloride</t>
+    <t>nicotine</t>
   </si>
   <si>
-    <t>nicotine</t>
+    <t>phenethyl chloride</t>
   </si>
   <si>
     <t>1-phenethyl-4-propionyloxypiperidine</t>
@@ -614,7 +614,7 @@
         <v>0</v>
       </c>
       <c r="AE2" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF2" s="2">
         <v>0</v>
@@ -638,7 +638,7 @@
         <v>0</v>
       </c>
       <c r="AM2" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN2" s="2">
         <v>0</v>
@@ -737,7 +737,7 @@
         <v>0</v>
       </c>
       <c r="AE3" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF3" s="2">
         <v>0</v>
@@ -764,7 +764,7 @@
         <v>0</v>
       </c>
       <c r="AN3" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO3" s="2">
         <v>0</v>
@@ -803,10 +803,10 @@
         <v>0</v>
       </c>
       <c r="L4" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M4" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N4" s="2">
         <v>0</v>
@@ -860,7 +860,7 @@
         <v>0</v>
       </c>
       <c r="AE4" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF4" s="2">
         <v>0</v>
@@ -983,7 +983,7 @@
         <v>0</v>
       </c>
       <c r="AE5" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF5" s="2">
         <v>0</v>
@@ -1007,10 +1007,10 @@
         <v>0</v>
       </c>
       <c r="AM5" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN5" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO5" s="2">
         <v>0</v>
@@ -1049,10 +1049,10 @@
         <v>0</v>
       </c>
       <c r="L6" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M6" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N6" s="2">
         <v>0</v>
@@ -1106,7 +1106,7 @@
         <v>0</v>
       </c>
       <c r="AE6" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF6" s="2">
         <v>0</v>
@@ -1130,7 +1130,7 @@
         <v>0</v>
       </c>
       <c r="AM6" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN6" s="2">
         <v>0</v>
@@ -1178,10 +1178,10 @@
         <v>0</v>
       </c>
       <c r="N7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P7" s="2">
         <v>0</v>
@@ -1229,7 +1229,7 @@
         <v>0</v>
       </c>
       <c r="AE7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF7" s="2">
         <v>0</v>
@@ -1253,7 +1253,7 @@
         <v>0</v>
       </c>
       <c r="AM7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN7" s="2">
         <v>0</v>
@@ -1301,10 +1301,10 @@
         <v>0</v>
       </c>
       <c r="N8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P8" s="2">
         <v>0</v>
@@ -1393,7 +1393,7 @@
         <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D9" t="s">
         <v>73</v>
@@ -1402,10 +1402,10 @@
         <v>44777</v>
       </c>
       <c r="F9" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2">
@@ -1454,7 +1454,7 @@
         <v>0</v>
       </c>
       <c r="X9" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y9" s="2">
         <v>0</v>
@@ -1516,7 +1516,7 @@
         <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D10" t="s">
         <v>73</v>
@@ -1525,10 +1525,10 @@
         <v>44777</v>
       </c>
       <c r="F10" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2">
@@ -1577,7 +1577,7 @@
         <v>0</v>
       </c>
       <c r="X10" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y10" s="2">
         <v>0</v>
@@ -1636,7 +1636,7 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
         <v>70</v>
@@ -1765,7 +1765,7 @@
         <v>71</v>
       </c>
       <c r="D12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E12" s="1">
         <v>44714</v>
@@ -1859,7 +1859,7 @@
         <v>0</v>
       </c>
       <c r="AJ12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK12" s="2">
         <v>0</v>
@@ -1943,7 +1943,7 @@
         <v>0</v>
       </c>
       <c r="W13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X13" s="2">
         <v>0</v>
@@ -1979,7 +1979,7 @@
         <v>0</v>
       </c>
       <c r="AI13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ13" s="2">
         <v>1</v>
@@ -2066,7 +2066,7 @@
         <v>0</v>
       </c>
       <c r="W14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X14" s="2">
         <v>0</v>
@@ -2102,10 +2102,10 @@
         <v>0</v>
       </c>
       <c r="AI14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK14" s="2">
         <v>0</v>
@@ -2131,7 +2131,7 @@
         <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D15" t="s">
         <v>73</v>
@@ -2140,10 +2140,10 @@
         <v>44714</v>
       </c>
       <c r="F15" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2">
@@ -2177,10 +2177,10 @@
         <v>0</v>
       </c>
       <c r="S15" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T15" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U15" s="2">
         <v>0</v>
@@ -2225,10 +2225,10 @@
         <v>0</v>
       </c>
       <c r="AI15" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ15" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK15" s="2">
         <v>0</v>
@@ -2254,19 +2254,19 @@
         <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E16" s="1">
         <v>44714</v>
       </c>
       <c r="F16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2">
@@ -2300,10 +2300,10 @@
         <v>0</v>
       </c>
       <c r="S16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U16" s="2">
         <v>0</v>
@@ -2380,7 +2380,7 @@
         <v>71</v>
       </c>
       <c r="D17" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E17" s="1">
         <v>44714</v>
@@ -2471,7 +2471,7 @@
         <v>0</v>
       </c>
       <c r="AI17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ17" s="2">
         <v>0</v>
@@ -2503,7 +2503,7 @@
         <v>71</v>
       </c>
       <c r="D18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E18" s="1">
         <v>44714</v>
@@ -2597,7 +2597,7 @@
         <v>0</v>
       </c>
       <c r="AJ18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK18" s="2">
         <v>0</v>
@@ -2687,7 +2687,7 @@
         <v>0</v>
       </c>
       <c r="Y19" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z19" s="2">
         <v>0</v>
@@ -2705,7 +2705,7 @@
         <v>0</v>
       </c>
       <c r="AE19" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF19" s="2">
         <v>0</v>
@@ -2729,10 +2729,10 @@
         <v>0</v>
       </c>
       <c r="AM19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO19" s="2">
         <v>0</v>
@@ -2746,7 +2746,7 @@
         <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D20" t="s">
         <v>74</v>
@@ -2755,10 +2755,10 @@
         <v>44759</v>
       </c>
       <c r="F20" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2">
@@ -2789,7 +2789,7 @@
         <v>0</v>
       </c>
       <c r="R20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S20" s="2">
         <v>0</v>
@@ -2843,7 +2843,7 @@
         <v>0</v>
       </c>
       <c r="AJ20" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK20" s="2">
         <v>0</v>
@@ -2866,7 +2866,7 @@
         <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C21" t="s">
         <v>70</v>
@@ -2894,10 +2894,10 @@
         <v>0</v>
       </c>
       <c r="L21" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M21" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N21" s="2">
         <v>0</v>
@@ -2978,7 +2978,7 @@
         <v>0</v>
       </c>
       <c r="AN21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO21" s="2">
         <v>0</v>
@@ -2989,7 +2989,7 @@
         <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C22" t="s">
         <v>70</v>
@@ -3017,10 +3017,10 @@
         <v>0</v>
       </c>
       <c r="L22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N22" s="2">
         <v>0</v>
@@ -3101,7 +3101,7 @@
         <v>0</v>
       </c>
       <c r="AN22" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO22" s="2">
         <v>0</v>
@@ -3118,7 +3118,7 @@
         <v>71</v>
       </c>
       <c r="D23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E23" s="1">
         <v>44759</v>
@@ -3158,7 +3158,7 @@
         <v>0</v>
       </c>
       <c r="R23" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S23" s="2">
         <v>0</v>
@@ -3179,7 +3179,7 @@
         <v>0</v>
       </c>
       <c r="Y23" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z23" s="2">
         <v>0</v>
@@ -3197,7 +3197,7 @@
         <v>0</v>
       </c>
       <c r="AE23" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF23" s="2">
         <v>0</v>
@@ -3235,13 +3235,13 @@
         <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="C24" t="s">
         <v>70</v>
       </c>
       <c r="D24" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E24" s="1">
         <v>44759</v>
@@ -3335,7 +3335,7 @@
         <v>0</v>
       </c>
       <c r="AJ24" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK24" s="2">
         <v>0</v>
@@ -3344,7 +3344,7 @@
         <v>0</v>
       </c>
       <c r="AM24" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN24" s="2">
         <v>0</v>
@@ -3358,10 +3358,10 @@
         <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D25" t="s">
         <v>73</v>
@@ -3370,10 +3370,10 @@
         <v>44759</v>
       </c>
       <c r="F25" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H25" s="2"/>
       <c r="I25" s="2">
@@ -3470,7 +3470,7 @@
         <v>1</v>
       </c>
       <c r="AN25" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO25" s="2">
         <v>0</v>
@@ -3484,7 +3484,7 @@
         <v>42</v>
       </c>
       <c r="C26" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D26" t="s">
         <v>73</v>
@@ -3493,10 +3493,10 @@
         <v>44721</v>
       </c>
       <c r="F26" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G26" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26" s="2"/>
       <c r="I26" s="2">
@@ -3536,7 +3536,7 @@
         <v>0</v>
       </c>
       <c r="U26" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V26" s="2">
         <v>0</v>
@@ -3581,7 +3581,7 @@
         <v>0</v>
       </c>
       <c r="AJ26" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK26" s="2">
         <v>0</v>
@@ -3596,7 +3596,7 @@
         <v>0</v>
       </c>
       <c r="AO26" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
@@ -3604,10 +3604,10 @@
         <v>6</v>
       </c>
       <c r="B27" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D27" t="s">
         <v>73</v>
@@ -3616,10 +3616,10 @@
         <v>44721</v>
       </c>
       <c r="F27" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G27" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H27" s="2"/>
       <c r="I27" s="2">
@@ -3650,7 +3650,7 @@
         <v>0</v>
       </c>
       <c r="R27" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S27" s="2">
         <v>0</v>
@@ -3659,7 +3659,7 @@
         <v>0</v>
       </c>
       <c r="U27" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V27" s="2">
         <v>0</v>
@@ -3704,7 +3704,7 @@
         <v>0</v>
       </c>
       <c r="AJ27" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK27" s="2">
         <v>0</v>
@@ -3727,7 +3727,7 @@
         <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C28" t="s">
         <v>71</v>
@@ -3773,7 +3773,7 @@
         <v>0</v>
       </c>
       <c r="R28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S28" s="2">
         <v>0</v>
@@ -3842,7 +3842,7 @@
         <v>0</v>
       </c>
       <c r="AO28" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -3850,10 +3850,10 @@
         <v>7</v>
       </c>
       <c r="B29" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="C29" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D29" t="s">
         <v>73</v>
@@ -3862,10 +3862,10 @@
         <v>44707</v>
       </c>
       <c r="F29" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G29" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H29" s="2"/>
       <c r="I29" s="2">
@@ -3935,7 +3935,7 @@
         <v>0</v>
       </c>
       <c r="AE29" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF29" s="2">
         <v>0</v>
@@ -3959,7 +3959,7 @@
         <v>0</v>
       </c>
       <c r="AM29" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN29" s="2">
         <v>0</v>
@@ -3973,22 +3973,22 @@
         <v>7</v>
       </c>
       <c r="B30" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="C30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D30" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E30" s="1">
         <v>44707</v>
       </c>
       <c r="F30" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G30" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H30" s="2"/>
       <c r="I30" s="2">
@@ -4007,10 +4007,10 @@
         <v>0</v>
       </c>
       <c r="N30" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O30" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P30" s="2">
         <v>0</v>
@@ -4082,7 +4082,7 @@
         <v>0</v>
       </c>
       <c r="AM30" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN30" s="2">
         <v>0</v>
@@ -4096,13 +4096,13 @@
         <v>7</v>
       </c>
       <c r="B31" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="C31" t="s">
         <v>70</v>
       </c>
       <c r="D31" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E31" s="1">
         <v>44707</v>
@@ -4124,10 +4124,10 @@
         <v>0</v>
       </c>
       <c r="L31" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M31" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N31" s="2">
         <v>0</v>
@@ -4181,7 +4181,7 @@
         <v>0</v>
       </c>
       <c r="AE31" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF31" s="2">
         <v>0</v>
@@ -4196,7 +4196,7 @@
         <v>0</v>
       </c>
       <c r="AJ31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK31" s="2">
         <v>0</v>
@@ -4219,7 +4219,7 @@
         <v>7</v>
       </c>
       <c r="B32" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="C32" t="s">
         <v>70</v>
@@ -4253,10 +4253,10 @@
         <v>0</v>
       </c>
       <c r="N32" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O32" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P32" s="2">
         <v>0</v>
@@ -4304,7 +4304,7 @@
         <v>0</v>
       </c>
       <c r="AE32" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF32" s="2">
         <v>0</v>
@@ -4328,7 +4328,7 @@
         <v>0</v>
       </c>
       <c r="AM32" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN32" s="2">
         <v>0</v>
@@ -4342,13 +4342,13 @@
         <v>7</v>
       </c>
       <c r="B33" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="C33" t="s">
         <v>71</v>
       </c>
       <c r="D33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E33" s="1">
         <v>44707</v>
@@ -4427,7 +4427,7 @@
         <v>0</v>
       </c>
       <c r="AE33" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF33" s="2">
         <v>0</v>
@@ -4451,7 +4451,7 @@
         <v>0</v>
       </c>
       <c r="AM33" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN33" s="2">
         <v>0</v>
@@ -4465,13 +4465,13 @@
         <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C34" t="s">
         <v>70</v>
       </c>
       <c r="D34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E34" s="1">
         <v>44707</v>
@@ -4550,7 +4550,7 @@
         <v>0</v>
       </c>
       <c r="AE34" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF34" s="2">
         <v>0</v>
@@ -4565,10 +4565,10 @@
         <v>0</v>
       </c>
       <c r="AJ34" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK34" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL34" s="2">
         <v>0</v>
@@ -4588,10 +4588,10 @@
         <v>7</v>
       </c>
       <c r="B35" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C35" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D35" t="s">
         <v>73</v>
@@ -4600,10 +4600,10 @@
         <v>44707</v>
       </c>
       <c r="F35" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G35" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H35" s="2"/>
       <c r="I35" s="2">
@@ -4616,10 +4616,10 @@
         <v>0</v>
       </c>
       <c r="L35" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M35" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N35" s="2">
         <v>0</v>
@@ -4673,7 +4673,7 @@
         <v>0</v>
       </c>
       <c r="AE35" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF35" s="2">
         <v>0</v>
@@ -4697,7 +4697,7 @@
         <v>0</v>
       </c>
       <c r="AM35" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN35" s="2">
         <v>0</v>
@@ -4711,22 +4711,22 @@
         <v>7</v>
       </c>
       <c r="B36" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="C36" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D36" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E36" s="1">
         <v>44707</v>
       </c>
       <c r="F36" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G36" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H36" s="2"/>
       <c r="I36" s="2">
@@ -4796,7 +4796,7 @@
         <v>0</v>
       </c>
       <c r="AE36" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF36" s="2">
         <v>0</v>
@@ -4814,13 +4814,13 @@
         <v>0</v>
       </c>
       <c r="AK36" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL36" s="2">
         <v>0</v>
       </c>
       <c r="AM36" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN36" s="2">
         <v>0</v>
@@ -4840,7 +4840,7 @@
         <v>71</v>
       </c>
       <c r="D37" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E37" s="1">
         <v>44707</v>
@@ -4919,7 +4919,7 @@
         <v>0</v>
       </c>
       <c r="AE37" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF37" s="2">
         <v>0</v>
@@ -4960,7 +4960,7 @@
         <v>26</v>
       </c>
       <c r="C38" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D38" t="s">
         <v>73</v>
@@ -4969,10 +4969,10 @@
         <v>44789</v>
       </c>
       <c r="F38" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G38" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H38" s="2"/>
       <c r="I38" s="2">
@@ -4985,10 +4985,10 @@
         <v>0</v>
       </c>
       <c r="L38" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M38" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N38" s="2">
         <v>0</v>
@@ -5042,7 +5042,7 @@
         <v>0</v>
       </c>
       <c r="AE38" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF38" s="2">
         <v>0</v>
@@ -5066,7 +5066,7 @@
         <v>0</v>
       </c>
       <c r="AM38" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN38" s="2">
         <v>0</v>
@@ -5080,7 +5080,7 @@
         <v>8</v>
       </c>
       <c r="B39" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="C39" t="s">
         <v>70</v>
@@ -5108,10 +5108,10 @@
         <v>0</v>
       </c>
       <c r="L39" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M39" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N39" s="2">
         <v>0</v>
@@ -5135,7 +5135,7 @@
         <v>0</v>
       </c>
       <c r="U39" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V39" s="2">
         <v>0</v>
@@ -5165,7 +5165,7 @@
         <v>0</v>
       </c>
       <c r="AE39" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF39" s="2">
         <v>0</v>
@@ -5180,7 +5180,7 @@
         <v>0</v>
       </c>
       <c r="AJ39" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK39" s="2">
         <v>0</v>
@@ -5203,10 +5203,10 @@
         <v>8</v>
       </c>
       <c r="B40" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C40" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D40" t="s">
         <v>73</v>
@@ -5215,10 +5215,10 @@
         <v>44789</v>
       </c>
       <c r="F40" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G40" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H40" s="2"/>
       <c r="I40" s="2">
@@ -5255,10 +5255,10 @@
         <v>0</v>
       </c>
       <c r="T40" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U40" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V40" s="2">
         <v>0</v>
@@ -5303,7 +5303,7 @@
         <v>0</v>
       </c>
       <c r="AJ40" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK40" s="2">
         <v>0</v>
@@ -5326,7 +5326,7 @@
         <v>8</v>
       </c>
       <c r="B41" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="C41" t="s">
         <v>71</v>
@@ -5378,7 +5378,7 @@
         <v>0</v>
       </c>
       <c r="T41" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U41" s="2">
         <v>0</v>
@@ -5435,7 +5435,7 @@
         <v>0</v>
       </c>
       <c r="AM41" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN41" s="2">
         <v>0</v>
@@ -5449,7 +5449,7 @@
         <v>9</v>
       </c>
       <c r="B42" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="C42" t="s">
         <v>71</v>
@@ -5516,7 +5516,7 @@
         <v>0</v>
       </c>
       <c r="Y42" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z42" s="2">
         <v>0</v>
@@ -5572,7 +5572,7 @@
         <v>9</v>
       </c>
       <c r="B43" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="C43" t="s">
         <v>71</v>
@@ -5681,7 +5681,7 @@
         <v>0</v>
       </c>
       <c r="AM43" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN43" s="2">
         <v>0</v>
@@ -5695,7 +5695,7 @@
         <v>9</v>
       </c>
       <c r="B44" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C44" t="s">
         <v>71</v>
@@ -5780,7 +5780,7 @@
         <v>0</v>
       </c>
       <c r="AE44" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF44" s="2">
         <v>0</v>
@@ -5804,7 +5804,7 @@
         <v>0</v>
       </c>
       <c r="AM44" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN44" s="2">
         <v>0</v>
@@ -5818,7 +5818,7 @@
         <v>9</v>
       </c>
       <c r="B45" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C45" t="s">
         <v>71</v>
@@ -5885,7 +5885,7 @@
         <v>0</v>
       </c>
       <c r="Y45" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z45" s="2">
         <v>0</v>
@@ -5903,7 +5903,7 @@
         <v>0</v>
       </c>
       <c r="AE45" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF45" s="2">
         <v>0</v>
@@ -5927,7 +5927,7 @@
         <v>0</v>
       </c>
       <c r="AM45" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN45" s="2">
         <v>0</v>
@@ -5941,10 +5941,10 @@
         <v>9</v>
       </c>
       <c r="B46" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="C46" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D46" t="s">
         <v>73</v>
@@ -5953,10 +5953,10 @@
         <v>44818</v>
       </c>
       <c r="F46" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G46" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H46" s="2"/>
       <c r="I46" s="2">
@@ -5969,10 +5969,10 @@
         <v>0</v>
       </c>
       <c r="L46" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M46" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N46" s="2">
         <v>0</v>
@@ -6026,7 +6026,7 @@
         <v>0</v>
       </c>
       <c r="AE46" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF46" s="2">
         <v>0</v>
@@ -6064,10 +6064,10 @@
         <v>9</v>
       </c>
       <c r="B47" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="C47" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D47" t="s">
         <v>73</v>
@@ -6076,10 +6076,10 @@
         <v>44818</v>
       </c>
       <c r="F47" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G47" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H47" s="2"/>
       <c r="I47" s="2">
@@ -6092,10 +6092,10 @@
         <v>0</v>
       </c>
       <c r="L47" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M47" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N47" s="2">
         <v>0</v>
@@ -6149,7 +6149,7 @@
         <v>0</v>
       </c>
       <c r="AE47" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF47" s="2">
         <v>0</v>
@@ -6173,7 +6173,7 @@
         <v>0</v>
       </c>
       <c r="AM47" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN47" s="2">
         <v>0</v>
@@ -6187,7 +6187,7 @@
         <v>9</v>
       </c>
       <c r="B48" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C48" t="s">
         <v>71</v>
@@ -6313,7 +6313,7 @@
         <v>27</v>
       </c>
       <c r="C49" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D49" t="s">
         <v>73</v>
@@ -6322,10 +6322,10 @@
         <v>44818</v>
       </c>
       <c r="F49" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G49" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H49" s="2"/>
       <c r="I49" s="2">
@@ -6344,10 +6344,10 @@
         <v>0</v>
       </c>
       <c r="N49" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O49" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P49" s="2">
         <v>0</v>
@@ -6395,7 +6395,7 @@
         <v>0</v>
       </c>
       <c r="AE49" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF49" s="2">
         <v>0</v>
@@ -6419,7 +6419,7 @@
         <v>0</v>
       </c>
       <c r="AM49" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN49" s="2">
         <v>0</v>
@@ -6433,7 +6433,7 @@
         <v>9</v>
       </c>
       <c r="B50" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C50" t="s">
         <v>70</v>
@@ -6467,10 +6467,10 @@
         <v>0</v>
       </c>
       <c r="N50" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O50" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P50" s="2">
         <v>0</v>
@@ -6556,10 +6556,10 @@
         <v>9</v>
       </c>
       <c r="B51" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C51" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D51" t="s">
         <v>73</v>
@@ -6568,10 +6568,10 @@
         <v>44818</v>
       </c>
       <c r="F51" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G51" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H51" s="2"/>
       <c r="I51" s="2">
@@ -6665,7 +6665,7 @@
         <v>0</v>
       </c>
       <c r="AM51" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN51" s="2">
         <v>0</v>
@@ -6679,7 +6679,7 @@
         <v>9</v>
       </c>
       <c r="B52" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="C52" t="s">
         <v>71</v>
@@ -6788,7 +6788,7 @@
         <v>0</v>
       </c>
       <c r="AM52" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN52" s="2">
         <v>0</v>
@@ -6802,7 +6802,7 @@
         <v>9</v>
       </c>
       <c r="B53" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C53" t="s">
         <v>71</v>
@@ -6925,7 +6925,7 @@
         <v>9</v>
       </c>
       <c r="B54" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C54" t="s">
         <v>71</v>
@@ -7028,7 +7028,7 @@
         <v>0</v>
       </c>
       <c r="AK54" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL54" s="2">
         <v>0</v>
@@ -7048,7 +7048,7 @@
         <v>9</v>
       </c>
       <c r="B55" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C55" t="s">
         <v>71</v>
@@ -7151,7 +7151,7 @@
         <v>0</v>
       </c>
       <c r="AK55" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL55" s="2">
         <v>0</v>
@@ -7171,7 +7171,7 @@
         <v>9</v>
       </c>
       <c r="B56" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C56" t="s">
         <v>71</v>
@@ -7256,7 +7256,7 @@
         <v>0</v>
       </c>
       <c r="AE56" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF56" s="2">
         <v>0</v>
@@ -7280,7 +7280,7 @@
         <v>0</v>
       </c>
       <c r="AM56" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN56" s="2">
         <v>0</v>
@@ -7294,7 +7294,7 @@
         <v>10</v>
       </c>
       <c r="B57" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="C57" t="s">
         <v>71</v>
@@ -7379,7 +7379,7 @@
         <v>0</v>
       </c>
       <c r="AE57" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF57" s="2">
         <v>0</v>
@@ -7397,13 +7397,13 @@
         <v>0</v>
       </c>
       <c r="AK57" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL57" s="2">
         <v>0</v>
       </c>
       <c r="AM57" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN57" s="2">
         <v>0</v>
@@ -7420,7 +7420,7 @@
         <v>53</v>
       </c>
       <c r="C58" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D58" t="s">
         <v>73</v>
@@ -7429,10 +7429,10 @@
         <v>44771</v>
       </c>
       <c r="F58" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G58" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H58" s="2"/>
       <c r="I58" s="2">
@@ -7499,10 +7499,10 @@
         <v>0</v>
       </c>
       <c r="AD58" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE58" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF58" s="2">
         <v>0</v>
@@ -7517,7 +7517,7 @@
         <v>0</v>
       </c>
       <c r="AJ58" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK58" s="2">
         <v>0</v>
@@ -7540,13 +7540,13 @@
         <v>10</v>
       </c>
       <c r="B59" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="C59" t="s">
         <v>70</v>
       </c>
       <c r="D59" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E59" s="1">
         <v>44771</v>
@@ -7640,7 +7640,7 @@
         <v>0</v>
       </c>
       <c r="AJ59" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK59" s="2">
         <v>0</v>
@@ -7649,7 +7649,7 @@
         <v>0</v>
       </c>
       <c r="AM59" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN59" s="2">
         <v>0</v>
@@ -7663,22 +7663,22 @@
         <v>10</v>
       </c>
       <c r="B60" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C60" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D60" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E60" s="1">
         <v>44771</v>
       </c>
       <c r="F60" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G60" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H60" s="2"/>
       <c r="I60" s="2">
@@ -7748,7 +7748,7 @@
         <v>0</v>
       </c>
       <c r="AE60" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF60" s="2">
         <v>0</v>
@@ -7763,10 +7763,10 @@
         <v>0</v>
       </c>
       <c r="AJ60" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK60" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL60" s="2">
         <v>0</v>
@@ -7786,10 +7786,10 @@
         <v>10</v>
       </c>
       <c r="B61" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C61" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D61" t="s">
         <v>73</v>
@@ -7798,10 +7798,10 @@
         <v>44771</v>
       </c>
       <c r="F61" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G61" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H61" s="2"/>
       <c r="I61" s="2">
@@ -7844,7 +7844,7 @@
         <v>0</v>
       </c>
       <c r="V61" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W61" s="2">
         <v>0</v>
@@ -7886,7 +7886,7 @@
         <v>0</v>
       </c>
       <c r="AJ61" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK61" s="2">
         <v>0</v>
@@ -7909,7 +7909,7 @@
         <v>10</v>
       </c>
       <c r="B62" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="C62" t="s">
         <v>70</v>
@@ -7937,10 +7937,10 @@
         <v>0</v>
       </c>
       <c r="L62" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M62" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N62" s="2">
         <v>0</v>
@@ -8032,7 +8032,7 @@
         <v>10</v>
       </c>
       <c r="B63" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C63" t="s">
         <v>70</v>
@@ -8090,7 +8090,7 @@
         <v>0</v>
       </c>
       <c r="V63" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W63" s="2">
         <v>0</v>
@@ -8114,10 +8114,10 @@
         <v>0</v>
       </c>
       <c r="AD63" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE63" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF63" s="2">
         <v>0</v>
@@ -8155,10 +8155,10 @@
         <v>10</v>
       </c>
       <c r="B64" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="C64" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D64" t="s">
         <v>73</v>
@@ -8167,10 +8167,10 @@
         <v>44771</v>
       </c>
       <c r="F64" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G64" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H64" s="2"/>
       <c r="I64" s="2">
@@ -8183,10 +8183,10 @@
         <v>0</v>
       </c>
       <c r="L64" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M64" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N64" s="2">
         <v>0</v>
@@ -8201,7 +8201,7 @@
         <v>0</v>
       </c>
       <c r="R64" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S64" s="2">
         <v>0</v>
@@ -8240,7 +8240,7 @@
         <v>0</v>
       </c>
       <c r="AE64" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF64" s="2">
         <v>0</v>
@@ -8278,7 +8278,7 @@
         <v>10</v>
       </c>
       <c r="B65" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C65" t="s">
         <v>70</v>
@@ -8401,22 +8401,22 @@
         <v>10</v>
       </c>
       <c r="B66" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="C66" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D66" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E66" s="1">
         <v>44771</v>
       </c>
       <c r="F66" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G66" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H66" s="2"/>
       <c r="I66" s="2">
@@ -8501,7 +8501,7 @@
         <v>0</v>
       </c>
       <c r="AJ66" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK66" s="2">
         <v>0</v>
@@ -8510,7 +8510,7 @@
         <v>0</v>
       </c>
       <c r="AM66" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN66" s="2">
         <v>0</v>
@@ -8524,10 +8524,10 @@
         <v>10</v>
       </c>
       <c r="B67" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="C67" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D67" t="s">
         <v>73</v>
@@ -8536,10 +8536,10 @@
         <v>44771</v>
       </c>
       <c r="F67" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G67" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H67" s="2"/>
       <c r="I67" s="2">
@@ -8570,7 +8570,7 @@
         <v>0</v>
       </c>
       <c r="R67" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S67" s="2">
         <v>0</v>
@@ -8606,10 +8606,10 @@
         <v>0</v>
       </c>
       <c r="AD67" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE67" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF67" s="2">
         <v>0</v>
@@ -8770,7 +8770,7 @@
         <v>10</v>
       </c>
       <c r="B69" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="C69" t="s">
         <v>70</v>
@@ -8855,7 +8855,7 @@
         <v>0</v>
       </c>
       <c r="AE69" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF69" s="2">
         <v>0</v>
@@ -8879,7 +8879,7 @@
         <v>0</v>
       </c>
       <c r="AM69" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN69" s="2">
         <v>0</v>
@@ -8893,7 +8893,7 @@
         <v>10</v>
       </c>
       <c r="B70" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="C70" t="s">
         <v>70</v>
@@ -9022,7 +9022,7 @@
         <v>70</v>
       </c>
       <c r="D71" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E71" s="1">
         <v>44771</v>
@@ -9098,10 +9098,10 @@
         <v>0</v>
       </c>
       <c r="AD71" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE71" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF71" s="2">
         <v>0</v>
@@ -9116,7 +9116,7 @@
         <v>0</v>
       </c>
       <c r="AJ71" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK71" s="2">
         <v>0</v>
@@ -9139,7 +9139,7 @@
         <v>11</v>
       </c>
       <c r="B72" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="C72" t="s">
         <v>70</v>
@@ -9167,10 +9167,10 @@
         <v>0</v>
       </c>
       <c r="L72" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M72" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N72" s="2">
         <v>0</v>
@@ -9224,7 +9224,7 @@
         <v>0</v>
       </c>
       <c r="AE72" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF72" s="2">
         <v>0</v>
@@ -9262,7 +9262,7 @@
         <v>11</v>
       </c>
       <c r="B73" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C73" t="s">
         <v>71</v>
@@ -9385,7 +9385,7 @@
         <v>11</v>
       </c>
       <c r="B74" t="s">
-        <v>60</v>
+        <v>24</v>
       </c>
       <c r="C74" t="s">
         <v>70</v>
@@ -9413,10 +9413,10 @@
         <v>0</v>
       </c>
       <c r="L74" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M74" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N74" s="2">
         <v>0</v>
@@ -9470,7 +9470,7 @@
         <v>0</v>
       </c>
       <c r="AE74" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF74" s="2">
         <v>0</v>
@@ -9508,7 +9508,7 @@
         <v>12</v>
       </c>
       <c r="B75" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C75" t="s">
         <v>70</v>
@@ -9631,7 +9631,7 @@
         <v>13</v>
       </c>
       <c r="B76" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="C76" t="s">
         <v>70</v>
@@ -9716,7 +9716,7 @@
         <v>0</v>
       </c>
       <c r="AE76" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF76" s="2">
         <v>0</v>
@@ -9740,7 +9740,7 @@
         <v>0</v>
       </c>
       <c r="AM76" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN76" s="2">
         <v>0</v>
@@ -9754,7 +9754,7 @@
         <v>13</v>
       </c>
       <c r="B77" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="C77" t="s">
         <v>70</v>
@@ -9803,10 +9803,10 @@
         <v>0</v>
       </c>
       <c r="S77" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T77" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U77" s="2">
         <v>0</v>
@@ -9854,7 +9854,7 @@
         <v>0</v>
       </c>
       <c r="AJ77" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK77" s="2">
         <v>0</v>
@@ -9877,7 +9877,7 @@
         <v>13</v>
       </c>
       <c r="B78" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="C78" t="s">
         <v>70</v>
@@ -9962,7 +9962,7 @@
         <v>0</v>
       </c>
       <c r="AE78" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF78" s="2">
         <v>0</v>
@@ -9977,7 +9977,7 @@
         <v>0</v>
       </c>
       <c r="AJ78" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK78" s="2">
         <v>0</v>
@@ -10000,7 +10000,7 @@
         <v>13</v>
       </c>
       <c r="B79" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C79" t="s">
         <v>70</v>
@@ -10028,16 +10028,16 @@
         <v>0</v>
       </c>
       <c r="L79" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M79" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N79" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O79" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P79" s="2">
         <v>0</v>
@@ -10085,7 +10085,7 @@
         <v>0</v>
       </c>
       <c r="AE79" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF79" s="2">
         <v>0</v>
@@ -10109,7 +10109,7 @@
         <v>0</v>
       </c>
       <c r="AM79" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN79" s="2">
         <v>0</v>
@@ -10123,7 +10123,7 @@
         <v>13</v>
       </c>
       <c r="B80" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C80" t="s">
         <v>70</v>
@@ -10151,16 +10151,16 @@
         <v>0</v>
       </c>
       <c r="L80" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M80" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N80" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O80" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P80" s="2">
         <v>0</v>
@@ -10208,7 +10208,7 @@
         <v>0</v>
       </c>
       <c r="AE80" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF80" s="2">
         <v>0</v>
@@ -10232,7 +10232,7 @@
         <v>0</v>
       </c>
       <c r="AM80" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN80" s="2">
         <v>0</v>
@@ -10246,7 +10246,7 @@
         <v>13</v>
       </c>
       <c r="B81" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C81" t="s">
         <v>70</v>
@@ -10295,10 +10295,10 @@
         <v>0</v>
       </c>
       <c r="S81" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T81" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U81" s="2">
         <v>0</v>
@@ -10355,7 +10355,7 @@
         <v>0</v>
       </c>
       <c r="AM81" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN81" s="2">
         <v>0</v>
@@ -10369,7 +10369,7 @@
         <v>14</v>
       </c>
       <c r="B82" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="C82" t="s">
         <v>71</v>
@@ -10492,10 +10492,10 @@
         <v>14</v>
       </c>
       <c r="B83" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C83" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D83" t="s">
         <v>73</v>
@@ -10504,10 +10504,10 @@
         <v>44894</v>
       </c>
       <c r="F83" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G83" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H83" s="2"/>
       <c r="I83" s="2">
@@ -10615,10 +10615,10 @@
         <v>14</v>
       </c>
       <c r="B84" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
       <c r="C84" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D84" t="s">
         <v>73</v>
@@ -10627,10 +10627,10 @@
         <v>44894</v>
       </c>
       <c r="F84" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G84" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H84" s="2"/>
       <c r="I84" s="2">
@@ -10652,10 +10652,10 @@
         <v>0</v>
       </c>
       <c r="O84" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P84" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q84" s="2">
         <v>0</v>
@@ -10724,7 +10724,7 @@
         <v>0</v>
       </c>
       <c r="AM84" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN84" s="2">
         <v>0</v>
@@ -10738,7 +10738,7 @@
         <v>14</v>
       </c>
       <c r="B85" t="s">
-        <v>64</v>
+        <v>25</v>
       </c>
       <c r="C85" t="s">
         <v>70</v>
@@ -10823,7 +10823,7 @@
         <v>0</v>
       </c>
       <c r="AE85" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF85" s="2">
         <v>0</v>
@@ -10847,10 +10847,10 @@
         <v>0</v>
       </c>
       <c r="AM85" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN85" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO85" s="2">
         <v>0</v>
@@ -10861,10 +10861,10 @@
         <v>14</v>
       </c>
       <c r="B86" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="C86" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D86" t="s">
         <v>73</v>
@@ -10873,10 +10873,10 @@
         <v>44894</v>
       </c>
       <c r="F86" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G86" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H86" s="2"/>
       <c r="I86" s="2">
@@ -10946,7 +10946,7 @@
         <v>0</v>
       </c>
       <c r="AE86" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF86" s="2">
         <v>0</v>
@@ -10984,10 +10984,10 @@
         <v>14</v>
       </c>
       <c r="B87" t="s">
-        <v>23</v>
+        <v>64</v>
       </c>
       <c r="C87" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D87" t="s">
         <v>73</v>
@@ -10996,10 +10996,10 @@
         <v>44894</v>
       </c>
       <c r="F87" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G87" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H87" s="2"/>
       <c r="I87" s="2">
@@ -11069,7 +11069,7 @@
         <v>0</v>
       </c>
       <c r="AE87" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF87" s="2">
         <v>0</v>
@@ -11096,7 +11096,7 @@
         <v>0</v>
       </c>
       <c r="AN87" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO87" s="2">
         <v>0</v>
@@ -11107,7 +11107,7 @@
         <v>14</v>
       </c>
       <c r="B88" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="C88" t="s">
         <v>71</v>
@@ -11144,10 +11144,10 @@
         <v>0</v>
       </c>
       <c r="O88" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P88" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q88" s="2">
         <v>0</v>
@@ -11216,7 +11216,7 @@
         <v>0</v>
       </c>
       <c r="AM88" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN88" s="2">
         <v>0</v>
@@ -11230,10 +11230,10 @@
         <v>14</v>
       </c>
       <c r="B89" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="C89" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D89" t="s">
         <v>73</v>
@@ -11242,10 +11242,10 @@
         <v>44894</v>
       </c>
       <c r="F89" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G89" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H89" s="2"/>
       <c r="I89" s="2">
@@ -11315,7 +11315,7 @@
         <v>0</v>
       </c>
       <c r="AE89" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF89" s="2">
         <v>0</v>
@@ -11339,10 +11339,10 @@
         <v>0</v>
       </c>
       <c r="AM89" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN89" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO89" s="2">
         <v>0</v>
@@ -11353,10 +11353,10 @@
         <v>14</v>
       </c>
       <c r="B90" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="C90" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D90" t="s">
         <v>73</v>
@@ -11365,10 +11365,10 @@
         <v>44894</v>
       </c>
       <c r="F90" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G90" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H90" s="2"/>
       <c r="I90" s="2">
@@ -11465,7 +11465,7 @@
         <v>1</v>
       </c>
       <c r="AN90" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO90" s="2">
         <v>0</v>
@@ -11476,7 +11476,7 @@
         <v>15</v>
       </c>
       <c r="B91" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C91" t="s">
         <v>70</v>
@@ -11531,7 +11531,7 @@
         <v>0</v>
       </c>
       <c r="U91" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V91" s="2">
         <v>0</v>
@@ -11599,10 +11599,10 @@
         <v>15</v>
       </c>
       <c r="B92" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="C92" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D92" t="s">
         <v>73</v>
@@ -11611,10 +11611,10 @@
         <v>44865</v>
       </c>
       <c r="F92" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G92" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H92" s="2"/>
       <c r="I92" s="2">
@@ -11684,7 +11684,7 @@
         <v>0</v>
       </c>
       <c r="AE92" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF92" s="2">
         <v>0</v>
@@ -11722,10 +11722,10 @@
         <v>15</v>
       </c>
       <c r="B93" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="C93" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D93" t="s">
         <v>73</v>
@@ -11734,10 +11734,10 @@
         <v>44865</v>
       </c>
       <c r="F93" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G93" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H93" s="2"/>
       <c r="I93" s="2">
@@ -11777,7 +11777,7 @@
         <v>0</v>
       </c>
       <c r="U93" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V93" s="2">
         <v>0</v>
@@ -11845,7 +11845,7 @@
         <v>15</v>
       </c>
       <c r="B94" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="C94" t="s">
         <v>71</v>
@@ -11954,7 +11954,7 @@
         <v>0</v>
       </c>
       <c r="AM94" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN94" s="2">
         <v>0</v>
@@ -11968,7 +11968,7 @@
         <v>15</v>
       </c>
       <c r="B95" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="C95" t="s">
         <v>70</v>
@@ -12068,7 +12068,7 @@
         <v>0</v>
       </c>
       <c r="AJ95" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK95" s="2">
         <v>0</v>
@@ -12077,7 +12077,7 @@
         <v>0</v>
       </c>
       <c r="AM95" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN95" s="2">
         <v>0</v>
@@ -12091,7 +12091,7 @@
         <v>15</v>
       </c>
       <c r="B96" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="C96" t="s">
         <v>71</v>
@@ -12200,7 +12200,7 @@
         <v>0</v>
       </c>
       <c r="AM96" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN96" s="2">
         <v>0</v>
@@ -12214,7 +12214,7 @@
         <v>15</v>
       </c>
       <c r="B97" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C97" t="s">
         <v>70</v>
@@ -12242,10 +12242,10 @@
         <v>0</v>
       </c>
       <c r="L97" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M97" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N97" s="2">
         <v>0</v>
@@ -12299,7 +12299,7 @@
         <v>0</v>
       </c>
       <c r="AE97" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF97" s="2">
         <v>0</v>
@@ -12323,7 +12323,7 @@
         <v>0</v>
       </c>
       <c r="AM97" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN97" s="2">
         <v>0</v>
@@ -12337,10 +12337,10 @@
         <v>15</v>
       </c>
       <c r="B98" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="C98" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D98" t="s">
         <v>73</v>
@@ -12349,10 +12349,10 @@
         <v>44865</v>
       </c>
       <c r="F98" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G98" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H98" s="2"/>
       <c r="I98" s="2">
@@ -12365,10 +12365,10 @@
         <v>0</v>
       </c>
       <c r="L98" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M98" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N98" s="2">
         <v>0</v>
@@ -12422,7 +12422,7 @@
         <v>0</v>
       </c>
       <c r="AE98" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF98" s="2">
         <v>0</v>
@@ -12437,7 +12437,7 @@
         <v>0</v>
       </c>
       <c r="AJ98" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK98" s="2">
         <v>0</v>
@@ -12460,10 +12460,10 @@
         <v>15</v>
       </c>
       <c r="B99" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="C99" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D99" t="s">
         <v>73</v>
@@ -12472,10 +12472,10 @@
         <v>44865</v>
       </c>
       <c r="F99" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G99" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H99" s="2"/>
       <c r="I99" s="2">
@@ -12545,7 +12545,7 @@
         <v>0</v>
       </c>
       <c r="AE99" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF99" s="2">
         <v>0</v>
@@ -12706,10 +12706,10 @@
         <v>16</v>
       </c>
       <c r="B101" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="C101" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D101" t="s">
         <v>73</v>
@@ -12718,10 +12718,10 @@
         <v>44879</v>
       </c>
       <c r="F101" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G101" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H101" s="2"/>
       <c r="I101" s="2">
@@ -12773,7 +12773,7 @@
         <v>0</v>
       </c>
       <c r="Y101" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z101" s="2">
         <v>0</v>
@@ -12791,7 +12791,7 @@
         <v>0</v>
       </c>
       <c r="AE101" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF101" s="2">
         <v>0</v>
@@ -12815,7 +12815,7 @@
         <v>0</v>
       </c>
       <c r="AM101" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN101" s="2">
         <v>0</v>
@@ -12857,10 +12857,10 @@
         <v>0</v>
       </c>
       <c r="L102" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M102" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N102" s="2">
         <v>0</v>
@@ -12914,7 +12914,7 @@
         <v>0</v>
       </c>
       <c r="AE102" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF102" s="2">
         <v>0</v>
@@ -12938,7 +12938,7 @@
         <v>0</v>
       </c>
       <c r="AM102" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN102" s="2">
         <v>0</v>
@@ -12952,10 +12952,10 @@
         <v>16</v>
       </c>
       <c r="B103" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C103" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D103" t="s">
         <v>73</v>
@@ -12964,10 +12964,10 @@
         <v>44879</v>
       </c>
       <c r="F103" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G103" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H103" s="2"/>
       <c r="I103" s="2">
@@ -13061,7 +13061,7 @@
         <v>0</v>
       </c>
       <c r="AM103" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN103" s="2">
         <v>0</v>
@@ -13075,7 +13075,7 @@
         <v>16</v>
       </c>
       <c r="B104" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C104" t="s">
         <v>71</v>
@@ -13121,7 +13121,7 @@
         <v>0</v>
       </c>
       <c r="R104" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S104" s="2">
         <v>0</v>
@@ -13142,7 +13142,7 @@
         <v>0</v>
       </c>
       <c r="Y104" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z104" s="2">
         <v>0</v>
@@ -13160,7 +13160,7 @@
         <v>0</v>
       </c>
       <c r="AE104" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF104" s="2">
         <v>0</v>
@@ -13198,7 +13198,7 @@
         <v>16</v>
       </c>
       <c r="B105" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="C105" t="s">
         <v>70</v>
@@ -13226,10 +13226,10 @@
         <v>0</v>
       </c>
       <c r="L105" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M105" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N105" s="2">
         <v>0</v>
@@ -13283,7 +13283,7 @@
         <v>0</v>
       </c>
       <c r="AE105" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF105" s="2">
         <v>0</v>
@@ -13321,7 +13321,7 @@
         <v>16</v>
       </c>
       <c r="B106" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="C106" t="s">
         <v>71</v>
@@ -13367,7 +13367,7 @@
         <v>0</v>
       </c>
       <c r="R106" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S106" s="2">
         <v>0</v>
@@ -13430,7 +13430,7 @@
         <v>0</v>
       </c>
       <c r="AM106" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN106" s="2">
         <v>0</v>
@@ -13444,10 +13444,10 @@
         <v>17</v>
       </c>
       <c r="B107" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="C107" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D107" t="s">
         <v>73</v>
@@ -13456,10 +13456,10 @@
         <v>44893</v>
       </c>
       <c r="F107" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G107" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H107" s="2"/>
       <c r="I107" s="2">
@@ -13475,7 +13475,7 @@
         <v>0</v>
       </c>
       <c r="M107" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N107" s="2">
         <v>0</v>
@@ -13487,10 +13487,10 @@
         <v>0</v>
       </c>
       <c r="Q107" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R107" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S107" s="2">
         <v>0</v>
@@ -13529,7 +13529,7 @@
         <v>0</v>
       </c>
       <c r="AE107" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF107" s="2">
         <v>0</v>
@@ -13567,10 +13567,10 @@
         <v>17</v>
       </c>
       <c r="B108" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="C108" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D108" t="s">
         <v>73</v>
@@ -13579,10 +13579,10 @@
         <v>44893</v>
       </c>
       <c r="F108" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G108" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H108" s="2"/>
       <c r="I108" s="2">
@@ -13598,7 +13598,7 @@
         <v>0</v>
       </c>
       <c r="M108" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N108" s="2">
         <v>0</v>
@@ -13610,10 +13610,10 @@
         <v>0</v>
       </c>
       <c r="Q108" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R108" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S108" s="2">
         <v>0</v>
@@ -13652,7 +13652,7 @@
         <v>0</v>
       </c>
       <c r="AE108" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF108" s="2">
         <v>0</v>
@@ -13690,7 +13690,7 @@
         <v>18</v>
       </c>
       <c r="B109" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C109" t="s">
         <v>70</v>
@@ -13751,7 +13751,7 @@
         <v>0</v>
       </c>
       <c r="W109" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X109" s="2">
         <v>0</v>
@@ -13790,7 +13790,7 @@
         <v>0</v>
       </c>
       <c r="AJ109" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK109" s="2">
         <v>0</v>
@@ -13813,10 +13813,10 @@
         <v>18</v>
       </c>
       <c r="B110" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C110" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D110" t="s">
         <v>73</v>
@@ -13825,10 +13825,10 @@
         <v>44887</v>
       </c>
       <c r="F110" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G110" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H110" s="2"/>
       <c r="I110" s="2">
@@ -13874,7 +13874,7 @@
         <v>0</v>
       </c>
       <c r="W110" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X110" s="2">
         <v>0</v>
@@ -13910,7 +13910,7 @@
         <v>0</v>
       </c>
       <c r="AI110" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ110" s="2">
         <v>1</v>
@@ -13936,10 +13936,10 @@
         <v>18</v>
       </c>
       <c r="B111" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C111" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D111" t="s">
         <v>73</v>
@@ -13948,10 +13948,10 @@
         <v>44887</v>
       </c>
       <c r="F111" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G111" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H111" s="2"/>
       <c r="I111" s="2">
@@ -13985,10 +13985,10 @@
         <v>0</v>
       </c>
       <c r="S111" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T111" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U111" s="2">
         <v>0</v>
@@ -14033,10 +14033,10 @@
         <v>0</v>
       </c>
       <c r="AI111" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ111" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK111" s="2">
         <v>0</v>
@@ -14059,10 +14059,10 @@
         <v>18</v>
       </c>
       <c r="B112" t="s">
-        <v>34</v>
+        <v>67</v>
       </c>
       <c r="C112" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D112" t="s">
         <v>73</v>
@@ -14071,10 +14071,10 @@
         <v>44887</v>
       </c>
       <c r="F112" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G112" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H112" s="2"/>
       <c r="I112" s="2">
@@ -14108,10 +14108,10 @@
         <v>0</v>
       </c>
       <c r="S112" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T112" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U112" s="2">
         <v>0</v>
@@ -14182,10 +14182,10 @@
         <v>18</v>
       </c>
       <c r="B113" t="s">
-        <v>67</v>
+        <v>31</v>
       </c>
       <c r="C113" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D113" t="s">
         <v>73</v>
@@ -14194,10 +14194,10 @@
         <v>44887</v>
       </c>
       <c r="F113" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G113" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H113" s="2"/>
       <c r="I113" s="2">
@@ -14305,7 +14305,7 @@
         <v>19</v>
       </c>
       <c r="B114" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C114" t="s">
         <v>70</v>

</xml_diff>

<commit_message>
codebook fixes, pending update
</commit_message>
<xml_diff>
--- a/datasets/lab_detail.xlsx
+++ b/datasets/lab_detail.xlsx
@@ -81,64 +81,64 @@
     <t>substance</t>
   </si>
   <si>
+    <t>p-fluorofentanyl</t>
+  </si>
+  <si>
     <t>4-ANPP</t>
   </si>
   <si>
     <t>fentanyl</t>
   </si>
   <si>
-    <t>p-fluorofentanyl</t>
+    <t>dimethyl sulfone (methylsulfonylmethane MSM)</t>
   </si>
   <si>
-    <t>dimethyl sulfone (methylsulfonylmethane MSM)</t>
+    <t>xylazine</t>
+  </si>
+  <si>
+    <t>despropionyl p-fluorofentanyl</t>
   </si>
   <si>
     <t>phenethyl 4-ANPP</t>
   </si>
   <si>
-    <t>despropionyl p-fluorofentanyl</t>
-  </si>
-  <si>
-    <t>xylazine</t>
+    <t>3,4-MDMA</t>
   </si>
   <si>
     <t>3,4-methylenedioxy-N-benzylcathinone (BMDP)</t>
   </si>
   <si>
-    <t>3,4-MDMA</t>
+    <t>norcocaine</t>
+  </si>
+  <si>
+    <t>tropacocaine</t>
+  </si>
+  <si>
+    <t>phenacetin</t>
+  </si>
+  <si>
+    <t>benzoylecgonine (BZ)</t>
+  </si>
+  <si>
+    <t>levamisole</t>
   </si>
   <si>
     <t>methyl ecgonidine (MED)</t>
   </si>
   <si>
-    <t>tropacocaine</t>
-  </si>
-  <si>
-    <t>benzoylecgonine (BZ)</t>
-  </si>
-  <si>
     <t>cocaine</t>
-  </si>
-  <si>
-    <t>levamisole</t>
-  </si>
-  <si>
-    <t>norcocaine</t>
-  </si>
-  <si>
-    <t>phenacetin</t>
-  </si>
-  <si>
-    <t>tramadol</t>
   </si>
   <si>
     <t>p-fluoro phenethyl 4-ANPP</t>
   </si>
   <si>
+    <t>non-specific sugars</t>
+  </si>
+  <si>
     <t>methamphetamine</t>
   </si>
   <si>
-    <t>non-specific sugars</t>
+    <t>tramadol</t>
   </si>
   <si>
     <t>eutylone</t>
@@ -147,52 +147,52 @@
     <t>caffeine</t>
   </si>
   <si>
+    <t>heroin</t>
+  </si>
+  <si>
     <t>urea</t>
   </si>
   <si>
     <t>6-monoacetylmorphine (6-MAM)</t>
   </si>
   <si>
-    <t>heroin</t>
+    <t>acetylcodeine</t>
   </si>
   <si>
-    <t>acetylcodeine</t>
+    <t>ethyl-4-ANPP</t>
+  </si>
+  <si>
+    <t>1,3-Diacetin</t>
+  </si>
+  <si>
+    <t>acetaminophen</t>
   </si>
   <si>
     <t>lidocaine</t>
   </si>
   <si>
-    <t>acetaminophen</t>
-  </si>
-  <si>
-    <t>ethyl-4-ANPP</t>
-  </si>
-  <si>
     <t>N-phenylpropanamide</t>
   </si>
   <si>
-    <t>1,3-Diacetin</t>
+    <t>diphenhydramine</t>
+  </si>
+  <si>
+    <t>gabapentin</t>
+  </si>
+  <si>
+    <t>quinine</t>
+  </si>
+  <si>
+    <t>metonitazene</t>
+  </si>
+  <si>
+    <t>inositol</t>
   </si>
   <si>
     <t>N-piperidinyl etonitazene</t>
   </si>
   <si>
-    <t>inositol</t>
-  </si>
-  <si>
-    <t>metonitazene</t>
-  </si>
-  <si>
-    <t>gabapentin</t>
-  </si>
-  <si>
-    <t>diphenhydramine</t>
-  </si>
-  <si>
     <t>methadone</t>
-  </si>
-  <si>
-    <t>quinine</t>
   </si>
   <si>
     <t>non-specific organic acids</t>
@@ -201,16 +201,16 @@
     <t>procaine</t>
   </si>
   <si>
-    <t>nicotine</t>
-  </si>
-  <si>
-    <t>menthol</t>
+    <t>phenethylbromide</t>
   </si>
   <si>
     <t>phenethyl chloride</t>
   </si>
   <si>
-    <t>phenethylbromide</t>
+    <t>nicotine</t>
+  </si>
+  <si>
+    <t>menthol</t>
   </si>
   <si>
     <t>1-phenethyl-4-propionyloxypiperidine</t>
@@ -614,7 +614,7 @@
         <v>0</v>
       </c>
       <c r="AE2" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF2" s="2">
         <v>0</v>
@@ -638,7 +638,7 @@
         <v>0</v>
       </c>
       <c r="AM2" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN2" s="2">
         <v>0</v>
@@ -680,10 +680,10 @@
         <v>0</v>
       </c>
       <c r="L3" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M3" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N3" s="2">
         <v>0</v>
@@ -737,7 +737,7 @@
         <v>0</v>
       </c>
       <c r="AE3" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF3" s="2">
         <v>0</v>
@@ -761,7 +761,7 @@
         <v>0</v>
       </c>
       <c r="AM3" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN3" s="2">
         <v>0</v>
@@ -803,10 +803,10 @@
         <v>0</v>
       </c>
       <c r="L4" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M4" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N4" s="2">
         <v>0</v>
@@ -1055,10 +1055,10 @@
         <v>0</v>
       </c>
       <c r="N6" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O6" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P6" s="2">
         <v>0</v>
@@ -1130,7 +1130,7 @@
         <v>0</v>
       </c>
       <c r="AM6" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN6" s="2">
         <v>0</v>
@@ -1301,10 +1301,10 @@
         <v>0</v>
       </c>
       <c r="N8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P8" s="2">
         <v>0</v>
@@ -1376,7 +1376,7 @@
         <v>0</v>
       </c>
       <c r="AM8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN8" s="2">
         <v>0</v>
@@ -1393,7 +1393,7 @@
         <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D9" t="s">
         <v>73</v>
@@ -1402,10 +1402,10 @@
         <v>44777</v>
       </c>
       <c r="F9" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2">
@@ -1454,7 +1454,7 @@
         <v>0</v>
       </c>
       <c r="X9" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y9" s="2">
         <v>0</v>
@@ -1516,7 +1516,7 @@
         <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D10" t="s">
         <v>73</v>
@@ -1525,10 +1525,10 @@
         <v>44777</v>
       </c>
       <c r="F10" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2">
@@ -1577,7 +1577,7 @@
         <v>0</v>
       </c>
       <c r="X10" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y10" s="2">
         <v>0</v>
@@ -1636,7 +1636,7 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
         <v>70</v>
@@ -1856,7 +1856,7 @@
         <v>0</v>
       </c>
       <c r="AI12" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ12" s="2">
         <v>0</v>
@@ -2105,7 +2105,7 @@
         <v>0</v>
       </c>
       <c r="AJ14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK14" s="2">
         <v>0</v>
@@ -2131,19 +2131,19 @@
         <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D15" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E15" s="1">
         <v>44714</v>
       </c>
       <c r="F15" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2">
@@ -2177,10 +2177,10 @@
         <v>0</v>
       </c>
       <c r="S15" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T15" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U15" s="2">
         <v>0</v>
@@ -2471,7 +2471,7 @@
         <v>0</v>
       </c>
       <c r="AI17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ17" s="2">
         <v>0</v>
@@ -2500,19 +2500,19 @@
         <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E18" s="1">
         <v>44714</v>
       </c>
       <c r="F18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H18" s="2"/>
       <c r="I18" s="2">
@@ -2546,10 +2546,10 @@
         <v>0</v>
       </c>
       <c r="S18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U18" s="2">
         <v>0</v>
@@ -2597,7 +2597,7 @@
         <v>0</v>
       </c>
       <c r="AJ18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK18" s="2">
         <v>0</v>
@@ -2687,7 +2687,7 @@
         <v>0</v>
       </c>
       <c r="Y19" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z19" s="2">
         <v>0</v>
@@ -2705,7 +2705,7 @@
         <v>0</v>
       </c>
       <c r="AE19" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF19" s="2">
         <v>0</v>
@@ -2729,10 +2729,10 @@
         <v>0</v>
       </c>
       <c r="AM19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO19" s="2">
         <v>0</v>
@@ -2746,19 +2746,19 @@
         <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D20" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E20" s="1">
         <v>44759</v>
       </c>
       <c r="F20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2">
@@ -2843,7 +2843,7 @@
         <v>0</v>
       </c>
       <c r="AJ20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK20" s="2">
         <v>0</v>
@@ -2852,10 +2852,10 @@
         <v>0</v>
       </c>
       <c r="AM20" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN20" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO20" s="2">
         <v>0</v>
@@ -2866,22 +2866,22 @@
         <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="C21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E21" s="1">
         <v>44759</v>
       </c>
       <c r="F21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2">
@@ -2912,7 +2912,7 @@
         <v>0</v>
       </c>
       <c r="R21" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S21" s="2">
         <v>0</v>
@@ -2951,7 +2951,7 @@
         <v>0</v>
       </c>
       <c r="AE21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF21" s="2">
         <v>0</v>
@@ -2978,7 +2978,7 @@
         <v>0</v>
       </c>
       <c r="AN21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO21" s="2">
         <v>0</v>
@@ -2989,22 +2989,22 @@
         <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="C22" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E22" s="1">
         <v>44759</v>
       </c>
       <c r="F22" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="2">
@@ -3017,10 +3017,10 @@
         <v>0</v>
       </c>
       <c r="L22" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M22" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N22" s="2">
         <v>0</v>
@@ -3035,7 +3035,7 @@
         <v>0</v>
       </c>
       <c r="R22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S22" s="2">
         <v>0</v>
@@ -3074,7 +3074,7 @@
         <v>0</v>
       </c>
       <c r="AE22" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF22" s="2">
         <v>0</v>
@@ -3112,13 +3112,13 @@
         <v>5</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="C23" t="s">
         <v>70</v>
       </c>
       <c r="D23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E23" s="1">
         <v>44759</v>
@@ -3212,7 +3212,7 @@
         <v>0</v>
       </c>
       <c r="AJ23" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK23" s="2">
         <v>0</v>
@@ -3221,7 +3221,7 @@
         <v>0</v>
       </c>
       <c r="AM23" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN23" s="2">
         <v>0</v>
@@ -3235,7 +3235,7 @@
         <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C24" t="s">
         <v>70</v>
@@ -3263,10 +3263,10 @@
         <v>0</v>
       </c>
       <c r="L24" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M24" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N24" s="2">
         <v>0</v>
@@ -3347,7 +3347,7 @@
         <v>0</v>
       </c>
       <c r="AN24" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO24" s="2">
         <v>0</v>
@@ -3358,10 +3358,10 @@
         <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="C25" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D25" t="s">
         <v>73</v>
@@ -3370,10 +3370,10 @@
         <v>44759</v>
       </c>
       <c r="F25" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G25" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25" s="2"/>
       <c r="I25" s="2">
@@ -3425,7 +3425,7 @@
         <v>0</v>
       </c>
       <c r="Y25" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z25" s="2">
         <v>0</v>
@@ -3443,7 +3443,7 @@
         <v>0</v>
       </c>
       <c r="AE25" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF25" s="2">
         <v>0</v>
@@ -3467,7 +3467,7 @@
         <v>0</v>
       </c>
       <c r="AM25" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN25" s="2">
         <v>0</v>
@@ -3481,7 +3481,7 @@
         <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C26" t="s">
         <v>71</v>
@@ -3527,7 +3527,7 @@
         <v>0</v>
       </c>
       <c r="R26" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S26" s="2">
         <v>0</v>
@@ -3596,7 +3596,7 @@
         <v>0</v>
       </c>
       <c r="AO26" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -3604,10 +3604,10 @@
         <v>6</v>
       </c>
       <c r="B27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C27" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D27" t="s">
         <v>73</v>
@@ -3616,10 +3616,10 @@
         <v>44721</v>
       </c>
       <c r="F27" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G27" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H27" s="2"/>
       <c r="I27" s="2">
@@ -3659,7 +3659,7 @@
         <v>0</v>
       </c>
       <c r="U27" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V27" s="2">
         <v>0</v>
@@ -3704,7 +3704,7 @@
         <v>0</v>
       </c>
       <c r="AJ27" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK27" s="2">
         <v>0</v>
@@ -3719,7 +3719,7 @@
         <v>0</v>
       </c>
       <c r="AO27" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28">
@@ -3727,10 +3727,10 @@
         <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D28" t="s">
         <v>73</v>
@@ -3739,10 +3739,10 @@
         <v>44721</v>
       </c>
       <c r="F28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G28" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H28" s="2"/>
       <c r="I28" s="2">
@@ -3773,7 +3773,7 @@
         <v>0</v>
       </c>
       <c r="R28" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S28" s="2">
         <v>0</v>
@@ -3782,7 +3782,7 @@
         <v>0</v>
       </c>
       <c r="U28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V28" s="2">
         <v>0</v>
@@ -3827,7 +3827,7 @@
         <v>0</v>
       </c>
       <c r="AJ28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK28" s="2">
         <v>0</v>
@@ -3850,22 +3850,22 @@
         <v>7</v>
       </c>
       <c r="B29" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="C29" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E29" s="1">
         <v>44707</v>
       </c>
       <c r="F29" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G29" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H29" s="2"/>
       <c r="I29" s="2">
@@ -3950,7 +3950,7 @@
         <v>0</v>
       </c>
       <c r="AJ29" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK29" s="2">
         <v>0</v>
@@ -3959,7 +3959,7 @@
         <v>0</v>
       </c>
       <c r="AM29" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN29" s="2">
         <v>0</v>
@@ -3973,10 +3973,10 @@
         <v>7</v>
       </c>
       <c r="B30" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D30" t="s">
         <v>74</v>
@@ -3985,10 +3985,10 @@
         <v>44707</v>
       </c>
       <c r="F30" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G30" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H30" s="2"/>
       <c r="I30" s="2">
@@ -4073,7 +4073,7 @@
         <v>0</v>
       </c>
       <c r="AJ30" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK30" s="2">
         <v>0</v>
@@ -4096,7 +4096,7 @@
         <v>7</v>
       </c>
       <c r="B31" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="C31" t="s">
         <v>70</v>
@@ -4130,10 +4130,10 @@
         <v>0</v>
       </c>
       <c r="N31" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O31" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P31" s="2">
         <v>0</v>
@@ -4181,7 +4181,7 @@
         <v>0</v>
       </c>
       <c r="AE31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF31" s="2">
         <v>0</v>
@@ -4219,7 +4219,7 @@
         <v>7</v>
       </c>
       <c r="B32" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C32" t="s">
         <v>70</v>
@@ -4247,16 +4247,16 @@
         <v>0</v>
       </c>
       <c r="L32" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M32" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N32" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O32" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P32" s="2">
         <v>0</v>
@@ -4304,7 +4304,7 @@
         <v>0</v>
       </c>
       <c r="AE32" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF32" s="2">
         <v>0</v>
@@ -4348,7 +4348,7 @@
         <v>71</v>
       </c>
       <c r="D33" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E33" s="1">
         <v>44707</v>
@@ -4427,7 +4427,7 @@
         <v>0</v>
       </c>
       <c r="AE33" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF33" s="2">
         <v>0</v>
@@ -4465,7 +4465,7 @@
         <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="C34" t="s">
         <v>71</v>
@@ -4550,7 +4550,7 @@
         <v>0</v>
       </c>
       <c r="AE34" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF34" s="2">
         <v>0</v>
@@ -4574,7 +4574,7 @@
         <v>0</v>
       </c>
       <c r="AM34" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN34" s="2">
         <v>0</v>
@@ -4588,7 +4588,7 @@
         <v>7</v>
       </c>
       <c r="B35" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="C35" t="s">
         <v>70</v>
@@ -4616,10 +4616,10 @@
         <v>0</v>
       </c>
       <c r="L35" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M35" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N35" s="2">
         <v>0</v>
@@ -4711,22 +4711,22 @@
         <v>7</v>
       </c>
       <c r="B36" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="C36" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D36" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E36" s="1">
         <v>44707</v>
       </c>
       <c r="F36" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G36" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H36" s="2"/>
       <c r="I36" s="2">
@@ -4796,7 +4796,7 @@
         <v>0</v>
       </c>
       <c r="AE36" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF36" s="2">
         <v>0</v>
@@ -4814,13 +4814,13 @@
         <v>0</v>
       </c>
       <c r="AK36" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL36" s="2">
         <v>0</v>
       </c>
       <c r="AM36" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN36" s="2">
         <v>0</v>
@@ -4834,22 +4834,22 @@
         <v>7</v>
       </c>
       <c r="B37" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="C37" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D37" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E37" s="1">
         <v>44707</v>
       </c>
       <c r="F37" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G37" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H37" s="2"/>
       <c r="I37" s="2">
@@ -4919,7 +4919,7 @@
         <v>0</v>
       </c>
       <c r="AE37" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF37" s="2">
         <v>0</v>
@@ -4937,13 +4937,13 @@
         <v>0</v>
       </c>
       <c r="AK37" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL37" s="2">
         <v>0</v>
       </c>
       <c r="AM37" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN37" s="2">
         <v>0</v>
@@ -4960,7 +4960,7 @@
         <v>23</v>
       </c>
       <c r="C38" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D38" t="s">
         <v>73</v>
@@ -4969,10 +4969,10 @@
         <v>44789</v>
       </c>
       <c r="F38" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G38" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H38" s="2"/>
       <c r="I38" s="2">
@@ -4985,10 +4985,10 @@
         <v>0</v>
       </c>
       <c r="L38" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M38" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N38" s="2">
         <v>0</v>
@@ -5042,7 +5042,7 @@
         <v>0</v>
       </c>
       <c r="AE38" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF38" s="2">
         <v>0</v>
@@ -5066,7 +5066,7 @@
         <v>0</v>
       </c>
       <c r="AM38" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN38" s="2">
         <v>0</v>
@@ -5080,10 +5080,10 @@
         <v>8</v>
       </c>
       <c r="B39" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="C39" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D39" t="s">
         <v>73</v>
@@ -5092,10 +5092,10 @@
         <v>44789</v>
       </c>
       <c r="F39" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G39" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H39" s="2"/>
       <c r="I39" s="2">
@@ -5135,7 +5135,7 @@
         <v>0</v>
       </c>
       <c r="U39" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V39" s="2">
         <v>0</v>
@@ -5180,7 +5180,7 @@
         <v>0</v>
       </c>
       <c r="AJ39" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK39" s="2">
         <v>0</v>
@@ -5189,7 +5189,7 @@
         <v>0</v>
       </c>
       <c r="AM39" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN39" s="2">
         <v>0</v>
@@ -5203,10 +5203,10 @@
         <v>8</v>
       </c>
       <c r="B40" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C40" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D40" t="s">
         <v>73</v>
@@ -5215,10 +5215,10 @@
         <v>44789</v>
       </c>
       <c r="F40" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G40" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H40" s="2"/>
       <c r="I40" s="2">
@@ -5231,10 +5231,10 @@
         <v>0</v>
       </c>
       <c r="L40" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M40" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N40" s="2">
         <v>0</v>
@@ -5255,7 +5255,7 @@
         <v>0</v>
       </c>
       <c r="T40" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U40" s="2">
         <v>0</v>
@@ -5288,7 +5288,7 @@
         <v>0</v>
       </c>
       <c r="AE40" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF40" s="2">
         <v>0</v>
@@ -5326,10 +5326,10 @@
         <v>8</v>
       </c>
       <c r="B41" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C41" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D41" t="s">
         <v>73</v>
@@ -5338,10 +5338,10 @@
         <v>44789</v>
       </c>
       <c r="F41" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G41" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H41" s="2"/>
       <c r="I41" s="2">
@@ -5378,10 +5378,10 @@
         <v>0</v>
       </c>
       <c r="T41" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U41" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V41" s="2">
         <v>0</v>
@@ -5426,7 +5426,7 @@
         <v>0</v>
       </c>
       <c r="AJ41" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK41" s="2">
         <v>0</v>
@@ -5449,10 +5449,10 @@
         <v>9</v>
       </c>
       <c r="B42" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="C42" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D42" t="s">
         <v>73</v>
@@ -5461,10 +5461,10 @@
         <v>44818</v>
       </c>
       <c r="F42" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G42" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H42" s="2"/>
       <c r="I42" s="2">
@@ -5483,10 +5483,10 @@
         <v>0</v>
       </c>
       <c r="N42" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O42" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P42" s="2">
         <v>0</v>
@@ -5558,7 +5558,7 @@
         <v>0</v>
       </c>
       <c r="AM42" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN42" s="2">
         <v>0</v>
@@ -5572,10 +5572,10 @@
         <v>9</v>
       </c>
       <c r="B43" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C43" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D43" t="s">
         <v>73</v>
@@ -5584,10 +5584,10 @@
         <v>44818</v>
       </c>
       <c r="F43" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G43" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H43" s="2"/>
       <c r="I43" s="2">
@@ -5600,10 +5600,10 @@
         <v>0</v>
       </c>
       <c r="L43" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M43" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N43" s="2">
         <v>0</v>
@@ -5657,7 +5657,7 @@
         <v>0</v>
       </c>
       <c r="AE43" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF43" s="2">
         <v>0</v>
@@ -5681,7 +5681,7 @@
         <v>0</v>
       </c>
       <c r="AM43" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN43" s="2">
         <v>0</v>
@@ -5695,7 +5695,7 @@
         <v>9</v>
       </c>
       <c r="B44" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="C44" t="s">
         <v>71</v>
@@ -5780,7 +5780,7 @@
         <v>0</v>
       </c>
       <c r="AE44" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF44" s="2">
         <v>0</v>
@@ -5818,7 +5818,7 @@
         <v>9</v>
       </c>
       <c r="B45" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C45" t="s">
         <v>71</v>
@@ -5885,7 +5885,7 @@
         <v>0</v>
       </c>
       <c r="Y45" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z45" s="2">
         <v>0</v>
@@ -5903,7 +5903,7 @@
         <v>0</v>
       </c>
       <c r="AE45" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF45" s="2">
         <v>0</v>
@@ -5918,7 +5918,7 @@
         <v>0</v>
       </c>
       <c r="AJ45" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK45" s="2">
         <v>0</v>
@@ -5941,7 +5941,7 @@
         <v>9</v>
       </c>
       <c r="B46" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="C46" t="s">
         <v>71</v>
@@ -6064,7 +6064,7 @@
         <v>9</v>
       </c>
       <c r="B47" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C47" t="s">
         <v>71</v>
@@ -6149,7 +6149,7 @@
         <v>0</v>
       </c>
       <c r="AE47" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF47" s="2">
         <v>0</v>
@@ -6187,10 +6187,10 @@
         <v>9</v>
       </c>
       <c r="B48" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="C48" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D48" t="s">
         <v>73</v>
@@ -6199,10 +6199,10 @@
         <v>44818</v>
       </c>
       <c r="F48" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G48" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H48" s="2"/>
       <c r="I48" s="2">
@@ -6310,7 +6310,7 @@
         <v>9</v>
       </c>
       <c r="B49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C49" t="s">
         <v>71</v>
@@ -6413,7 +6413,7 @@
         <v>0</v>
       </c>
       <c r="AK49" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL49" s="2">
         <v>0</v>
@@ -6533,7 +6533,7 @@
         <v>0</v>
       </c>
       <c r="AJ50" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK50" s="2">
         <v>0</v>
@@ -6542,7 +6542,7 @@
         <v>0</v>
       </c>
       <c r="AM50" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN50" s="2">
         <v>0</v>
@@ -6556,7 +6556,7 @@
         <v>9</v>
       </c>
       <c r="B51" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C51" t="s">
         <v>71</v>
@@ -6641,7 +6641,7 @@
         <v>0</v>
       </c>
       <c r="AE51" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF51" s="2">
         <v>0</v>
@@ -6665,7 +6665,7 @@
         <v>0</v>
       </c>
       <c r="AM51" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN51" s="2">
         <v>0</v>
@@ -6679,7 +6679,7 @@
         <v>9</v>
       </c>
       <c r="B52" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C52" t="s">
         <v>71</v>
@@ -6764,7 +6764,7 @@
         <v>0</v>
       </c>
       <c r="AE52" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF52" s="2">
         <v>0</v>
@@ -6782,7 +6782,7 @@
         <v>0</v>
       </c>
       <c r="AK52" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL52" s="2">
         <v>0</v>
@@ -6802,10 +6802,10 @@
         <v>9</v>
       </c>
       <c r="B53" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="C53" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D53" t="s">
         <v>73</v>
@@ -6814,10 +6814,10 @@
         <v>44818</v>
       </c>
       <c r="F53" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G53" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H53" s="2"/>
       <c r="I53" s="2">
@@ -6836,10 +6836,10 @@
         <v>0</v>
       </c>
       <c r="N53" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O53" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P53" s="2">
         <v>0</v>
@@ -6869,7 +6869,7 @@
         <v>0</v>
       </c>
       <c r="Y53" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z53" s="2">
         <v>0</v>
@@ -6887,7 +6887,7 @@
         <v>0</v>
       </c>
       <c r="AE53" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF53" s="2">
         <v>0</v>
@@ -6925,7 +6925,7 @@
         <v>9</v>
       </c>
       <c r="B54" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C54" t="s">
         <v>70</v>
@@ -6953,10 +6953,10 @@
         <v>0</v>
       </c>
       <c r="L54" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M54" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N54" s="2">
         <v>0</v>
@@ -7010,7 +7010,7 @@
         <v>0</v>
       </c>
       <c r="AE54" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF54" s="2">
         <v>0</v>
@@ -7034,7 +7034,7 @@
         <v>0</v>
       </c>
       <c r="AM54" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN54" s="2">
         <v>0</v>
@@ -7048,7 +7048,7 @@
         <v>9</v>
       </c>
       <c r="B55" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="C55" t="s">
         <v>71</v>
@@ -7133,7 +7133,7 @@
         <v>0</v>
       </c>
       <c r="AE55" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF55" s="2">
         <v>0</v>
@@ -7171,7 +7171,7 @@
         <v>9</v>
       </c>
       <c r="B56" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C56" t="s">
         <v>71</v>
@@ -7256,7 +7256,7 @@
         <v>0</v>
       </c>
       <c r="AE56" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF56" s="2">
         <v>0</v>
@@ -7280,7 +7280,7 @@
         <v>0</v>
       </c>
       <c r="AM56" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN56" s="2">
         <v>0</v>
@@ -7294,7 +7294,7 @@
         <v>10</v>
       </c>
       <c r="B57" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C57" t="s">
         <v>70</v>
@@ -7379,7 +7379,7 @@
         <v>0</v>
       </c>
       <c r="AE57" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF57" s="2">
         <v>0</v>
@@ -7445,10 +7445,10 @@
         <v>0</v>
       </c>
       <c r="L58" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M58" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N58" s="2">
         <v>0</v>
@@ -7502,7 +7502,7 @@
         <v>0</v>
       </c>
       <c r="AE58" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF58" s="2">
         <v>0</v>
@@ -7526,7 +7526,7 @@
         <v>0</v>
       </c>
       <c r="AM58" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN58" s="2">
         <v>0</v>
@@ -7540,22 +7540,22 @@
         <v>10</v>
       </c>
       <c r="B59" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C59" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D59" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E59" s="1">
         <v>44771</v>
       </c>
       <c r="F59" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G59" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H59" s="2"/>
       <c r="I59" s="2">
@@ -7625,7 +7625,7 @@
         <v>0</v>
       </c>
       <c r="AE59" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF59" s="2">
         <v>0</v>
@@ -7640,10 +7640,10 @@
         <v>0</v>
       </c>
       <c r="AJ59" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK59" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL59" s="2">
         <v>0</v>
@@ -7663,7 +7663,7 @@
         <v>10</v>
       </c>
       <c r="B60" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="C60" t="s">
         <v>71</v>
@@ -7709,7 +7709,7 @@
         <v>0</v>
       </c>
       <c r="R60" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S60" s="2">
         <v>0</v>
@@ -7772,7 +7772,7 @@
         <v>0</v>
       </c>
       <c r="AM60" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN60" s="2">
         <v>0</v>
@@ -7786,7 +7786,7 @@
         <v>10</v>
       </c>
       <c r="B61" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="C61" t="s">
         <v>71</v>
@@ -7886,7 +7886,7 @@
         <v>0</v>
       </c>
       <c r="AJ61" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK61" s="2">
         <v>0</v>
@@ -7895,7 +7895,7 @@
         <v>0</v>
       </c>
       <c r="AM61" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN61" s="2">
         <v>0</v>
@@ -7909,7 +7909,7 @@
         <v>10</v>
       </c>
       <c r="B62" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C62" t="s">
         <v>70</v>
@@ -7967,7 +7967,7 @@
         <v>0</v>
       </c>
       <c r="V62" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W62" s="2">
         <v>0</v>
@@ -7991,10 +7991,10 @@
         <v>0</v>
       </c>
       <c r="AD62" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE62" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF62" s="2">
         <v>0</v>
@@ -8032,7 +8032,7 @@
         <v>10</v>
       </c>
       <c r="B63" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C63" t="s">
         <v>70</v>
@@ -8155,7 +8155,7 @@
         <v>10</v>
       </c>
       <c r="B64" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C64" t="s">
         <v>70</v>
@@ -8278,10 +8278,10 @@
         <v>10</v>
       </c>
       <c r="B65" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="C65" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D65" t="s">
         <v>73</v>
@@ -8290,10 +8290,10 @@
         <v>44771</v>
       </c>
       <c r="F65" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G65" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H65" s="2"/>
       <c r="I65" s="2">
@@ -8336,7 +8336,7 @@
         <v>0</v>
       </c>
       <c r="V65" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W65" s="2">
         <v>0</v>
@@ -8363,7 +8363,7 @@
         <v>0</v>
       </c>
       <c r="AE65" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF65" s="2">
         <v>0</v>
@@ -8381,7 +8381,7 @@
         <v>0</v>
       </c>
       <c r="AK65" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL65" s="2">
         <v>0</v>
@@ -8401,7 +8401,7 @@
         <v>10</v>
       </c>
       <c r="B66" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="C66" t="s">
         <v>70</v>
@@ -8486,7 +8486,7 @@
         <v>0</v>
       </c>
       <c r="AE66" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF66" s="2">
         <v>0</v>
@@ -8510,7 +8510,7 @@
         <v>0</v>
       </c>
       <c r="AM66" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN66" s="2">
         <v>0</v>
@@ -8524,7 +8524,7 @@
         <v>10</v>
       </c>
       <c r="B67" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="C67" t="s">
         <v>71</v>
@@ -8570,7 +8570,7 @@
         <v>0</v>
       </c>
       <c r="R67" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S67" s="2">
         <v>0</v>
@@ -8624,7 +8624,7 @@
         <v>0</v>
       </c>
       <c r="AJ67" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK67" s="2">
         <v>0</v>
@@ -8647,13 +8647,13 @@
         <v>10</v>
       </c>
       <c r="B68" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C68" t="s">
         <v>70</v>
       </c>
       <c r="D68" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E68" s="1">
         <v>44771</v>
@@ -8732,7 +8732,7 @@
         <v>0</v>
       </c>
       <c r="AE68" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF68" s="2">
         <v>0</v>
@@ -8747,7 +8747,7 @@
         <v>0</v>
       </c>
       <c r="AJ68" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK68" s="2">
         <v>0</v>
@@ -8770,13 +8770,13 @@
         <v>10</v>
       </c>
       <c r="B69" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="C69" t="s">
         <v>70</v>
       </c>
       <c r="D69" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E69" s="1">
         <v>44771</v>
@@ -8852,10 +8852,10 @@
         <v>0</v>
       </c>
       <c r="AD69" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE69" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF69" s="2">
         <v>0</v>
@@ -8870,7 +8870,7 @@
         <v>0</v>
       </c>
       <c r="AJ69" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK69" s="2">
         <v>0</v>
@@ -8893,13 +8893,13 @@
         <v>10</v>
       </c>
       <c r="B70" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
       <c r="C70" t="s">
         <v>70</v>
       </c>
       <c r="D70" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E70" s="1">
         <v>44771</v>
@@ -8921,10 +8921,10 @@
         <v>0</v>
       </c>
       <c r="L70" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M70" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N70" s="2">
         <v>0</v>
@@ -8978,7 +8978,7 @@
         <v>0</v>
       </c>
       <c r="AE70" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF70" s="2">
         <v>0</v>
@@ -8993,7 +8993,7 @@
         <v>0</v>
       </c>
       <c r="AJ70" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK70" s="2">
         <v>0</v>
@@ -9016,7 +9016,7 @@
         <v>10</v>
       </c>
       <c r="B71" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="C71" t="s">
         <v>70</v>
@@ -9101,7 +9101,7 @@
         <v>0</v>
       </c>
       <c r="AE71" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF71" s="2">
         <v>0</v>
@@ -9262,7 +9262,7 @@
         <v>11</v>
       </c>
       <c r="B73" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="C73" t="s">
         <v>70</v>
@@ -9290,10 +9290,10 @@
         <v>0</v>
       </c>
       <c r="L73" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M73" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N73" s="2">
         <v>0</v>
@@ -9347,7 +9347,7 @@
         <v>0</v>
       </c>
       <c r="AE73" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF73" s="2">
         <v>0</v>
@@ -9385,7 +9385,7 @@
         <v>11</v>
       </c>
       <c r="B74" t="s">
-        <v>60</v>
+        <v>24</v>
       </c>
       <c r="C74" t="s">
         <v>70</v>
@@ -9413,10 +9413,10 @@
         <v>0</v>
       </c>
       <c r="L74" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M74" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N74" s="2">
         <v>0</v>
@@ -9470,7 +9470,7 @@
         <v>0</v>
       </c>
       <c r="AE74" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF74" s="2">
         <v>0</v>
@@ -9631,7 +9631,7 @@
         <v>13</v>
       </c>
       <c r="B76" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C76" t="s">
         <v>70</v>
@@ -9754,7 +9754,7 @@
         <v>13</v>
       </c>
       <c r="B77" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C77" t="s">
         <v>70</v>
@@ -9803,10 +9803,10 @@
         <v>0</v>
       </c>
       <c r="S77" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T77" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U77" s="2">
         <v>0</v>
@@ -9839,7 +9839,7 @@
         <v>0</v>
       </c>
       <c r="AE77" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF77" s="2">
         <v>0</v>
@@ -10000,7 +10000,7 @@
         <v>13</v>
       </c>
       <c r="B79" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C79" t="s">
         <v>70</v>
@@ -10123,7 +10123,7 @@
         <v>13</v>
       </c>
       <c r="B80" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C80" t="s">
         <v>70</v>
@@ -10246,7 +10246,7 @@
         <v>13</v>
       </c>
       <c r="B81" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="C81" t="s">
         <v>70</v>
@@ -10295,10 +10295,10 @@
         <v>0</v>
       </c>
       <c r="S81" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T81" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U81" s="2">
         <v>0</v>
@@ -10331,7 +10331,7 @@
         <v>0</v>
       </c>
       <c r="AE81" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF81" s="2">
         <v>0</v>
@@ -10369,7 +10369,7 @@
         <v>14</v>
       </c>
       <c r="B82" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="C82" t="s">
         <v>71</v>
@@ -10406,10 +10406,10 @@
         <v>0</v>
       </c>
       <c r="O82" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P82" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q82" s="2">
         <v>0</v>
@@ -10492,10 +10492,10 @@
         <v>14</v>
       </c>
       <c r="B83" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="C83" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D83" t="s">
         <v>73</v>
@@ -10504,10 +10504,10 @@
         <v>44894</v>
       </c>
       <c r="F83" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G83" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H83" s="2"/>
       <c r="I83" s="2">
@@ -10577,7 +10577,7 @@
         <v>0</v>
       </c>
       <c r="AE83" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF83" s="2">
         <v>0</v>
@@ -10604,7 +10604,7 @@
         <v>0</v>
       </c>
       <c r="AN83" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO83" s="2">
         <v>0</v>
@@ -10738,10 +10738,10 @@
         <v>14</v>
       </c>
       <c r="B85" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="C85" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D85" t="s">
         <v>73</v>
@@ -10750,10 +10750,10 @@
         <v>44894</v>
       </c>
       <c r="F85" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G85" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H85" s="2"/>
       <c r="I85" s="2">
@@ -10823,7 +10823,7 @@
         <v>0</v>
       </c>
       <c r="AE85" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF85" s="2">
         <v>0</v>
@@ -10847,10 +10847,10 @@
         <v>0</v>
       </c>
       <c r="AM85" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN85" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO85" s="2">
         <v>0</v>
@@ -10861,7 +10861,7 @@
         <v>14</v>
       </c>
       <c r="B86" t="s">
-        <v>63</v>
+        <v>22</v>
       </c>
       <c r="C86" t="s">
         <v>70</v>
@@ -10946,7 +10946,7 @@
         <v>0</v>
       </c>
       <c r="AE86" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF86" s="2">
         <v>0</v>
@@ -10984,7 +10984,7 @@
         <v>14</v>
       </c>
       <c r="B87" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C87" t="s">
         <v>70</v>
@@ -11107,7 +11107,7 @@
         <v>14</v>
       </c>
       <c r="B88" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="C88" t="s">
         <v>71</v>
@@ -11144,10 +11144,10 @@
         <v>0</v>
       </c>
       <c r="O88" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P88" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q88" s="2">
         <v>0</v>
@@ -11216,10 +11216,10 @@
         <v>0</v>
       </c>
       <c r="AM88" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN88" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO88" s="2">
         <v>0</v>
@@ -11230,10 +11230,10 @@
         <v>14</v>
       </c>
       <c r="B89" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="C89" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D89" t="s">
         <v>73</v>
@@ -11242,10 +11242,10 @@
         <v>44894</v>
       </c>
       <c r="F89" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G89" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H89" s="2"/>
       <c r="I89" s="2">
@@ -11315,7 +11315,7 @@
         <v>0</v>
       </c>
       <c r="AE89" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF89" s="2">
         <v>0</v>
@@ -11342,7 +11342,7 @@
         <v>0</v>
       </c>
       <c r="AN89" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO89" s="2">
         <v>0</v>
@@ -11356,7 +11356,7 @@
         <v>65</v>
       </c>
       <c r="C90" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D90" t="s">
         <v>73</v>
@@ -11365,10 +11365,10 @@
         <v>44894</v>
       </c>
       <c r="F90" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G90" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H90" s="2"/>
       <c r="I90" s="2">
@@ -11476,7 +11476,7 @@
         <v>15</v>
       </c>
       <c r="B91" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="C91" t="s">
         <v>71</v>
@@ -11561,7 +11561,7 @@
         <v>0</v>
       </c>
       <c r="AE91" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF91" s="2">
         <v>0</v>
@@ -11599,10 +11599,10 @@
         <v>15</v>
       </c>
       <c r="B92" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
       <c r="C92" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D92" t="s">
         <v>73</v>
@@ -11611,10 +11611,10 @@
         <v>44865</v>
       </c>
       <c r="F92" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G92" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H92" s="2"/>
       <c r="I92" s="2">
@@ -11627,10 +11627,10 @@
         <v>0</v>
       </c>
       <c r="L92" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M92" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N92" s="2">
         <v>0</v>
@@ -11684,7 +11684,7 @@
         <v>0</v>
       </c>
       <c r="AE92" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF92" s="2">
         <v>0</v>
@@ -11699,7 +11699,7 @@
         <v>0</v>
       </c>
       <c r="AJ92" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK92" s="2">
         <v>0</v>
@@ -11722,10 +11722,10 @@
         <v>15</v>
       </c>
       <c r="B93" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C93" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D93" t="s">
         <v>73</v>
@@ -11734,10 +11734,10 @@
         <v>44865</v>
       </c>
       <c r="F93" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G93" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H93" s="2"/>
       <c r="I93" s="2">
@@ -11822,7 +11822,7 @@
         <v>0</v>
       </c>
       <c r="AJ93" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK93" s="2">
         <v>0</v>
@@ -11831,7 +11831,7 @@
         <v>0</v>
       </c>
       <c r="AM93" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN93" s="2">
         <v>0</v>
@@ -11845,10 +11845,10 @@
         <v>15</v>
       </c>
       <c r="B94" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="C94" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D94" t="s">
         <v>73</v>
@@ -11857,10 +11857,10 @@
         <v>44865</v>
       </c>
       <c r="F94" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G94" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H94" s="2"/>
       <c r="I94" s="2">
@@ -11900,7 +11900,7 @@
         <v>0</v>
       </c>
       <c r="U94" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V94" s="2">
         <v>0</v>
@@ -11968,7 +11968,7 @@
         <v>15</v>
       </c>
       <c r="B95" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C95" t="s">
         <v>70</v>
@@ -12068,7 +12068,7 @@
         <v>0</v>
       </c>
       <c r="AJ95" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK95" s="2">
         <v>0</v>
@@ -12091,7 +12091,7 @@
         <v>15</v>
       </c>
       <c r="B96" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="C96" t="s">
         <v>70</v>
@@ -12119,10 +12119,10 @@
         <v>0</v>
       </c>
       <c r="L96" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M96" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N96" s="2">
         <v>0</v>
@@ -12146,7 +12146,7 @@
         <v>0</v>
       </c>
       <c r="U96" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V96" s="2">
         <v>0</v>
@@ -12176,7 +12176,7 @@
         <v>0</v>
       </c>
       <c r="AE96" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF96" s="2">
         <v>0</v>
@@ -12191,7 +12191,7 @@
         <v>0</v>
       </c>
       <c r="AJ96" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK96" s="2">
         <v>0</v>
@@ -12214,10 +12214,10 @@
         <v>15</v>
       </c>
       <c r="B97" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C97" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D97" t="s">
         <v>73</v>
@@ -12226,10 +12226,10 @@
         <v>44865</v>
       </c>
       <c r="F97" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G97" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H97" s="2"/>
       <c r="I97" s="2">
@@ -12323,7 +12323,7 @@
         <v>0</v>
       </c>
       <c r="AM97" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN97" s="2">
         <v>0</v>
@@ -12337,10 +12337,10 @@
         <v>15</v>
       </c>
       <c r="B98" t="s">
-        <v>66</v>
+        <v>23</v>
       </c>
       <c r="C98" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D98" t="s">
         <v>73</v>
@@ -12349,10 +12349,10 @@
         <v>44865</v>
       </c>
       <c r="F98" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G98" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H98" s="2"/>
       <c r="I98" s="2">
@@ -12446,7 +12446,7 @@
         <v>0</v>
       </c>
       <c r="AM98" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN98" s="2">
         <v>0</v>
@@ -12463,7 +12463,7 @@
         <v>22</v>
       </c>
       <c r="C99" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D99" t="s">
         <v>73</v>
@@ -12472,10 +12472,10 @@
         <v>44865</v>
       </c>
       <c r="F99" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G99" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H99" s="2"/>
       <c r="I99" s="2">
@@ -12545,7 +12545,7 @@
         <v>0</v>
       </c>
       <c r="AE99" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF99" s="2">
         <v>0</v>
@@ -12569,7 +12569,7 @@
         <v>0</v>
       </c>
       <c r="AM99" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN99" s="2">
         <v>0</v>
@@ -12583,10 +12583,10 @@
         <v>16</v>
       </c>
       <c r="B100" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="C100" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D100" t="s">
         <v>73</v>
@@ -12595,10 +12595,10 @@
         <v>44879</v>
       </c>
       <c r="F100" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G100" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H100" s="2"/>
       <c r="I100" s="2">
@@ -12706,7 +12706,7 @@
         <v>16</v>
       </c>
       <c r="B101" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C101" t="s">
         <v>71</v>
@@ -12752,7 +12752,7 @@
         <v>0</v>
       </c>
       <c r="R101" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S101" s="2">
         <v>0</v>
@@ -12773,7 +12773,7 @@
         <v>0</v>
       </c>
       <c r="Y101" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z101" s="2">
         <v>0</v>
@@ -12791,7 +12791,7 @@
         <v>0</v>
       </c>
       <c r="AE101" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF101" s="2">
         <v>0</v>
@@ -12829,7 +12829,7 @@
         <v>16</v>
       </c>
       <c r="B102" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="C102" t="s">
         <v>70</v>
@@ -12938,7 +12938,7 @@
         <v>0</v>
       </c>
       <c r="AM102" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN102" s="2">
         <v>0</v>
@@ -12952,10 +12952,10 @@
         <v>16</v>
       </c>
       <c r="B103" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="C103" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D103" t="s">
         <v>73</v>
@@ -12964,10 +12964,10 @@
         <v>44879</v>
       </c>
       <c r="F103" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G103" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H103" s="2"/>
       <c r="I103" s="2">
@@ -12980,10 +12980,10 @@
         <v>0</v>
       </c>
       <c r="L103" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M103" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N103" s="2">
         <v>0</v>
@@ -13037,7 +13037,7 @@
         <v>0</v>
       </c>
       <c r="AE103" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF103" s="2">
         <v>0</v>
@@ -13061,7 +13061,7 @@
         <v>0</v>
       </c>
       <c r="AM103" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN103" s="2">
         <v>0</v>
@@ -13075,10 +13075,10 @@
         <v>16</v>
       </c>
       <c r="B104" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C104" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D104" t="s">
         <v>73</v>
@@ -13087,10 +13087,10 @@
         <v>44879</v>
       </c>
       <c r="F104" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G104" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H104" s="2"/>
       <c r="I104" s="2">
@@ -13184,7 +13184,7 @@
         <v>0</v>
       </c>
       <c r="AM104" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN104" s="2">
         <v>0</v>
@@ -13198,10 +13198,10 @@
         <v>16</v>
       </c>
       <c r="B105" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="C105" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D105" t="s">
         <v>73</v>
@@ -13210,10 +13210,10 @@
         <v>44879</v>
       </c>
       <c r="F105" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G105" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H105" s="2"/>
       <c r="I105" s="2">
@@ -13226,10 +13226,10 @@
         <v>0</v>
       </c>
       <c r="L105" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M105" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N105" s="2">
         <v>0</v>
@@ -13265,7 +13265,7 @@
         <v>0</v>
       </c>
       <c r="Y105" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z105" s="2">
         <v>0</v>
@@ -13321,7 +13321,7 @@
         <v>16</v>
       </c>
       <c r="B106" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C106" t="s">
         <v>71</v>
@@ -13367,7 +13367,7 @@
         <v>0</v>
       </c>
       <c r="R106" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S106" s="2">
         <v>0</v>
@@ -13430,7 +13430,7 @@
         <v>0</v>
       </c>
       <c r="AM106" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN106" s="2">
         <v>0</v>
@@ -13444,10 +13444,10 @@
         <v>17</v>
       </c>
       <c r="B107" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="C107" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D107" t="s">
         <v>73</v>
@@ -13456,10 +13456,10 @@
         <v>44893</v>
       </c>
       <c r="F107" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G107" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H107" s="2"/>
       <c r="I107" s="2">
@@ -13475,7 +13475,7 @@
         <v>0</v>
       </c>
       <c r="M107" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N107" s="2">
         <v>0</v>
@@ -13487,10 +13487,10 @@
         <v>0</v>
       </c>
       <c r="Q107" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R107" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S107" s="2">
         <v>0</v>
@@ -13529,7 +13529,7 @@
         <v>0</v>
       </c>
       <c r="AE107" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF107" s="2">
         <v>0</v>
@@ -13567,10 +13567,10 @@
         <v>17</v>
       </c>
       <c r="B108" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="C108" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D108" t="s">
         <v>73</v>
@@ -13579,10 +13579,10 @@
         <v>44893</v>
       </c>
       <c r="F108" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G108" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H108" s="2"/>
       <c r="I108" s="2">
@@ -13598,7 +13598,7 @@
         <v>0</v>
       </c>
       <c r="M108" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N108" s="2">
         <v>0</v>
@@ -13610,10 +13610,10 @@
         <v>0</v>
       </c>
       <c r="Q108" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R108" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S108" s="2">
         <v>0</v>
@@ -13652,7 +13652,7 @@
         <v>0</v>
       </c>
       <c r="AE108" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF108" s="2">
         <v>0</v>
@@ -13690,10 +13690,10 @@
         <v>18</v>
       </c>
       <c r="B109" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C109" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D109" t="s">
         <v>73</v>
@@ -13702,10 +13702,10 @@
         <v>44887</v>
       </c>
       <c r="F109" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G109" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H109" s="2"/>
       <c r="I109" s="2">
@@ -13739,10 +13739,10 @@
         <v>0</v>
       </c>
       <c r="S109" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T109" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U109" s="2">
         <v>0</v>
@@ -13787,7 +13787,7 @@
         <v>0</v>
       </c>
       <c r="AI109" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ109" s="2">
         <v>0</v>
@@ -13813,10 +13813,10 @@
         <v>18</v>
       </c>
       <c r="B110" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C110" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D110" t="s">
         <v>73</v>
@@ -13825,10 +13825,10 @@
         <v>44887</v>
       </c>
       <c r="F110" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G110" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H110" s="2"/>
       <c r="I110" s="2">
@@ -13862,10 +13862,10 @@
         <v>0</v>
       </c>
       <c r="S110" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T110" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U110" s="2">
         <v>0</v>
@@ -13910,7 +13910,7 @@
         <v>0</v>
       </c>
       <c r="AI110" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ110" s="2">
         <v>0</v>
@@ -14059,10 +14059,10 @@
         <v>18</v>
       </c>
       <c r="B112" t="s">
-        <v>31</v>
+        <v>67</v>
       </c>
       <c r="C112" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D112" t="s">
         <v>73</v>
@@ -14071,10 +14071,10 @@
         <v>44887</v>
       </c>
       <c r="F112" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G112" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H112" s="2"/>
       <c r="I112" s="2">
@@ -14182,10 +14182,10 @@
         <v>18</v>
       </c>
       <c r="B113" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="C113" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D113" t="s">
         <v>73</v>
@@ -14194,10 +14194,10 @@
         <v>44887</v>
       </c>
       <c r="F113" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G113" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H113" s="2"/>
       <c r="I113" s="2">
@@ -14434,7 +14434,7 @@
         <v>70</v>
       </c>
       <c r="D115" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E115" s="1">
         <v>44714</v>
@@ -14559,7 +14559,7 @@
         <v>70</v>
       </c>
       <c r="D116" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E116" s="1">
         <v>44714</v>

</xml_diff>